<commit_message>
Grans: moving towards proper config treatment; tried out google translate v3, but then it gets complicated
</commit_message>
<xml_diff>
--- a/data2/EM-SM/translate.xlsx
+++ b/data2/EM-SM/translate.xlsx
@@ -34571,7 +34571,7 @@
   <dimension ref="A1:E286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B2:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -34588,7 +34588,7 @@
       </c>
       <c r="B1" s="21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>EN*</t>
         </is>
       </c>
       <c r="C1" s="19" t="inlineStr">
@@ -34617,9 +34617,13 @@
 Erhaltungszustand: Gut</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>", adjella ifa´ or abbreviated, Adjelefa´. The foot represents a kneeling woman holding a child on her back. Partially covered with clay" Bowl for the Ife service Form: The two people hold a bowl with the tips of their headgear Color: gray-brown Condition: good</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>", adjella ifa´ or abbreviated, Adjelefa´. The foot represents a kneeling woman holding a child on her back. Partly covered with clay"
+Bowl for the Ife service
+Shape: The two people hold a bowl with the tips of their headgear
+Color: gray-brown
+Condition: good</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -34635,9 +34639,12 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>", sako´, plur., masako´. Comb of women; made of wood." Shape: Six strong, thorn-shaped, light tines with a semi-oval comb back. A partially ribbed handle on it Color: Dark brown, black Condition: Good.</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>", sako´, plur., masako´. Comb of women; made of wood."
+Shape: Six strong, thorn-shaped, light tines with a semi-oval comb back. A partially ribbed handle on it
+Color: dark brown, black
+Condition: good.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -34653,9 +34660,12 @@
 Erhaltungszustand: kleine Bruchstelle am unteren Ende</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>"Ancestral carving with brass stripes; Ogowe, Odumbo" "The back has no brass fittings; in the middle there is a block-shaped, 18 cm long, 3.2 cm wide and up to 1.5 cm high bump in the wood." (Index card) Color: brown, brass Condition: small break at the lower end</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"Ancestral carving covered with brass strips; Ogowe, Odumbo"
+"The back has no brass fittings; in the middle there is a block-shaped, 18 cm long, 3.2 cm wide and up to 1.5 cm high bump in the wood." (Index card)
+Color: brown, brass
+Condition: small break at the lower end</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -34669,9 +34679,10 @@
 Farbe: Braun</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>"Mug, in the shape of a human head, carved out of wood. Bakuba." color: brown</t>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"Mug, in the shape of a human head, carved out of wood. Bakuba."
+color: brown</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -34688,9 +34699,13 @@
 Erhaltungszustand:</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>"Wooden figure (deceased brother!) ´sakela´; H: 17 cm; Cokwe" shape: color: dark brown pattern: condition:</t>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"Wooden figure (deceased brother!) ´sakela´; H: 17 cm; Cokwe"
+Shape:
+Color: dark brown
+Template:
+Condition:</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -34705,9 +34720,11 @@
 Farbe: Braun, gelb</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>"Head covered with fur (atikpa)." Shape: human hair on the head, the eyes covered with metal. Color: brown, yellow</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>"Head covered with fur (atikpa)."
+Shape: human hair is on the head, the eyes are covered with metal
+Color: brown, yellow</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -34723,9 +34740,12 @@
 Erhaltungszustand:</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>"Oracle device. Upper Djuma." Shape: Stylized crocodile Color: Black Condition:</t>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>"Oracle device. Upper Djuma."
+Shape: stylized crocodile
+Color: Black
+Condition:</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -34739,9 +34759,10 @@
 Farbe: Braun poliert</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>"Oracle device: crocodile carved out of wood." Color: polished brown</t>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>"Oracle device: crocodile carved out of wood."
+Color: polished brown</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -34760,9 +34781,15 @@
 Wawemba (Manda)"</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>"Wooden doll, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say when they carry the doll: 'This is my child I gave birth to .´ "Cylindrical body with breasts, navel and several tattoo bands. Instead of the head sits a cone with a hairstyle made of natural fibers and clay balls. On it hangs jewelry made of 5 glass beads. Color: dark brown, beads = red, blue. Condition: good. Main catalog: "" muâna, plur .: vâna "Doll made of wood, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say if they carry the doll: 'This is my child I gave birth to.' With artificial hair. 22 cm h. Wawemba (Manda) "</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>"Wooden doll, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say when they carry the doll: 'This is my child that I gave birth to. ""
+Cylindrical body with breasts, navel and several tattoo bands. Instead of the head sits a cone with a hairstyle made of natural fibers and clay balls. On it is a jewelry made of 5 glass beads
+Color: dark brown, pearls = red, blue
+Condition: good.
+Main catalog: "" muâna, plur .: vâna "Doll made of wood, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say if they carry the doll: 'This is my child I gave birth to.' With artificial hair.
+22 cm h.
+Wawemba (Manda) "</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -34779,9 +34806,13 @@
 Erhaltungszustand: gut</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>"sayizumbo; male figure from a group of figures used as a fertility charm; H: 21 cm; Tsokwe, Mahakaholo" shape: color: dark brown pattern: condition: good</t>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>"sayizumbo; male figure from a group of figures used as a fertility spell; H: 21 cm; Tsokwe, Mahakaholo"
+Shape:
+Color: dark brown
+Template:
+Condition: good</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -34795,9 +34826,10 @@
 Farbe: Braun, schwarz, kleine rote Reste</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>"Standing woman with five-part hairstyle" Color: brown, black, small red remains</t>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>"Standing woman with five-part hairstyle"
+Color: brown, black, small red remains</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -34813,9 +34845,12 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>"Tsitwamo tsa soba, chief chair Tsokwe (Tsipukungu)." Shape: armchair in European form but on all 4 sides and on the back with figurative representations from life. The seat is a tight leather Color: Black Condition: Good.</t>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>"Tsitwamo tsa soba, chief chair Tsokwe (Tsipukungu)."
+Shape: armchair in European form but on all 4 sides and on the back with figurative representations from life. The seat is a tight leather
+Color: Black
+Condition: good.</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -34831,9 +34866,12 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>"Tsitwamo, armchair (with two Tsikusa masks and a Tsihongo mask). Luma. Cokwe." Shape: armchair in European form but with figurative representations from life Color: black Condition: good.</t>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>"Tsitwamo, armchair (with two Tsikusa masks and a Tsihongo mask). Luma. Cokwe."
+Form: armchair in European form but with figurative representations from life
+Color: Black
+Condition: good.</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -34850,9 +34888,13 @@
 Erhaltungszustand: im Horn ist ein Loch</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>"Tooth (pipe?) And ivory fetish figure. Hunting trophy, which is highly honored. Loango. (Caio)" "The detachable figure sits on a hollow horn. A cord is attached to an opening in the tip, which pierced the vertically Body runs through and emerges from the skull. " (Index card) Color: ivory, brown Pattern: carving Condition: there is a hole in the horn</t>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>"Tooth (pipe?) And fetish figure made of ivory. Hunting trophy that is highly honored. Loango. (Caio)"
+"The detachable figure sits on a hollow horn. A cord is attached to an opening in its tip, which runs through the vertically pierced body and emerges from the skull." (Index card)
+Color: ivory, brown
+Pattern: carving
+Condition: there is a hole in the horn</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -34865,7 +34907,7 @@
           <t>"Zierkamm mit Kopf"</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>"Comb with head"</t>
         </is>
@@ -34880,7 +34922,7 @@
           <t>"´Ibedji´-Figur aus Holz. Männliche Figur, bis zum Hals dunkelrot glänzend gefärbt, teilweise mit rotem Lehm beschmiert; Haare (geteilte Frisur) schwarz gefärbt; Gesicht holzfarben; um das linke Handgelenk und den linken Fuß je eine Perlkette, um den Leib eine Kette aus kleinen, runden, schwarzen Scheiben. Höhe: 26,6 cm. Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>"´Ibedji´ figure made of wood. Male figure, dyed dark red glossy up to the neck, partly smeared with red clay; hair (split hairstyle) colored black; face wood-colored; a pearl necklace around the left wrist and the left foot A chain made of small, round, black discs. Height: 26.6 cm. North Yoruba "</t>
         </is>
@@ -34901,9 +34943,15 @@
 Urua"</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr">
-        <is>
-          <t>Ancestor figure, female Characteristics: Cross hairstyle, reptile skin-like tattoos on the sternum and abdomen, more on the back, legs not worked out, kneeling. A simple cord is tied around the neck. Color: blackened. Condition: abrasions. The right arm has broken off and is missing. Main catalog: "Wooden figure (ancestor figure), [...] 36 ctm. L. Urua"</t>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ancestor figure, female
+Features: cross hairstyle, reptile skin-like tattoos on the sternum and abdomen, more on the back, legs not worked out, kneeling. A simple cord is tied around the neck
+Color: blackened
+Condition: abrasions. The right arm has broken off and is missing.
+Main catalog: "Wooden figure (ancestor figure) [...], m. [...]
+36 ctm. l.
+Urua "</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -34918,9 +34966,11 @@
 aus Ulrich Wegner: Afrikanische Saiteninstrumente, Staatliche Museen Berlin – SPK, 1984 (Anhang Objektkatalog)</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>As a corpus, a hemispherical calabash half with a flocked-over lizard skin membrane flipped over to the outside. A large, round membrane opening on the side. As a string holder, a straight round wooden stick, at the free end of which the ponytail hair string is tied with goat leather straps. As a lower tailpiece, a loop made of antelope leather that extends far from the spit to the ceiling. The lower end of the string was knotted behind a piece of money perforated in the center, which is buttoned through the outlet of the loop. A cross-shaped wooden walkway. As a bow, a flat, curved iron rod with horsehair stringing. The bow string is tied at one end behind a perforation to form a knot and fastened at the other end under fabric and cord wraps. At the end of the neck a goat leather strap with knotted pearls, coins, a cowrie shell and a belt buckle. "Bayan Dutse" from Ulrich Wegner: African stringed instruments, State Museums Berlin - SPK, 1984 (attachment object catalog)</t>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>As a corpus, a hemispherical calabash half with a flocked-over lizard skin membrane flipped over to the outside. A large, round membrane opening on the side. As a string holder, a straight round wooden stick, at the free end of which the ponytail hair string is tied with goat leather straps. As a lower tailpiece, a loop made of antelope leather that extends far from the spit to the ceiling. The lower end of the string was knotted behind a piece of money perforated in the center, which is buttoned through the outlet of the loop. A cross-shaped wooden walkway. As a bow, a flat, curved iron rod with horsehair stringing. The bow string is tied at one end behind a perforation to form a knot and fastened at the other end under fabric and cord wraps. At the end of the neck a goat leather strap with knotted pearls, coins, a cowrie shell and a belt buckle.
+"Bayan Dutse"
+from Ulrich Wegner: African stringed instruments, State Museums Berlin - SPK, 1984 (Appendix object catalog)</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -34933,7 +34983,7 @@
           <t>Am Bauch des Gefäßes und am Deckel befinden sich Darstellungen von Portugiesen mit Gewehren und von Leoparden. Auf dem Deckel stehen zwei Figuren mit Gefäßen in den Händen. Die Leoparden und die bewaffneten Portugiesen sind Hinweise, dass dieses Gefäß Teil eines königlichen Altars war.</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>On the belly of the vessel and on the lid there are representations of Portuguese with rifles and leopards. On the lid there are two figures with vessels in their hands. The leopards and the armed Portuguese are indications that this vessel was part of a royal altar.</t>
         </is>
@@ -34948,7 +34998,7 @@
           <t>Am breiten Ende mit 30 Noppen verziert</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Decorated with 30 knobs on the wide end</t>
         </is>
@@ -34963,7 +35013,7 @@
           <t>Aufsatzmaske mit Stielaugen und flach trichterförmigem Mund.</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>Attachment mask with long eyes and flat, funnel-shaped mouth.</t>
         </is>
@@ -34981,9 +35031,12 @@
 Der hist. Vollständigkeit halber soll hier auch der unter 4. aufgeführte Gegenstand erwähnt werden, obgleich er sich hier auch nicht mehr im Museum befindet; es war dies eine Krone, die am 27.02.1869 vom König zurückgefordert wurde wurde. (Vgl. Akt. 214/69). Die Krone wurde als Geschenk an Victoria von England nach England geschickt (Vgl. Akt. 286/69). Dem Museum wurden Fotos von der Krone zugestellt. Rohlfs laufte die Krone "während der Plünderung der Bergfeste Magdala am 13.04.1868" ... "und zwar von einem englischen Infanterie Soldaten (wahrscheinlich 33. Regiment)."</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>from file case E 1126/1868: report from Mr. Rohlfs to Wilhelm von Prussia ... it is handed over to the king (see also III A 250a, b; III A 251). 1. The older state seal of King Theodor made of silver and with the double inscription in Amharic and Arabic, which is the same and means "ras Kassa sultan el habescha" or "the city keeper Kassa King of Abyssinia". This seal was in the possession of Eduard Zander, formerly sent to Abessinen for the sake of the Duke of Anhalt, and later employed by King Theosor as "alter ego", meaning that he had to be done with the royal clothes, in battles and battles the enemy projectiles from the king lead from time to time. The seal was purchased. For the sake of completeness, the item listed under 4 should also be mentioned here, although it is no longer in the museum; it was a crown that was reclaimed by the king on February 27, 1869. (See Act 214/69). The crown was sent as a gift to Victoria from England to England (see Act 286/69). Photos of the crown were sent to the museum. Rohlfs wore the crown "during the looting of the Magdala mountain fortress on April 13, 1868" ... "by an English infantry soldier (probably 33rd regiment)."</t>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>from file case E 1126/1868: report from Mr. Rohlfs to Wilhelm von Preußen
+... it is given to the king (see also III A 250a, b; III A 251).
+1. The older state seal of King Theodor made of silver and with the double inscription in Amharic and Arabic, which is the same and means "ras Kassa sultan el habescha" or "the city keeper Kassa King of Abyssinia". This seal was in the possession of Eduard Zander, formerly sent to Abessinen for the sake of the Duke of Anhalt, and was later employed by King Theosor as "alter ego", i.e. he had to be done with the royal clothes, in battles and battles he had to direct the enemy projectiles from the king to himself. The seal was purchased.
+For the sake of completeness, the item listed under 4 should also be mentioned here, although it is no longer in the museum; it was a crown that was reclaimed by the king on February 27, 1869. (See Act 214/69). The crown was sent as a gift to Victoria from England to England (see Act 286/69). Photos of the crown were sent to the museum. Rohlfs wore the crown "during the looting of the Magdala mountain fortress on April 13, 1868" ... "by an English infantry soldier (probably 33rd regiment)."</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -34996,7 +35049,7 @@
           <t>Aus einem Stück geschnitzte Nackenstütze. Nackenstützen stützten den Kopf des liegenden Mannes und schützten seine Frisur.</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>One-piece carved neck support. Neck supports supported the lying man's head and protected his hairstyle.</t>
         </is>
@@ -35011,7 +35064,7 @@
           <t>Beil mit kunstvoll geschmiedeter Klinge, Stiel mit Kupferblech überzogen</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>Hatchet with artistically forged blade, handle covered with copper sheet</t>
         </is>
@@ -35026,7 +35079,7 @@
           <t>Beil mit schmaler, langer Eisenklige, die dürch einen schönen geschnitzten Holzstiel gesteckt ist. Den obren Teil des Stieles bildet eine weiblich reitende Figür, geschnitzt mit einer glasperlenkette und Perlenschnür.KB-104</t>
         </is>
       </c>
-      <c r="B26" s="3" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Hatchet with a narrow, long iron claw, which is stuck through a beautiful carved wooden handle. The upper part of the stem is a female riding figure, carved with a glass pearl necklace and pearl string. KB-104</t>
         </is>
@@ -35046,9 +35099,14 @@
 Deutsche Expedition 1874</t>
         </is>
       </c>
-      <c r="B27" s="3" t="inlineStr">
-        <is>
-          <t>Description: Shape: face is painted red with a vertical line over nose and mouth, left half of the face is painted white, around the neck is a metal hoop with a long chain, in front of the upper body a round raised disc with a mirror, in the back a carved hole , Lower body and legs wrapped in fabric Color: brown, white, red Pattern: painting Condition: rust, breakage on the nose German expedition 1874</t>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Description:
+Shape: face is painted red with a vertical line over nose and mouth, left half of the face is painted white, around the neck is a metal hoop with a long chain, in front of the upper body a round raised disc with a mirror, in the back a carved hole, lower body uud legs wrapped in fabric
+Color: brown, white, red
+Pattern: painting
+Condition: rust, breakage on the nose
+German expedition 1874</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -35061,7 +35119,7 @@
           <t>Deckelgefäß aus Holz, auf dem Deckel (Höhe 19,5 cm) Figurenpaar</t>
         </is>
       </c>
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Lid container made of wood, on the lid (height 19.5 cm) pair of figures</t>
         </is>
@@ -35077,9 +35135,10 @@
 Eintrag im historischen Hauptkatalog: "Holzgefäß. Form eines Metallbechers der seitlich so zusammengedrückt worden, dass der obere Rand die Gestalt einer 8 angenommen hat. Bodenfläche leicht oval."</t>
         </is>
       </c>
-      <c r="B29" s="3" t="inlineStr">
-        <is>
-          <t>The edge of the polished cup is drawn in so that it makes an eight. Like a vessel with two spouts. A 4 cm long nose runs down from the narrowing on each side. Entry in the historical main catalog: "Wooden vessel. Shape of a metal cup that has been compressed laterally in such a way that the upper edge has the shape of an 8. Bottom surface slightly oval."</t>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>The edge of the polished cup is drawn in so that it makes an eight. Like a vessel with two spouts. A 4 cm long nose runs down from the narrowing on each side.
+Entry in the historical main catalog: "Wooden vessel. Shape of a metal cup that has been compressed laterally in such a way that the upper edge has the shape of an 8. Bottom surface slightly oval."</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -35092,7 +35151,7 @@
           <t>Die Figur gehörte ursprünglich zur Altargruppe einer Königinmutter. Sie hält einen Spiegel, der als „Fenster“ zur Welt spiritueller Kräfte angesehen wurde. Bei zeremoniellen Auftritten des Königs und der Königinmutter dienten Spiegel zur Abwehr gefährlicher Kräfte.</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>The figure originally belonged to the altar group of a queen mother. She holds a mirror that was viewed as a “window” to the world of spiritual powers. At ceremonial appearances of the king and the queen mother mirrors were used to ward off dangerous forces.</t>
         </is>
@@ -35107,7 +35166,7 @@
           <t>Die kleine Vase wird von unten beginnend langsam breiter, verjüngt sich wieder und setzt sich dann in gleichbleibender Breite fort. Sie ist mit runden und eckigen geometr. Mustern - typ. Kadiweu-Mustern - versehen.Außen bunt bemalt.</t>
         </is>
       </c>
-      <c r="B31" s="3" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>The small vase slowly widens from the bottom, tapers again and then continues in a constant width. It is with round and angular geometr. Patterns - typical Kadiweu patterns - provided.</t>
         </is>
@@ -35123,9 +35182,10 @@
 Hauptkatalog: Ein Paar versilberte Armverzierungen.</t>
         </is>
       </c>
-      <c r="B32" s="3" t="inlineStr">
-        <is>
-          <t>Between 1890 and 1893, the workshop of the artist Hountoundji made these arm cuffs for the last king of the independent kingdom of Dahomey, Béhanzin, as a gift for German Emperor Wilhelm II. They are made from a silver ligation and are decorated with flowers or stars made from precious gold. With these arm cuffs, the king also gave the emperor other objects that indicated the high rank of the king and emperor at the same time: an umbrella, a saber, a throne, leather bags, and stripe blankets made of velvet. The gifts were given during France's war against Dahomey. With these magnificent gifts, Béhanzin tried to defend the independence of his empire through an alliance with the German Empire. Main catalog: A pair of silver-plated arm decorations.</t>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Between 1890 and 1893, the workshop of the artist Hountoundji produced these arm cuffs as a gift for the German Emperor Wilhelm II for the last king of the independent kingdom of Dahomey, Béhanzin. They are made from a silver ligation and are decorated with flowers or stars made from precious gold. With these arm cuffs, the king also gave the emperor other objects that indicated the high rank of the king and emperor at the same time: an umbrella, a saber, a throne, leather bags, and stripe blankets made of velvet. The gifts were given during France's war against Dahomey. With these magnificent gifts, Béhanzin tried to defend the independence of his empire through an alliance with the German Empire.
+Main catalog: A pair of silver-plated arm decorations.</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -35139,9 +35199,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>This pipe made of red clay with a pipe decorated with copper wire represents a ruler or dignitary. It was manufactured in the Cameroonian grasslands in the Kingdom of Bali at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>This pipe made of red clay with a pipe decorated with copper wire represents a ruler or dignitary. It was manufactured in the Cameroonian grasslands in the Kingdom of Bali at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -35155,9 +35216,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B34" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl is decorated with depictions of human faces and other motifs. It was manufactured in Bamessing in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl is decorated with depictions of human faces and other motifs. It was manufactured in Bamessing in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -35171,9 +35233,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B35" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl is decorated with depictions of human faces and other motifs. It was manufactured in the Babungo in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl is decorated with depictions of human faces and other motifs. It was manufactured in the Babungo in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -35187,9 +35250,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B36" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a face. It was manufactured in the Kingdom of Bali in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a face. It was manufactured in the Kingdom of Bali in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -35203,9 +35267,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B37" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a ruler or a high-ranking noble woman from the grasslands of Cameroon. It was manufactured in Bamunka at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a ruler or a high-ranking noble woman from the grasslands of Cameroon. It was manufactured in Bamunka at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -35219,9 +35284,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B38" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a seated human figure. It was manufactured in Bamessing in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a seated human figure. It was manufactured in Bamessing in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -35235,9 +35301,10 @@
 Hauptkatalog: Pfeifenkopf aus Ton in Gestalt eines Menschen (nur der Oberkörper) mit hoher Frisur (od. Mütze?); auf der Brust ein Ornament</t>
         </is>
       </c>
-      <c r="B39" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a ruler or a dignitary. It was manufactured in the Kingdom of Bali in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Main catalog: Pipe bowl made of clay in the shape of a person (only the upper body) with a high hairstyle (or cap?); an ornament on the chest</t>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a ruler or a dignitary. It was manufactured in the Kingdom of Bali in the Cameroonian grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Main catalog: Pipe bowl made of clay in the shape of a person (only the upper body) with a high hairstyle (or cap?); an ornament on the chest</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -35251,9 +35318,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B40" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a ruler or a dignitary. It was manufactured in Bamessing in the Cameroon Grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a ruler or a dignitary. It was manufactured in Bamessing in the Cameroon Grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -35267,9 +35335,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb (JF 03.01.2017).</t>
         </is>
       </c>
-      <c r="B41" s="3" t="inlineStr">
-        <is>
-          <t>This clay pipe bowl represents a crocodile. It was manufactured in the Bamum kingdom in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them (JF January 3, 2017).</t>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>This clay pipe bowl represents a crocodile. It was manufactured in the Bamum kingdom in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them (JF January 3, 2017).</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -35283,9 +35352,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B42" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the early 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the early 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -35299,9 +35369,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag und er kaufte anderen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B43" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon and bought others in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon and bought others in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -35315,9 +35386,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B44" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -35331,9 +35403,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. It has the shape of the head of a ruler or a dignitary. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. It has the shape of the head of a ruler or a dignitary. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -35347,9 +35420,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B46" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. He represents a ruler or a dignitary. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. He represents a ruler or dignitary. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -35363,9 +35437,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B47" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Babungo in the Cameroon grasslands at the beginning of the 20th century. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -35379,9 +35454,10 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B48" s="3" t="inlineStr">
-        <is>
-          <t>This tobacco pipe bowl was manufactured in Bamessing in the Cameroonian grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>This tobacco pipe bowl was manufactured in Bamessing in the Cameroonian grasslands at the beginning of the 20th century. Human faces and the head of a buffalo are depicted on the head. In the grasslands, buffaloes often symbolized dignitaries who served in a ruler's palace. Around 1900 kings, dignitaries and heads of families smoked tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -35394,7 +35470,7 @@
           <t>Dreiteilige Nackenstütze (kali) aus Bambusrohr (bitu) und zwei angebundenen Holzbeinen. Nackenstützen stützten den Kopf des liegenden Mannes und schützten seine Frisur.</t>
         </is>
       </c>
-      <c r="B49" s="3" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>Three-part headrest (kali) made of bamboo cane (bitu) and two attached wooden legs. Neck supports supported the lying man's head and protected his hairstyle.</t>
         </is>
@@ -35409,7 +35485,7 @@
           <t>Dunkelbraune Gesichtsmaske, des Bwame-Bundes, mit Röhrenmund.</t>
         </is>
       </c>
-      <c r="B50" s="3" t="inlineStr">
+      <c r="B50" t="inlineStr">
         <is>
           <t>Dark brown face mask, of the Bwame-Bund, with a tubular mouth.</t>
         </is>
@@ -35424,7 +35500,7 @@
           <t>Dunkelbraune Patina</t>
         </is>
       </c>
-      <c r="B51" s="3" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>Dark brown patina</t>
         </is>
@@ -35440,9 +35516,10 @@
 Eintrag im historischen Hauptkatalog: "Holzgeschnitzte Maske"</t>
         </is>
       </c>
-      <c r="B52" s="3" t="inlineStr">
-        <is>
-          <t>Dark mask, of the Gelede-Bund, carved with a human face. Entry in the historical main catalog: "Wood carved mask"</t>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Dark mask, of the Gelede-Bund, carved with a human face.
+Entry in the historical main catalog: "Wood carved mask"</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -35455,7 +35532,7 @@
           <t>Ein glockenförmiger Holzgong mit flach ovalem Querschnitt. Die beiden großen Ansichten sind mit je einem Gesicht schnitzverziert. Oben ein Henkel mit geflochtener Bastschlaufe</t>
         </is>
       </c>
-      <c r="B53" s="3" t="inlineStr">
+      <c r="B53" t="inlineStr">
         <is>
           <t>A bell-shaped wooden gong with a flat oval cross-section. The two large views are each carved with a face. On the top a handle with a braided bast loop</t>
         </is>
@@ -35470,7 +35547,7 @@
           <t>Ein Stiefel, früher immer mit Pelz besetzt) der Dacota. Außen mit zierlicher Stachelscheinborstenstickerei. (S. Karteikarte )</t>
         </is>
       </c>
-      <c r="B54" s="3" t="inlineStr">
+      <c r="B54" t="inlineStr">
         <is>
           <t>A boot, formerly always covered with fur) of the Dacota. On the outside with delicate stinging bristle embroidery. (See index card)</t>
         </is>
@@ -35490,9 +35567,14 @@
 d.  An der Schale des Korpus sind zwei große menschliche Gesichter angeschnitzt (eines mit Bart).</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr">
-        <is>
-          <t>A tumbler with two human faces opposite and goat beards. The membrane is tuned with resin. Entry in the historical main catalog: "Large wooden drum, coated with wax plaster on top". a. Without fur ring. The membrane is mostly covered with vocal paste. b. Bowl cylindrical. Stand (type B). c. A carrying strap is attached to two x-shaped carved brackets. d. Two large human faces are carved on the shell of the body (one with a beard).</t>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>A tumbler with two human faces opposite and goat beards. The membrane is tuned with resin.
+Entry in the historical main catalog: "Large wooden drum, coated with wax plaster on top".
+a. Without fur ring. The membrane is mostly covered with vocal paste.
+b. Bowl cylindrical. Stand (type B).
+c. A carrying strap is attached to two x-shaped carved brackets.
+d. Two large human faces are carved on the shell of the body (one with a beard).</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -35511,9 +35593,15 @@
 Muliro, Tara (Uemba)"</t>
         </is>
       </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>A doll with a disproportionately long neck, cylindrical body with breasts, navel and several tattoo bands. Color: yellow-brown Condition: good. Main catalog: "Wooden doll, with head. 23 cm h. Tabwa, Wemba, Congo Muliro, Tara (Uemba)"</t>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>A doll with a disproportionately long neck, a cylindrical body with breasts, a navel and several tattoo bands
+Color: tan
+Condition: good.
+Main catalog: "Wooden doll, with head.
+23 cm h.
+Tabwa, Wemba, Congo
+Muliro, Tara (Uemba) "</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -35526,7 +35614,7 @@
           <t>Eine weibliche Figur mit auffallend großen Füßen und einer Drahtspirale am linken Arm steht auf einer runden Grundfläche und trägt auf dem Kopf eine ebenso geformte Sitzfläche.</t>
         </is>
       </c>
-      <c r="B57" s="3" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>A female figure with strikingly large feet and a wire spiral on the left arm stands on a round base and has an equally shaped seat on her head.</t>
         </is>
@@ -35542,9 +35630,10 @@
 Eintrag im historischen Hauptkatalog: Wassertopf aus Ton.</t>
         </is>
       </c>
-      <c r="B58" s="3" t="inlineStr">
-        <is>
-          <t>Entry of historical index card: Large water pot, made of clay, closed with corn on the cob. 2 handles. Entry in the historical main catalog: clay water pot.</t>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Entry of historical index card: Large water pot, made of clay, closed with corn on the cob. 2 handles.
+Entry in the historical main catalog: clay water pot.</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -35558,9 +35647,10 @@
 Eintrag im historischen Hauptkatalog: Schmuckschüssel</t>
         </is>
       </c>
-      <c r="B59" s="3" t="inlineStr">
-        <is>
-          <t>Entry of historical index card: jewelry bowl made of clay. Entry in the historical main catalog: jewelry bowl</t>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Entry of historical index card: jewelry bowl made of clay.
+Entry in the historical main catalog: jewelry bowl</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -35577,9 +35667,13 @@
 Krieger in voller Bewaffnung. Das Gesicht ist tätowiert und die rechte Gesichtshälfte ist rot bemalt. Termitenfraß an den Füßen</t>
         </is>
       </c>
-      <c r="B60" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog (partial quote): "The whole figure, apparently the portrait of a deceased in full armor, stood on a grave." [Then it was touched up] "after personal communication from Dr. Wolf as a 'fetish' in a house." further description: warrior in full armament. The face is tattooed and the right half of the face is painted red. Termite feeding on the feet</t>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog (partial quote):
+"The whole figure, apparently the portrait of a deceased in full armor, stood on a grave."
+[Then it was touched up] "after personal communication from Dr. Wolf as a 'fetish' in a house."
+further description:
+Warriors in full armament. The face is tattooed and the right half of the face is painted red. Termite feeding on the feet</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -35599,9 +35693,16 @@
 &gt; Lehne) Dem rechten Trommler in der zweiten Reihe von oben fehlt der rechte Arm. Abschabungen an Außenkante der Lehne auf Höhe des oben erwähnten Trommlers.</t>
         </is>
       </c>
-      <c r="B61" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Chief chair of the Kakoma." Shape: armchair in European form but on all 4 sides and on the back with figurative representations from life. Some figures have little brass highlights in their hairstyles. The seat is a tight leather with brown / white fur Condition: (O.Helmcke, January 25th, 1999)&gt; Front) A woman giving birth is missing her right arm. Right outer figure is missing left foot and left upper arm. Middle figure in middle row is missing left earrings&gt; left side) Figure below right is missing left arm. Middle figure in the middle row, flaking on the left bangle. Crack starting from the cone of the top ornament on the front leg&gt; back) Crack in the base of the right leg. Scraping on the vessel, which is held by the lower right figure. Spalling on the collar from the transverse figure&gt; right side) Restored fractures on the arms of the lower middle figure can be seen. Lower left figure probably glued on. Crack in the back of the figure on the front leg&gt; back) The right drummer in the second row from above is missing the right arm. Scraping on the outer edge of the backrest at the level of the drummer mentioned above.</t>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Chief chair of the Kakoma."
+Shape: armchair in European form but on all 4 sides and on the back with figurative representations from life. Some figures have little brass highlights in their hairstyles. The seat is a tight leather with brown / white fur
+Condition: (O.Helmcke, January 25th, 1999)
+&gt; Obverse) Gynecologist missing right arm. Right outer figure is missing left foot and left upper arm. Middle figure in the middle row is missing left earrings
+&gt; left side) figure lower right missing left arm. Middle figure in the middle row, flaking on the left bangle. Crack starting from the cone of the top ornament on the front leg
+Cracked in the base of the right leg. Scraping on the vessel, which is held by the lower right figure. Chipping on the collar of a transverse figure
+&gt; right side) Restored fractures on the arms of the lower middle figure. Lower left figure probably glued on. Crack in the back of the figure on the leg
+&gt; Right) The right drummer in the second row from above is missing the right arm. Scraping on the outer edge of the backrest at the level of the drummer mentioned above.</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -35618,9 +35719,13 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B62" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: ", etsiokum´ face mask made of wood. Defective. Land of the Ekoi" shape: oval, human facial features color: brown pattern: two tattooed scars on the forehead above the root of the nose condition: good.</t>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "etsiokum´ face mask made of wood. Defective. Land of the Ekoi"
+Shape: oval, human facial features
+color: brown
+Pattern: Two tattooed scars on the forehead above the root of the nose
+Condition: good.</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -35635,9 +35740,11 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Ancestral figure, souvenir of deceased relatives" Form: A slim human figure Condition: Good.</t>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Ancestor figure, souvenir of deceased relatives"
+Shape: a slim human figure
+Condition: good.</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -35650,7 +35757,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Becher in Gestalt eines menschlichen Kopfes,aus Holz geschnitzt"</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr">
+      <c r="B64" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Cup in the shape of a human head, carved from wood"</t>
         </is>
@@ -35670,9 +35777,14 @@
 Erhaltungszustand: Spiegel fehlt,</t>
         </is>
       </c>
-      <c r="B65" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Chicoco". Wooden figure (48 cm high); Head black and red, body half black, half painted white, a round mirror in front of the body, several nails in the chest. Beats those who want to inflict evil on the owner of the fetish; hence the position of the figure who put his hands on his knees. Description: Shape: kneeling, open mouth with carved teeth, head jewelry with pieces of bone Color: brown, black, white, red Pattern: painting, carved tires on both wrists Condition: mirror missing,</t>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Chicoco". Wooden figure (48 cm high); Head black and red, body half black, half painted white, a round mirror in front of the body, several nails in the chest. Beats those who want to inflict evil on the owner of the fetish; hence the position of the figure who put his hands on his knees.
+Description:
+Shape: kneeling, open mouth with carved teeth, head jewelry with pieces of bone
+Color: brown, black, white, red
+Pattern: painting, carved hoops on both wrists
+Condition: mirror missing,</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -35686,9 +35798,10 @@
 Kraftfigur von untersetzt, muskulöser Statur. In drohend, leicht nach vorn gebeugter Haltung. Die Hände an die Hüften gelegt.</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "The greatest and most feared idol of the Mayumbe." Power figure of stocky, muscular build. In a threatening, slightly leaning forward position. Put your hands on your hips.</t>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "The greatest and most feared idol of the Mayumbe."
+Power figure of stocky, muscular build. In a threatening, slightly leaning forward position. Put your hands on your hips.</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -35702,9 +35815,10 @@
 Farbe: Rot</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Des. H. 72; Br. 41 cm. Painted red, Bekom? Bangangte?" refers to III C 23807: "Human figure with a vessel on his lap (...)" Color: red</t>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Des. H. 72; Br. 41 cm. Painted red, Bekom? Bangangte?" refers to III C 23807: "human figure with a vessel on his lap (...)"
+Red color</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -35719,9 +35833,11 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "A female figure, carved from wood, sitting with her legs stretched out, holding a wooden lid pot on her lower legs." Color: dark brown Condition: good.</t>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "A female figure, carved from wood, sitting with her legs stretched out, holding a wooden lid pot on her lower legs."
+Color: dark brown
+Condition: good.</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -35734,7 +35850,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Elfenbeinpfeife"</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr">
+      <c r="B69" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Ivory pipe"</t>
         </is>
@@ -35751,9 +35867,11 @@
 Deutsche Expedition 1874</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Fetish from the Loango coast" power figure nkisi lumweno, Vili, Rep. Of Congo, Loango region, 19th century, German expedition in 1874</t>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Fetish from the Loango Coast"
+Power figure nkisi lumweno, Vili, Rep. Of Congo, Loango Region, 19th century
+German expedition 1874</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -35769,9 +35887,12 @@
 Erhaltungszustand: Fragmente fehlen.</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Fetish figure male" Form: nail fetish with glass eyes, a bundle of fabric in the mouth and a carved container for magic mass in front of the stomach. The latter is open and without content. Color: black, white, red Condition: fragments are missing.</t>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Fetish figure male"
+Shape: nail fetish with glass eyes, a bundle of fabric in the mouth and a carved container for magic mass in front of the stomach. The latter is open and without content
+Color: black, white, red
+Condition: fragments are missing.</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -35788,9 +35909,13 @@
 Erhaltungszustand: Medizineinsätze, auf Rücken und Schultern fehlen, Zinken auf dem Kopf fehlen, Kopf und Sockel sind schadhaft</t>
         </is>
       </c>
-      <c r="B72" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Figure with a mirror in front of the belly, humps on the shoulders and back, wooden tines on the head. 50 cm h. Loango" shape: standing, left hand is on the hip, the right hand is raised to shoulder height, around the neck a leather ring, around the hips a dark blue apron held by a cord, the right leg is slightly bent color: brown, black, red, dark blue pattern: painting: face black, body red condition: medical inserts, on back and shoulders missing, tines on the head missing, head and base are damaged</t>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Figure with a mirror in front of the stomach, humps on the shoulders and back, wooden tines on the head. 50 cm h. Loango"
+Shape: standing, left hand lies on the hip, the right hand is raised to shoulder height, a leather ring around the neck, a dark blue apron held by a cord, the right leg is slightly bent
+Color: brown, black, red, dark blue
+Pattern: Painting: black face, red body
+Conservation: medical inserts are missing on the back and shoulders, the tines on the head are missing, the head and base are damaged</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -35807,9 +35932,13 @@
 Erhaltungszustand: Schadhaft (Risse)</t>
         </is>
       </c>
-      <c r="B73" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Gangenbumba, the owner of the house. This fetish, placed in front of the door of a house, protects it more than a lock. Loango (Caio)" shape: sitting on two bars, hands on the mouth, round, unfilled Belly attachment with a hole in the middle, a funnel-shaped hole in the back of the head Color: brown Pattern: carved transverse grooves in the bars Condition: damaged (cracks)</t>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Gangenbumba, the owner of the house. This fetish, placed in front of the door of a house, protects it more than a castle. Loango (Caio)"
+Shape: sitting on two sticks, hands lying on the mouth, round, unfilled belly attachment with a hole in the middle, a funnel-shaped hole in the back of the head
+Color: brown
+Pattern: carved cross grooves in the bars
+Conservation: defective (cracks)</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -35822,9 +35951,9 @@
           <t>Eintrag im historischen Hauptkatalog: "Gesichtsmaske in Ianus-Kopfform aus mit Fell überzogenem Holze. Das eine Gesicht mit schwarzem Barte auf Backen und Kinn."</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Face mask in Ianus head shape made of wood covered with fur. One face with black beard on cheeks and chin."</t>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Face mask in Ianus head shape made of fur covered wood. One face with a black beard on cheeks and chin."</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -35840,9 +35969,12 @@
 Erhaltungszustand: Schadhaft (Risse)</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Gold weight made of brass; smoking Negro with barrel on the head" "Koeten Ganje, a female fetish. There are male and female, but the latter are much more feared. Loango (Caio)" Form: right arm raised, closed Hand at eye level, left arm angled from the body, hand on the hip, a string with a fruit around the neck, a blue cloth is looped around the legs, eyes made of glass color: dark brown, ocher, white, blue Condition: damaged (cracks )</t>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Gold weight made of brass; smoking Negro with barrel on the head" "Koeten Ganje, a female fetish. There are male and female, but the latter are much more feared. Loango (Caio)"
+Shape: right arm raised, closed hand at eye level, left arm angled from the body, hand on the hip, a string with a fruit around the neck, a blue cloth is wrapped around the legs, eyes made of glass
+Color: dark brown, ocher, white, blue
+Conservation: defective (cracks)</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -35857,9 +35989,11 @@
 Erhaltungszustand: Der Bastumhang ist sehr dezimiert.</t>
         </is>
       </c>
-      <c r="B76" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Large dance mask, Manjema. Helmet-like, covering almost the entire head, with a cape made of bast fibers." Color: reddish brown colored wood with blackish parts Condition: The bast cloak is very decimated.</t>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Large dance mask, Manjema. Helmet-like, covering almost the entire head, with a cape made of bast fibers."
+Color: reddish brown colored wood with blackish areas
+Condition: The bast cloak is very decimated.</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -35875,9 +36009,12 @@
 Erhaltungszustand:</t>
         </is>
       </c>
-      <c r="B77" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Large animal figure, fetish very old. Loango? Mayumbe ??" Shape: Wild looking animal confused with different fibers. Condition:</t>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Large animal figure, fetish very old.
+Loango? Mayumbe ?? "
+Shape: Wild looking animal confused with different fibers
+Condition:</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -35891,9 +36028,10 @@
 Farbe: Braun</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Wooden mug, conical, carried on a plate by a central and four peripheral feet. The handle is decorated with a human face and a six-fingered hand. Bakuba." color: brown</t>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Wooden mug, conical, carried on a plate by a central and four peripheral feet. The handle is decorated with a human face and a six-fingered hand. Bakuba."
+color: brown</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -35906,7 +36044,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Holzbecher, Tonnenförmig. Die Ornamente sind mit weißer Farbe eingerieben."</t>
         </is>
       </c>
-      <c r="B79" s="3" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Wooden cup, barrel-shaped. The ornaments are rubbed in with white paint."</t>
         </is>
@@ -35924,9 +36062,12 @@
 Holz, auf sechs Beinen ruhend, geschnitzt</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Wooden mug, similar to the previous one, but resting on 6 bent legs. Ditto [reference as to III 4169] =" Bakuba. Bena Lussambo. "Description: Wood, resting on six legs, carved</t>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Wooden mug, similar to the previous one, but resting on 6 bent legs.
+ditto [reference as III 4169] = "Bakuba. Bena Lussambo."
+Description:
+Wood, resting on six legs, carved</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -35939,9 +36080,9 @@
           <t>Eintrag im historischen Hauptkatalog: "Holzfigur. männlich trägt auf dem Oberkörper einen Behang aus Stofffransen, herausgetriebener Nabel. Der offene Mund zeigt ausgefeilte Zähne. 66 cm hoch. Loango"</t>
         </is>
       </c>
-      <c r="B81" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Wooden figure. Male has a curtain of fabric fringes on his upper body, the navel is driven out. The open mouth shows sophisticated teeth. 66 cm high. Loango"</t>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Wooden figure. Male has a curtain made of fabric fringes on his upper body, his navel is driven out. The open mouth shows sophisticated teeth. 66 cm high. Loango"</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -35954,7 +36095,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Holzlöffel; Stiel mit Menschenkopf verziert."</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Wooden spoon; handle decorated with human head."</t>
         </is>
@@ -35969,7 +36110,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Kamm aus Holz geschnitzt. 8 zinkig"</t>
         </is>
       </c>
-      <c r="B83" s="3" t="inlineStr">
+      <c r="B83" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Carved comb made of wood. 8 teeth"</t>
         </is>
@@ -35984,7 +36125,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Kamm mit Figur"</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr">
+      <c r="B84" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Comb with figure"</t>
         </is>
@@ -36003,9 +36144,13 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B85" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Comb with female figure" For men Shape: With a wide back on which the figure sits and six conical tines Color: Brown Condition: Good.</t>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Comb with female figure"
+For men
+Shape: With a wide back on which the figure sits and six conical tines
+color: brown
+Condition: good.</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -36018,7 +36163,7 @@
           <t>Eintrag im historischen Hauptkatalog: "N'Vali. Sehr alter Fetisch. Loango (Ciao)</t>
         </is>
       </c>
-      <c r="B86" s="3" t="inlineStr">
+      <c r="B86" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "N'Vali. Very old fetish. Loango (Ciao)</t>
         </is>
@@ -36039,9 +36184,15 @@
 c) menschliche Figur als Wächter</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Ngule malang". Fetish (cf. III C 6434). Cylindrical vessel made of tree bark (a); on the edge there are 2 wooden figures (b, c). In the vessel there are 5 skulls (from the chief's grandparents, father, grandfather etc.) (ie ); under the same "medicine", including 2 tin cans and a bark can, filled with redwood (il) wrapped in leaves, 2 spearheads (m, n) and a lot of pieces of bark and wood. Ngumba. Description: c) human figure as a guard</t>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Ngule malang". Fetish (cf. III C 6434).
+Cylindrical vessel made of tree bark (a);
+2 wooden figures sit on the edge (b, c).
+There are 5 skulls in the vessel (from the chief's grandparents, father, grandfather etc.) (d-h); under the same "medicine", including 2 tin cans and a bark can filled with redwood wrapped in leaves (i-l),
+2 spearheads (m, n) and a lot of pieces of bark and wood. Ngumba.
+Description:
+c) human figure as guardian</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -36054,7 +36205,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Opferschale aus Holz geschnitzt mit weiblicher Figur als Henkel."</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Victim bowl carved from wood with a female figure as a handle."</t>
         </is>
@@ -36069,7 +36220,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Scepter"</t>
         </is>
       </c>
-      <c r="B89" s="3" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Scepter"</t>
         </is>
@@ -36084,7 +36235,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Sugunimaske" auf dem oberen Teil stehende weibliche Figur. Muscheln und Perlenverzierung."</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Sugunimaske" female figure standing on the upper part. Shells and pearl ornament. "</t>
         </is>
@@ -36102,9 +36253,12 @@
 Nord Yoruba</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Temple figure; horseman, who perhaps represents the founder of the Jaruba Empire; partly blue, partly colored red." H .: 56 cm. Yagha North Yoruba</t>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Temple figure; horseman, who perhaps represents the founder of the Jaruba Empire; partly blue, partly colored red."
+H .: 56 cm.
+Yagha
+North Yoruba</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -36117,7 +36271,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Ti Suite, Wache, welche der Mann bei seiner Frau lässt, damit diese nicht überfallen wird. Loango (Caio)"</t>
         </is>
       </c>
-      <c r="B92" s="3" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Ti Suite, guard, which the man leaves with his wife so that she is not attacked. Loango (Caio)"</t>
         </is>
@@ -36132,7 +36286,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Zierkamm mit Figur"</t>
         </is>
       </c>
-      <c r="B93" s="3" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Decorative comb with figure"</t>
         </is>
@@ -36147,7 +36301,7 @@
           <t>Eintrag im historischen Hauptkatalog: "Zierkamm mit Vogelmotiv"</t>
         </is>
       </c>
-      <c r="B94" s="3" t="inlineStr">
+      <c r="B94" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: "Ornamental comb with bird motif"</t>
         </is>
@@ -36165,9 +36319,12 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: "Decorative comb with a female figure" Shape: With a broad back on which the figure sits and seven conical tines Color: Brown Condition: Good.</t>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: "Decorative comb with female figure"
+Shape: With a wide back on which the figure sits and seven conical tines
+color: brown
+Condition: good.</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -36181,9 +36338,10 @@
 b: Holzdeckel mit fünf aufgeschnitzten Figuren</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: (a: Cabinda pot) b: Wooden lid with five carved figures</t>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: (a: Cooking pot from Cabinda)
+b: wooden lid with five carved figures</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -36196,7 +36354,7 @@
           <t>Eintrag im historischen Hauptkatalog: Alte Form des Balubamessers, [...] Fetisch.</t>
         </is>
       </c>
-      <c r="B97" s="3" t="inlineStr">
+      <c r="B97" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Old form of the baluba knife, [...] fetish.</t>
         </is>
@@ -36214,9 +36372,12 @@
 Ähnliches Beil (wie III C 4206 mit Skizze im Katalog) mit gleichen Ornamenten, Schaft mit Kupfer überzogen</t>
         </is>
       </c>
-      <c r="B98" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Biel as [III C9 4211. ditto [Geo reference as III C 4208] = "Bassonge". Description: Similar ax (like III C 4206 with sketch in the catalog) with the same ornaments, shaft covered with copper</t>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Biel as [III C9 4211.
+ditto [reference like III C 4208] = "Bassonge".
+Description:
+Similar hatchet (like III C 4206 with sketch in the catalog) with the same ornaments, shaft covered with copper</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -36231,9 +36392,11 @@
 Eine weibliche Figur mit einem Spazierstock in der Rechten und einem tassenänhlichen Gefäß in der Linken. Auffällig ist der sehr lange Hals.KB-5</t>
         </is>
       </c>
-      <c r="B99" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Buanga, female Fetish. Bakuanpiko. Baluba. Description: A female figure with a walking stick in her right hand and a cup-like vessel in her left. The very long neck is striking.KB-5</t>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Buanga, female Fetish. Bakuanpiko. Baluba.
+Description:
+A female figure with a walking stick in her right hand and a cup-like container in her left. The very long neck is striking.KB-5</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -36246,7 +36409,7 @@
           <t>Eintrag im historischen Hauptkatalog: desgl. [wie III C 1706] = "Spielschild", vorn mit geflochtenen Ornamenten versehen. Hinten beflochten u. mit Holzgriff versehen. Baschilange.</t>
         </is>
       </c>
-      <c r="B100" s="3" t="inlineStr">
+      <c r="B100" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: like [III C 1706] = "Spielschild", with braided ornaments on the front. Braided on the back and provided with wooden handle. Baschilange.</t>
         </is>
@@ -36265,9 +36428,13 @@
 Erhaltungszustand: Leicht schadhaft (Risse im Sockel)</t>
         </is>
       </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Desgl. [as III C 8107] = "fetish". Protects against wounds in war. Jesmitti. 24 cm high figure. Bawili. Description: Shape: flat torso, arms close to the body, violet wrapping covers the lower body and legs, cord wrapped under the drape, glass eyes, carved groove behind the right ear Color: black-brown, violet Condition: slightly damaged (cracks in the base )</t>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Desgl. [as III C 8107] = "fetish". Protects against wounds in war. Jesmitti. 24 cm high figure. Bawili.
+Description:
+Shape: flat torso, arms close to the body, violet wrapping covers the lower body and legs, cord wrapped under the cloth, glass eyes, carved groove behind the right ear
+Color: black-brown, violet
+Condition: slightly damaged (cracks in the base)</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -36280,7 +36447,7 @@
           <t>Eintrag im historischen Hauptkatalog: Die Ruhefläche wird von einer knienden Frauengestalt, mit einer Kreuzfrisur am Hinterkopf und einem Kleinkind auf dem Rücken, auf den ausgestreckten Händen getragen.</t>
         </is>
       </c>
-      <c r="B102" s="3" t="inlineStr">
+      <c r="B102" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: The resting area is carried on the outstretched hands by a kneeling female figure, with a cross hairstyle on the back of the head and a toddler on the back.</t>
         </is>
@@ -36298,9 +36465,12 @@
 Erhaltungszustand: sehr gut</t>
         </is>
       </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: dto. [As III C 1102] = "ivory carving" shape: rod, at the upper end a raised carved ring, above it a carving: an egg held by a bird's foot color: ivory condition: very good</t>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: dto. [As III C 1102] = "ivory carving"
+Shape: stick, at the upper end a raised carved ring, above a carving: an egg held by a bird's foot
+Color: ivory
+Condition: very good</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -36316,9 +36486,12 @@
 Erhaltungszustand: sehr gut</t>
         </is>
       </c>
-      <c r="B104" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Ivory carving from Ambriz. Shape: rod, upper end columnar, a monkey squats on a platform. Color: ivory. Condition: very good</t>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Ivory carving from Ambriz.
+Shape: rod, upper end columnar, a monkey perches on a platform
+Color: ivory
+Condition: very good</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -36331,7 +36504,7 @@
           <t>Eintrag im historischen Hauptkatalog: Elfenbeinschnitzerei.</t>
         </is>
       </c>
-      <c r="B105" s="3" t="inlineStr">
+      <c r="B105" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: ivory carving.</t>
         </is>
@@ -36346,7 +36519,7 @@
           <t>Eintrag im historischen Hauptkatalog: Fetisch</t>
         </is>
       </c>
-      <c r="B106" s="3" t="inlineStr">
+      <c r="B106" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Fetish</t>
         </is>
@@ -36363,9 +36536,11 @@
 (It. Etikett: Klingelhöfer)</t>
         </is>
       </c>
-      <c r="B107" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Fetish German Expedition 1874 (label: Klingelhöfer)</t>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Fetish
+German expedition 1874
+(It. Label: Klingelhöfer)</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -36379,9 +36554,10 @@
 Eine dünne Schlange ist um den Körper geschlungen, daran hängt ein Zahn. Eisenhaken zum Tragen der Figur.</t>
         </is>
       </c>
-      <c r="B108" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Wooden fetish nailed with copper buttons. Taken away from a sick man's house. 20 cm high. Bassonge. A thin snake is wrapped around the body with a tooth attached to it. Iron hook for carrying the figure.</t>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Wooden fetish nailed with copper buttons. Taken away from a sick man's house. 20 cm high. Bassonge.
+A thin snake is wrapped around the body with a tooth attached to it. Iron hook for carrying the figure.</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -36398,9 +36574,13 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B109" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Fetish hung over shoulder [...] Mayombe. Description: Shape: monkey figure, a tube-like intermediate piece with faces and an antelope croissant are loosely connected by means of bast cord. Color: brown, white (remnants), black Condition: good.</t>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Fetish hung over shoulder [...] Mayombe.
+Description:
+Shape: monkey figure, a tube-like intermediate piece with faces and an antelope croissant are loosely connected with bast cord
+Color: brown, white (remains), black
+Condition: good.</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -36413,7 +36593,7 @@
           <t>Eintrag im historischen Hauptkatalog: Fetisch. Boabercote (Bambocotó). Zweck wie bei [III C] 8097. 35 cm hoch. Bawili.</t>
         </is>
       </c>
-      <c r="B110" s="3" t="inlineStr">
+      <c r="B110" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Fetish. Boabercote (Bambocotó). Purpose as in [III C] 8097. 35 cm high. Bawili.</t>
         </is>
@@ -36428,7 +36608,7 @@
           <t>Eintrag im historischen Hauptkatalog: Fetischmuschel</t>
         </is>
       </c>
-      <c r="B111" s="3" t="inlineStr">
+      <c r="B111" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: fetish shell</t>
         </is>
@@ -36445,9 +36625,11 @@
 Farbe: Elfenbeinweiß</t>
         </is>
       </c>
-      <c r="B112" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Ivory flute. Russuna Shape: A human head is carved on the tip. Color: Ivory white</t>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Ivory flute. Russuna
+Shape: A human head is carved on the tip
+Color: ivory white</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -36460,7 +36642,7 @@
           <t>Eintrag im historischen Hauptkatalog: Gurt mit Muschelbesatz. Bakuba.</t>
         </is>
       </c>
-      <c r="B113" s="3" t="inlineStr">
+      <c r="B113" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Belt with shell trim. Bakuba.</t>
         </is>
@@ -36479,9 +36661,13 @@
 Farbe: Braun, weiß, rosa, rot, gelb</t>
         </is>
       </c>
-      <c r="B114" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: necklace with fetish figures (Luanda). Description: String of pearls with two wooden figures. Shape: String of pearls is four rows, at irregular intervals summarized by larger pearls. Color: brown, white, pink, red, yellow</t>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: necklace with fetish figures (Luanda).
+Description:
+String of pearls with two wooden figures.
+Shape: String of pearls is four rows, at irregular intervals summarized by larger pearls
+Color: brown, white, pink, red, yellow</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -36495,9 +36681,10 @@
 dito. [GeoBezug wie III 4169] = "Bakuba. Bena Lussambo."</t>
         </is>
       </c>
-      <c r="B115" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: wooden cup, richly carved, bulbous. dito. [Geo reference as III 4169] = "Bakuba. Bena Lussambo."</t>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: wooden cup, richly carved, bulbous.
+dito. [Geo reference as III 4169] = "Bakuba. Bena Lussambo."</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -36513,9 +36700,12 @@
 Form: Maske, Holz, Gesicht weiss, Frisur schwarz bemalt. Asiatisch anmutend, ovales Gesicht, Schlitzaugen, sichelförmige strichbreite Augenbrauen, Mund sowie Nase klein und spitz</t>
         </is>
       </c>
-      <c r="B116" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Wooden mask with filed incisors from the area north of the lower Congo. Description: Mask, wood, face white, hairstyle painted black. Shape: mask, wood, face white, hairstyle painted black. Asian-style, oval face, slit eyes, crescent-shaped stroke-wide eyebrows, mouth and nose small and pointed</t>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Wooden mask with filed incisors from the area north of the lower Congo.
+Description:
+Mask, wood, face white, hairstyle painted black.
+Shape: mask, wood, face white, hairstyle painted black. Asian-style, oval face, slit eyes, crescent-shaped stroke-wide eyebrows, mouth and nose small and pointed</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -36531,9 +36721,12 @@
 Gefäß mit Deckel, Schlangen- und Drachendarstellungen. Der Decke wird von einer weiblichen Figur verziert.</t>
         </is>
       </c>
-      <c r="B117" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Goblet-like jar with lid. Ivory with snakes and dragons. Formerly IA87 Schaunn [r] .: 2849. Description: Vessel with lid, depicting snakes and dragons. The ceiling is decorated with a female figure.</t>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Goblet-like jar with lid. Ivory with snakes and dragons.
+Formerly I.A. 87 Schaunn [r] .: 2849.
+Description:
+Vessel with lid, depicting snakes and dragons. The ceiling is decorated with a female figure.</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -36547,9 +36740,10 @@
 Karteikarte : Eine menschenähliche Figur mit Kupferbeschlägen, Schurz, Schlangenteile darum sowie um den Hals und 2 Kauris als Augen</t>
         </is>
       </c>
-      <c r="B118" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Small fetish made of wood with copper fittings and fur and snake skin clothing. H. 18 cm. See [III C] 1792. Probably Bassonge. Index card: A human figure with copper fittings, apron, snake parts around it as well as around the neck and 2 cowries as eyes</t>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Small fetish made of wood with copper fittings and fur and snake skin clothing. H. 18 cm. See [III C] 1792. Probably Bassonge.
+Index card: A human figure with copper fittings, apron, snake parts around it as well as around the neck and 2 cowries as eyes</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -36562,7 +36756,7 @@
           <t>Eintrag im historischen Hauptkatalog: Kopfaufsatz ("Maske"),Holz, langhörniges Tier ohne Füsse. Kopf, Hals und Körper aus verschiedenen Stücken zusammengefügt.</t>
         </is>
       </c>
-      <c r="B119" s="3" t="inlineStr">
+      <c r="B119" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: headpiece ("mask"), wood, long-horned animal without feet. Head, neck and body put together from different pieces.</t>
         </is>
@@ -36577,7 +36771,7 @@
           <t>Eintrag im historischen Hauptkatalog: Kupferring (verziert) von Chicambo.</t>
         </is>
       </c>
-      <c r="B120" s="3" t="inlineStr">
+      <c r="B120" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Copper ring (decorated) by Chicambo.</t>
         </is>
@@ -36593,9 +36787,10 @@
 Deutsche Expedition 1874</t>
         </is>
       </c>
-      <c r="B121" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Music pipe (?) German expedition 1874</t>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: music pipe (?)
+German expedition 1874</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -36608,7 +36803,7 @@
           <t>Eintrag im historischen Hauptkatalog: Nadel aus Knochen mit schwarzen Einlegungen.</t>
         </is>
       </c>
-      <c r="B122" s="3" t="inlineStr">
+      <c r="B122" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Bone needle with black inlays.</t>
         </is>
@@ -36623,7 +36818,7 @@
           <t>Eintrag im historischen Hauptkatalog: Rassel zum Aufhängen, drei Klöppel</t>
         </is>
       </c>
-      <c r="B123" s="3" t="inlineStr">
+      <c r="B123" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: rattle for hanging, three clappers</t>
         </is>
@@ -36638,7 +36833,7 @@
           <t>Eintrag im historischen Hauptkatalog: Saiteninstrument. Bakuba. (vgl. Im Innern Afrikas S. 253)</t>
         </is>
       </c>
-      <c r="B124" s="3" t="inlineStr">
+      <c r="B124" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: stringed instrument. Bakuba. (cf. Inside Africa p. 253)</t>
         </is>
@@ -36656,9 +36851,12 @@
 Messergriff aus Eisen mit einem kunstvoll gearbeitetem Menschenkopf als Knauf und Kupferringen um die Griffläche.</t>
         </is>
       </c>
-      <c r="B125" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Narrow knife, including the handle 53 cm long; forged from a piece of iron. The pommel is formed by a human head excellently cut in iron, the long handle is otherwise square, with 8 and 4 wide iron and copper rings on the top and bottom. ditto [Geo reference like III C 4218] = "Bassonge. East of Lomami." Description: Knife handle made of iron with an artistically crafted human head as a knob and copper rings around the handle surface.</t>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Narrow knife, including the handle 53 cm long; forged from a piece of iron. The pommel is formed by a human head excellently cut in iron, the long handle is otherwise square, with 8 and 4 wide iron and copper rings on the top and bottom.
+ditto [Geo reference like III C 4218] = "Bassonge. East of Lomami."
+Description:
+Knife handle made of iron with an artistically worked human head as a knob and copper rings around the handle surface.</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -36671,7 +36869,7 @@
           <t>Eintrag im historischen Hauptkatalog: Wurfmesser und Scheide.</t>
         </is>
       </c>
-      <c r="B126" s="3" t="inlineStr">
+      <c r="B126" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: throwing knife and sheath.</t>
         </is>
@@ -36687,9 +36885,10 @@
 dito [GeoBezug wie III C 4208] =  Bassonge.</t>
         </is>
       </c>
-      <c r="B127" s="3" t="inlineStr">
-        <is>
-          <t>Entry in the historical main catalog: Similar ax [like III C 4206] with the same ornaments, shaft covered with copper. ditto [reference as III C 4208] = Bassonge.</t>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Entry in the historical main catalog: Similar ax [like III C 4206] with the same ornaments, shaft covered with copper.
+ditto [reference as III C 4208] = Bassonge.</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -36702,7 +36901,7 @@
           <t>Eintrag im historischen Hauptkatalog:Ditto ]wie III C 2653] = "Messer". geschweifte Klinge.</t>
         </is>
       </c>
-      <c r="B128" s="3" t="inlineStr">
+      <c r="B128" t="inlineStr">
         <is>
           <t>Entry in the historical main catalog: Ditto] as III C 2653] = "knife". curly blade.</t>
         </is>
@@ -36717,7 +36916,7 @@
           <t>Fidschianische Töpferwaren wurden keiner hohen Hitze beim Brennen ausgesetzt, daher waren sie nicht ganz wasserdicht. Ein Harz vom dakua-Baum (Agathis vitiensis), das auf die heiße Oberfläche aufgetragen wurde, ergab einen bräunlichen, halbdurchlässigen Firnis.</t>
         </is>
       </c>
-      <c r="B129" s="3" t="inlineStr">
+      <c r="B129" t="inlineStr">
         <is>
           <t>Fijian pottery was not exposed to high heat when fired, so it was not completely waterproof. A resin from the dakua tree (Agathis vitiensis), which was applied to the hot surface, gave a brownish, semi-permeable varnish.</t>
         </is>
@@ -36732,9 +36931,9 @@
           <t>Figur soll wohl ein Krokodil mit geöffnetem Maul darstellen; braun eingefärbt; Schwanz und Rücken bunt bemalt; z.T. mit runden und eckigen geometrischen Mustern versehen.</t>
         </is>
       </c>
-      <c r="B130" s="3" t="inlineStr">
-        <is>
-          <t>Figure is supposed to represent a crocodile with its mouth open; colored brown; Colorfully painted tail and back; some with round and angular geometric patterns.</t>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Figure is supposed to represent a crocodile with its mouth open; colored brown; Colorfully painted tail and back; partly provided with round and angular geometric patterns.</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -36749,9 +36948,11 @@
 Karteikarte  "Bei den Bamum ist die doppelköpfige Schlange Wahrzeichen des Königtums und gleichzeitig Hüterin des heiligen Feuers"</t>
         </is>
       </c>
-      <c r="B131" s="3" t="inlineStr">
-        <is>
-          <t>Form: As a double-headed snake, main catalog: "TAMTON tobacco pipe. Head and the pipe made of brass made of 2 teles. Double head, in the form of a two-headed snake." Index card "For the Bamum, the double-headed serpent is the symbol of the kingship and at the same time guardian of the holy fire"</t>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Shape: As a double-headed snake
+Main catalog: "TAMTON tobacco pipe. Head and the brass tube made of 2 teles. Double head, in the form of a two-headed snake."
+Index card "For the Bamum, the double-headed serpent is the symbol of the kingship and at the same time guardian of the holy fire"</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -36764,7 +36965,7 @@
           <t>Form: Dunkle Gesichtsmaske aus Holz mit einem Eisennagel, der aus dem Kinn hervorragt. Sonstige Merkmale: Breiter, vorstehender Mund und Schlitzaugen.</t>
         </is>
       </c>
-      <c r="B132" s="3" t="inlineStr">
+      <c r="B132" t="inlineStr">
         <is>
           <t>Shape: Dark wooden face mask with an iron nail sticking out of the chin. Other features: Wide, protruding mouth and slit eyes.</t>
         </is>
@@ -36781,9 +36982,11 @@
 Karteikarte  "Pfeifenkopf aus Ton mit roter Glasur und teilweise schwarzer Bemalung. Kleiner Pfeifenkopf (7 cm) und spiztwinklig dazu ein höheres Pfeifenrohransatzstück. Beid emit Stef verbunden...stark stilisertes Eidecksenmotiv"</t>
         </is>
       </c>
-      <c r="B133" s="3" t="inlineStr">
-        <is>
-          <t>Shape: corrugated head, pipe attachment with strongly stylized lizards (spiders?) Motif Color: red, black index card "Pipe bowl made of clay with red glaze and partly black painting. Small pipe bowl (7 cm) and at a sharp angle a higher pipe pipe attachment. Both connected to Stef ... highly stylized lizard motif "</t>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Shape: ribbed head, tube attachment with strongly stylized lizards (spiders?) Motif
+Color: red, black
+Index card "Pipe bowl made of clay with red glaze and partly black painting. Small pipe bowl (7 cm) and at a sharp angle a higher pipe pipe attachment. Both connected to Stef ... highly stylized corner motif"</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -36797,9 +37000,10 @@
 Farbe: Schwarz</t>
         </is>
       </c>
-      <c r="B134" s="3" t="inlineStr">
-        <is>
-          <t>Shape: head mask with human, chubby face. On her head she carries a basket-like structure made of spider motifs. Color: black</t>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Shape: head mask with human, chubby face. On her head she carries a basket-like structure made of spider motifs
+Color: Black</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -36818,9 +37022,15 @@
 Gerhard Kubik: Kalimba, Nsansi, Mbira - Lamellophone in Afrika: Veröffentlichungen des Museums für Völkerkunde Berlin (SMB), 1998 - Neue Folge 68 - Musikethnologie X, S. 174-175 (Abb. 121 / Abb. 122)</t>
         </is>
       </c>
-      <c r="B135" s="3" t="inlineStr">
-        <is>
-          <t>Form: Solid wooden body with iron lamellas, detailed description in: Kubik, Lamellophone (1998), pp. 174-5 The instrument is characterized by its two rows of lamellae arranged one above the other. The bottom row of 3 plus 3, the top of 3 plus 4 slats. The specimen has indicated increases in the left and right edges of the board: so-called lateral ridges. The clipboard has a figurative motif engraved in relief within a rhombus outline. Gerhard Kubik: Kalimba, Nsansi, Mbira - Lamellophones in Africa: Publications of the Museum für Völkerkunde Berlin (SMB), 1998 - New episode 68 - Musikethnologie X, pp. 174-175 (Fig. 121 / Fig. 122)</t>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Shape: Solid wooden body with iron slats
+exact description in:
+Kubik, Lamellophone (1998), pp. 174-5
+The instrument is characterized by its two rows of lamellae arranged one above the other. The bottom row of 3 plus 3, the top of 3 plus 4 slats.
+The specimen has indicated increases in the left and right edges of the board: so-called lateral ridges.
+The clipboard has a figurative motif engraved in relief within a rhombus outline.
+Gerhard Kubik: Kalimba, Nsansi, Mbira - Lamellophones in Africa: Publications of the Museum für Völkerkunde Berlin (SMB), 1998 - New episode 68 - Musikethnologie X, pp. 174-175 (Fig. 121 / Fig. 122)</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -36833,7 +37043,7 @@
           <t>Frauenschleier; gefochten</t>
         </is>
       </c>
-      <c r="B136" s="3" t="inlineStr">
+      <c r="B136" t="inlineStr">
         <is>
           <t>Women's veil; fought</t>
         </is>
@@ -36848,7 +37058,7 @@
           <t>Fuß eines afro-portugiesischen Salzgefäßes aus Elfenbein mit zwei männlichen und zwei weiblichen Figuren sowie einigen Tierdarstellungen. Solche Salzgefäße schnitzten Sapi-Künstler an der westafrikanischen Küste Ende des 15. Jh. und Anfang des 16. Jhs als Auftragsarbeiten für reisende Portugiesen. Sie wurden nach Europa gebracht, wo Herrscher sie für ihre Kunstkammer begehrten. Der Oberteil dieses Gefäßes wurde früher von dem Fuß abgetrennt, und nur der Fuß befindet sich im Bestand des Museums. (JF 16.05.2017)</t>
         </is>
       </c>
-      <c r="B137" s="3" t="inlineStr">
+      <c r="B137" t="inlineStr">
         <is>
           <t>Foot of an Afro-Portuguese salt vessel made of ivory with two male and two female figures and some animal representations. Sapi artists carved such salt vessels on the West African coast at the end of the 15th century and beginning of the 16th century as commissioned work for traveling Portuguese. They were brought to Europe, where rulers wanted them for their art chamber. The upper part of this vessel was previously separated from the foot, and only the foot is in the museum's holdings. (JF May 16, 2017)</t>
         </is>
@@ -36866,9 +37076,12 @@
 Das Trinkorn, Geschenk Stumms an den preußischen König, wurde der ethnolog. Sammlung übergeben. (Vgl. AKt. 954/68): "... von dem Gefährten des Rohlfs, dem Lieutnant Stumm, ...: ein Trinkhorn von Büffelhorn mit Lederüberzug, welches an dem aus Metall gefertigtem Mundstück die Inschrift : "Trinkhorn des Kaisers Theodoros von Abissinien - Magdala 13. April 1868," trägt und mit einem Pfropfen von Holz mit metallener Kugel versehen ist. Mit Rücksicht darauf, dass diese Gegenstände auch für das größere Publikum von Interesse sind, haben Seine Majestät der König beschlossen, dieselben - vorbehaltlich Allerhöchst ihres Eigentumsreich - der ethnographischen Sammlung der Museen zu überweisen. ..." (Brief des Geheim Kabinets-Rathes von Mühler an den Generaldirektor der Kgl. Museen, Dr. von Olfers.)</t>
         </is>
       </c>
-      <c r="B138" s="3" t="inlineStr">
-        <is>
-          <t>History of the bottle (see file process E.1126 / 1868, sheet 5 (Stumm) and file process E 954/1868): "The present drinking horn was mine (Stumm, A. d. V.) during the storm and the ingestion discovered by Magdala by the English on April 13, 1868, in the tents of the emperor Theodoros of Abyssinia, ... one of the first to climb over and encircle the enclosure of the fortress, in which Theodors had locked himself with 19 companions I the corpse of the emperor, apparently barely a few moments after Theodoros committed suicide by a pistol shot, not far from the entrance to the tent, which, because of its size and magnificence, was immediately recognizable as that of the emperor: a divan and a lot blankets heaped on top of each other took up the interior, and on the former lay the drinking horn, still half-filled with araki, apparently the last item of everyday use by the emperor known for his drunkenness The drinking horn consisted of a wooden stopper with a brass button, the latter of which was lost during transport to the coast, and which I later restored in Germany, according to the original form, in ... (illegible) silver. " Florence December 1, 1868. Silent, second lieutenant à la suite of the Hanover Hussar Regiment No. 15 (letter to Wilhelm I of Prussia). The drinking horn, Stumm's gift to the Prussian king, became the ethnolog. Hand over collection. (Cf. Act 954/68): "... by the companion of Rohlfs, Lieutenant Stumm, ...: a drinking horn by Büffelhorn with leather cover, which has the inscription on the mouthpiece made of metal:" Drinking horn of the emperor Theodoros von Abisslinien - Magdala April 13, 1868, "and is provided with a graft of wood with a metal ball. Considering that these objects are also of interest to the larger public, His Majesty the King decided to reserve them - subject to the Supreme your property - to be transferred to the ethnographic collection of the museums ... "(Letter from the secret cabinet council of Mühler to the general director of the royal museums, Dr. von Olfers.)</t>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>History of the bottle (see file process E.1126 / 1868, sheet 5 (silent) and file process E 954/1868):
+"The present drinking horn was found by me (Stumm, A. d. V.) during the storm and the English taking Magdala on April 13, 1868, in the tents of the Emperor Theodoros of Abyssinia, ...
+As one of the first to climb over the fence of the fortress, in which Theodors had locked himself with 19 companions, I found the body of the emperor, apparently hardly a moment after Theodoros had committed suicide by shooting a pistol far from the entrance to the tent, which, because of its size and grandeur, was immediately recognizable as that of the emperor. A divan and a lot of blankets heaped on top of each other took up the interior, and on the first one was the drinking horn, still half-filled with araki, apparently the last item of use by the emperor, who was known for his alcoholism. - The closure of the drinking horn consisted of a wooden stopper with a brass button, the latter was lost during transport to the coast, and was later restored by me in Germany, according to the original form, in ... (illegible) silver. "Florence the 1st December 1868. Signed Stumm, second lieutenant à la suite of the Hanover Hussar Regiment No. 15 (letter to Wilhelm I of Prussia).
+The drinking horn, Stumm's gift to the Prussian king, became the ethnolog. Hand over collection. (Cf. Act 954/68): "... by the companion of Rohlfs, Lieutenant Stumm, ...: a drinking horn by Büffelhorn with leather cover, which has the inscription on the mouthpiece made of metal:" Drinking horn of Emperor Theodoros von Abissinia - Magdala April 13, 1868, "and is provided with a graft of wood with a metal ball. Considering that these objects are also of interest to the larger public, His Majesty the King decided to reserve them - subject to the Supreme your property - to be transferred to the ethnographic collection of the museums ... "(Letter from the secret cabinet council of Mühler to the general director of the royal museums, Dr. von Olfers.)</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -36882,9 +37095,10 @@
 Eintrag im historischen Hauptkatalog:  "Ein holzgeschnitzter Menschenkopf in Becherform. Mit Kunstvoller Frisur und eingewogenem Becherrand."</t>
         </is>
       </c>
-      <c r="B139" s="3" t="inlineStr">
-        <is>
-          <t>Carved mug in the shape of a human head with a bulbous hairstyle. The opening is from the bottom of the neck. Entry in the historical main catalog: "A wooden carved human head in the shape of a cup. With an artistic hairstyle and a weighed-in cup rim."</t>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Carved mug in the shape of a human head with a bulbous hairstyle. The opening is from the bottom of the neck.
+Entry in the historical main catalog: "A wooden carved human head in the shape of a cup. With an artistic hairstyle and a weighed-in cup rim."</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -36897,7 +37111,7 @@
           <t>Hacke aus Holz, besteht aus Stiel und langer, schmaler Schaufel, beides mit Rofang verbunden. Der unter runde Teilder schnur ist mit einscharfkantig. Stück Eisen umgeben.KB-119</t>
         </is>
       </c>
-      <c r="B140" s="3" t="inlineStr">
+      <c r="B140" t="inlineStr">
         <is>
           <t>Hoe made of wood, consists of a handle and a long, narrow shovel, both connected with rofang. The lower part of the cord is with a sharp edge. Piece of iron surrounded. KB-119</t>
         </is>
@@ -36912,7 +37126,7 @@
           <t>Hauptkatalog:  dito [= III C 29319: "kusson" Ahnenkrug aus Ton]</t>
         </is>
       </c>
-      <c r="B141" s="3" t="inlineStr">
+      <c r="B141" t="inlineStr">
         <is>
           <t>Main catalog: Ditto [= III C 29319: "kusson" ancestral jug made of clay]</t>
         </is>
@@ -36928,9 +37142,10 @@
 Hausa, Anka</t>
         </is>
       </c>
-      <c r="B142" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: drum. "Tabshi" Hausa, Anka</t>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Main catalog: drum. "Tabshi"
+Hausa, Anka</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -36945,9 +37160,11 @@
 Wawemba (Muliro)"</t>
         </is>
       </c>
-      <c r="B143" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "" muâna, plur .: vâna "Doll made of wood, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say if they carry the doll: 'This is my child I gave birth to.' 26 cm h. Wawemba (Muliro) "</t>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Main catalog: "" muâna, plur .: vâna "Doll made of wood, without head, with tattoo. For girls. They are carried on the shoulder by them, even in adulthood until they have a child. They say if they carry the doll: 'This is my child I gave birth to.'
+26 cm h.
+Wawemba (Muliro) "</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -36961,9 +37178,10 @@
 Karteikarte  "ein Paar Perlenarmringe, von Frauen getragen, von dunkelblauer und hellblauer Farbe, KATA"</t>
         </is>
       </c>
-      <c r="B144" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "1 pair of pearls worn by women" index card "a pair of pearl bracelets, worn by women, of dark blue and light blue color, KATA"</t>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Main catalog: "1 pair of pearls worn by women"
+Index card "a pair of pearl bracelets, worn by women, of dark blue and light blue color, KATA"</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -36977,9 +37195,10 @@
 Karteikarte  "aus Kupferbronze"</t>
         </is>
       </c>
-      <c r="B145" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "2 ear pegs made of brass, mushroom-shaped. For women. Now out of fashion, replaced by pearl-knitted earbuds), disc" index card "made of copper bronze"</t>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Main catalog: "2 ear pegs made of brass, mushroom-shaped. For women. Now out of fashion, replaced by pearl-knitted earbuds), disc"
+Index card "made of copper bronze"</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -36992,7 +37211,7 @@
           <t>Hauptkatalog: "Ahnenmaske, männlich."</t>
         </is>
       </c>
-      <c r="B146" s="3" t="inlineStr">
+      <c r="B146" t="inlineStr">
         <is>
           <t>Main catalog: "Ancestral mask, male."</t>
         </is>
@@ -37007,7 +37226,7 @@
           <t>Hauptkatalog: "Geschenk des Oberhäuptlings Joya von Bamum"</t>
         </is>
       </c>
-      <c r="B147" s="3" t="inlineStr">
+      <c r="B147" t="inlineStr">
         <is>
           <t>Main catalog: "Gift from Chief Joya von Bamum"</t>
         </is>
@@ -37024,9 +37243,11 @@
 Wawemba (Muliro)"</t>
         </is>
       </c>
-      <c r="B148" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "Carved male wooden figure, colored red. Made by a Wawemba Askari. 58.5 cm high. Wawemba (Muliro)"</t>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Main catalog: "Carved male wooden figure, colored red. Made by a Wawemba Askari.
+58.5 cm h.
+Wawemba (Muliro) "</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -37041,9 +37262,11 @@
 Urua."</t>
         </is>
       </c>
-      <c r="B149" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "Wooden figure. Female. Purpose? 28 cm high. Urua."</t>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Main catalog: "Wooden figure. Female. Purpose?
+28 cm high.
+Urua. "</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -37061,9 +37284,14 @@
 Erhaltungszustand: Mehrere senkrechte Risse in Kopf und Körper.</t>
         </is>
       </c>
-      <c r="B150" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "Wooden doll with carved head. 27.8 cm h. Wawmba (Muliro)" Female. Cylindrical body with breasts, navel and several ring grooves on both ends. The face has neither eyes nor mouth. Color: medium brown. Condition: Several vertical cracks in the head and body.</t>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Main catalog: "Wooden doll with carved head.
+27.8 cm h.
+Wawmba (Muliro) "
+Female. Cylindrical body with breasts, navel and several ring grooves on both ends. The face has neither eyes nor mouth
+Color: medium brown
+Condition: Several vertical cracks in the head and body.</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -37076,9 +37304,9 @@
           <t>Hauptkatalog: "Streitaxt des älteren Sohnes des Häuptlings Zappu Zapp, Stiel ganz mit Kupfer überzogen, Klinge durchbrochen gearbeitet, mit 6 menschlichen Köpfen verziert. Die Bassonge Fürsten sollen als Lohn für ihre Kriegsthaten an ihre Krieger die Befugnis verleihen, sich beile oder Messer mit solchen Köpfen machen zu lassen."</t>
         </is>
       </c>
-      <c r="B151" s="3" t="inlineStr">
-        <is>
-          <t>Main catalog: "Battle ax of the elder son of the chief Zappu Zapp, handle entirely covered with copper, blade worked openwork, decorated with 6 human heads. The Bassonge princes are to reward their warriors with the authority to hurry up or use knives with them as a reward for their war deeds To have heads made. "</t>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Main catalog: "Battle ax of the older son of the chief Zappu Zapp, handle entirely covered with copper, blade worked openwork, decorated with 6 human heads. The Bassonge princes are to reward their warriors with the authority to hurry up or use knives with such wares as a reward To have heads made. "</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -37091,7 +37319,7 @@
           <t>Hauptkatalog: Messinghalsring einer Frau (auch von Männern getragen). Vierkantig. Enden zu Hacken gebogen.</t>
         </is>
       </c>
-      <c r="B152" s="3" t="inlineStr">
+      <c r="B152" t="inlineStr">
         <is>
           <t>Main catalog: brass neck ring of a woman (also worn by men). Square. Ends bent into hoes.</t>
         </is>
@@ -37109,9 +37337,12 @@
 Erhaltungszustand: Gut.</t>
         </is>
       </c>
-      <c r="B153" s="3" t="inlineStr">
-        <is>
-          <t>Historical entry in the main catalog: "Dance mask, wood. Bongo South Sudan" Shape: Elongated face, pointed nose, rectangular mouth and eye openings. Remains of a mustache, stone chips as teeth Color: brown, beige Condition: good.</t>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Historical entry in the main catalog: "Dance mask, wood. Bongo South Sudan"
+Shape: Long face, pointed nose, rectangular mouth and eye openings. Remains of a mustache, stone chips as teeth
+Color: brown, beige
+Condition: good.</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -37128,9 +37359,13 @@
 und Urambia)."</t>
         </is>
       </c>
-      <c r="B154" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'kisago'. Wooden head bench. 19 cm high, 24 cm long. Wanyika work (from Tschitete, border between Unyika and Urambia)."</t>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'kisago'. Wooden head bench.
+19 cm h., 24 cm lg.
+Wanyika work
+(from Tschitete, border between Unyika
+and Urambia). "</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -37143,7 +37378,7 @@
           <t>Historischer Hauptkatalog:  " 'kula'. Halskette. Lederriemen mit Kauris. Waniramba (Sultan Kivioma)"</t>
         </is>
       </c>
-      <c r="B155" s="3" t="inlineStr">
+      <c r="B155" t="inlineStr">
         <is>
           <t>Historical main catalog: "'kula'. Necklace. Leather straps with cowries. Waniramba (Sultan Kivioma)"</t>
         </is>
@@ -37160,9 +37395,11 @@
 Ebendaher [Kinyangiri, Iramba]."</t>
         </is>
       </c>
-      <c r="B156" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'mpingo (mapingo).' 4 wooden ear pegs (b covered with tinfoil). 5.3 cm diameter. Ebendaher [Kinyangiri, Iramba]. "</t>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'mpingo (mapingo).' 4 wooden ear pegs (b covered with tin foil).
+5.3 cm diameter
+Therefore [Kinyangiri, Iramba]. "</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -37178,9 +37415,12 @@
 Marungu."</t>
         </is>
       </c>
-      <c r="B157" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'msamina'. Head bench with 2 figures. 15 cm high. Marungu."</t>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'msamina'.
+Head bench with 2 figures.
+15 cm h.
+Marungu. "</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -37193,7 +37433,7 @@
           <t>Historischer Hauptkatalog:  "desgl. [Ohrpflock] aus Elefantenknochen. 3 cm dm. Iraku"</t>
         </is>
       </c>
-      <c r="B158" s="3" t="inlineStr">
+      <c r="B158" t="inlineStr">
         <is>
           <t>Historical main catalog: "The like [ear peg] from elephant bones. 3 cm dm. Iraq"</t>
         </is>
@@ -37208,7 +37448,7 @@
           <t>Historischer Hauptkatalog:  "desgl., gleichzeitig als Schnupftabakbüchse dienend." Das Zitat bezieht sich auf den Eintrag für III E 7562 = "´ndevule´ Ohrpflock aus Flaschenkürbis. Eine Seite mit blauen u. weißen Perlen verziert, auf der entgegengesetzten 4 runde Löcher, mit Kupfer- u. Messingblech gerandet. 4,8 cm Dm. 2,4 cm dick. Von Wasafua-Weibern getragen (wahrschnl. Wanyika-Arbeit). Vora am Songwe"</t>
         </is>
       </c>
-      <c r="B159" s="3" t="inlineStr">
+      <c r="B159" t="inlineStr">
         <is>
           <t>Historical main catalog: "The like, also serving as a snuff box." The quote refers to the entry for III E 7562 = "´ndevule´ ear plug made from bottle gourd. One side decorated with blue and white pearls, on the opposite 4 round holes, with copper and brass sheet edges. 4.8 cm diameter 2.4 cm thick. Worn by Wasafua women (probably Wanyika work). Especially on the Songwe "</t>
         </is>
@@ -37225,9 +37465,11 @@
 Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B160" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Ditto [= III C 27222: 'ifa iroke' horn-shaped knocker]; decorated with a carved kneeling woman. L. 36.5 cm. North Yoruba"</t>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Ditto [= III C 27222: 'ifa iroke' horn-shaped knocker];
+decorated with a carved kneeling woman. L. 36.5 cm.
+North Yoruba "</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -37243,9 +37485,12 @@
 aus Mkomaki.]"</t>
         </is>
       </c>
-      <c r="B161" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Headrest in the form of a praying mantis 49 cm long. Ebendaher [= Wangoni work from Mkomaki.]"</t>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Headrest in the form of a praying mantis
+49 cm lg.
+Therefore [= Wangoni work
+from Mkomaki.] "</t>
         </is>
       </c>
       <c r="D161" t="n">
@@ -37261,9 +37506,12 @@
 aus Mkomaki.]"</t>
         </is>
       </c>
-      <c r="B162" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Headrest [drawing / width] 20 cm Ebendaher [= Wangoni work from Mkomaki.]"</t>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Headrest
+[Drawing / width] 20 cm
+Therefore [= Wangoni work
+from Mkomaki.] "</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -37276,7 +37524,7 @@
           <t>Historischer hauptkatalog:  "ose schango" Tanzkeule, Stab mit einer Öse am unteren und 2 Donnerkeilen am oberen Ende. Der Faden, mit dem die Donnerkeile festgebunden dargestellt sind, wickelt sich um den Stab. H.: 54,2 cm. Nord Yoruba</t>
         </is>
       </c>
-      <c r="B163" s="3" t="inlineStr">
+      <c r="B163" t="inlineStr">
         <is>
           <t>Historical main catalog: "ose schango" dance club, stick with an eyelet at the bottom and 2 thunderbolts at the top. The thread with which the thunderbolts are tied is wrapped around the rod. H .: 54.2 cm. North Yoruba</t>
         </is>
@@ -37291,9 +37539,9 @@
           <t>Historischer Hauptkatalog:  "Tabaksbüchse (´mtwigo´) aus Holz, geschnitzt u.z.T. mit Stanniol überzogen [Maße] von einem Wanyamwesi-Fundi neu angefertigt."</t>
         </is>
       </c>
-      <c r="B164" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Tobacco rifle (´mtwigo´) made of wood, carved now with tin foil [dimensions] newly made by a Wanyamwesi fundi."</t>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Tobacco rifle (´mtwigo´) made of wood, carved and partly covered with tinfoil [dimensions] newly made by a Wanyamwesi fund."</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -37331,9 +37579,34 @@
 SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
-      <c r="B165" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Tobacco can with lid, made of wood. 10 cm high. Matschemba." Previous owner Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of what is now Tanzania Biographical fragments Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and has been from the Makonde plateau since the 1870s dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania. His residence was in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908. Appropriation context When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. Von Trotha reports: “Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched on the 6th from Sudi, where the companies were gathered partly by steamers, partly by foot, to Luagalla, the residence of Matschembas , from. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys a great reputation among his people and through several small features he showed that he has a more developed sense of decency than the native chiefs. ”(Deutsches Kolonialblatt 1896, p. 101) Trotha decided to stay in Luagalla only for a short time and so she marched 8. Company with Glauning with powder, ivory and guns back to the coast. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102). In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known. Sources Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag. Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest. Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On a visit to Machemba , Pp. 408-411. Deutsches Kolonialblatt 1897: On the situation in the hinterland of Lindi, p. 167. Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510. Bundesarchiv R 1001/287 Bundesarchiv R 1001/747 SMB -PK, EM, E 254/1896 SMB-PK, EM, E 1150/1896 SMB-PK, EM, E 1021/1896</t>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Tobacco can with lid, made of wood.
+10 cm high.
+Matschemba. "
+Previous owner
+Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of today's Tanzania
+Biographical fragments
+Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and had dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania from the Makonde plateau since the 1870s. His residence was among others in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908.
+Appropriation context
+When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. From Trotha reports:
+"Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched from Sudi on the 6th, where the companies were gathered, partly by steamboat, partly by foot, to Luagalla, the residence of Matschemba. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys great prestige among his people and, through several small traits, shows that he has a more developed sense of decency than the native chiefs otherwise. ”(Deutsches Kolonialblatt 1896, p. 101)
+Trotha decided to stay in Luagalla only for a short time and so the 8th company marched back to the coast with powder, ivory and guns under Glauning. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102).
+In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known.
+sources
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag.
+Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest.
+Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the Raids of the Chief Machemba.
+Deutsches Kolonialblatt 1896: About his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: About a visit to Machemba, pp. 408-411.
+Deutsches Kolonialblatt 1897: About the conditions in the hinterland by Lindi, p. 167.
+Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510.
+Federal archive R 1001/287
+Federal archive R 1001/747
+SMB-PK, EM, E 254/1896
+SMB-PK, EM, E 1150/1896
+SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -37349,9 +37622,12 @@
 (Luagalla, Residenz Matschembas)"</t>
         </is>
       </c>
-      <c r="B166" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Two small combs. B ge [...] t lt 1191/38 Wayao (Luagalla, residence Matschembas)"</t>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Two small combs.
+b ge [...] according to 1191/38
+Wayao
+(Luagalla, Residence Matschembas) "</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -37365,9 +37641,10 @@
 Farbe: hell- bis rotbraun</t>
         </is>
       </c>
-      <c r="B167" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "´ose schango´. North Yoruba. Dance club; red-colored, round staff, with carved line ornaments and an eyelet at the lower end. On the upper third of the staff four human faces, each with 2 opposite to each other; upper end, of which two continue horn-like upwards (thunderbolts). H .: 32.4 cm. " Color: light to reddish brown</t>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "´ose schango´. North Yoruba. Dance club; red-colored, round staff, with carved line ornaments and an eyelet at the lower end. On the upper third of the staff four human faces, each with 2 opposite to each other; upper end, of which two continue horn-like upwards (thunderbolts). H .: 32.4 cm. "
+Color: light to reddish brown</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -37380,7 +37657,7 @@
           <t>Historischer Hauptkatalog:  'kusson'. Ahnenkrug aus Ton; der Kopf stellt wahrscheinlich den Verstorbenen vor.</t>
         </is>
       </c>
-      <c r="B168" s="3" t="inlineStr">
+      <c r="B168" t="inlineStr">
         <is>
           <t>Historical main catalog: 'kusson'. Ancestral jug made of clay; the head probably represents the deceased.</t>
         </is>
@@ -37395,7 +37672,7 @@
           <t>Historischer Hauptkatalog:  Swago Figur anuf einem Stabförmigen Sockel stehende [...] Figut mit groben aber gut gearbeiteten Gesichtszügen, die Brüste mit beiden Händen tragend, auf dem Kopf zwei [...] tragend. Spuren von roter Bemalung, Höhe: 29,3 cm. Nord Yoruba</t>
         </is>
       </c>
-      <c r="B169" s="3" t="inlineStr">
+      <c r="B169" t="inlineStr">
         <is>
           <t>Historical main catalog: Swago figure standing on a rod-shaped base [...] with rough but well-worked facial features, carrying the breasts with both hands, [...] carrying two on the head. Traces of red painting, height: 29.3 cm. North Yoruba</t>
         </is>
@@ -37437,9 +37714,36 @@
 Interview mit Hakim Saleh geführt von Hanna Nieber im August 2015 in Vikokotoni/ Zanzibar Town.</t>
         </is>
       </c>
-      <c r="B170" s="3" t="inlineStr">
-        <is>
-          <t>Historic main catalog: "" upatu wa vita. "Warplate by" Sultan "Hassan bin Omari. Gong-like musical instrument made of brass with apparently senseless magic formulas in Arabic script. 33.5 cm in diameter. (Hassan b. O. called Makunganja, chief of a branch of Slave traders at Marudji, was hanged in Kilwa on November 26th, 1995.) "Previous owner Hassan bin Omari (Makunganya) (until 1905) Biographical fragments of Hassan bin Omari (Makunganya): Hassan bin Omari, also called Makunganya, was one of the most influential traders in Southeastern part of today's Tanzania. Its origin is said to go back to the Makanjila-Yao near Lake Nyassa, but he lived in Kilwa Kisiwani from an early age, was very well integrated into the Swahili Muslim coastal community and controlled the slave trade and caravan routes from Makanjila to to the coast. As early as 1888 he was said to have participated in the resistance against representatives of the German-East African society. Hassan bin Omari fought so successfully against the Germans' claim to power in parts of the southern coastal region that the latter had no control over the territory and the population outside the heavily fortified district of Kilwa, whose fort Makunganya was said to have attacked with several thousand soldiers in 1894. In 1895, four companies of the so-called Imperial Guard under the command of Lieutenant Colonel Lothar von Trotha advanced against Makunganya and his followers with the declared aim of "destroying" him. His residence was destroyed and his possessions, including correspondence, captured and Makunganya finally captured. In November 1895, he was brought to Kilwa by German troops (including the "collector" of Lieutnant Hans Glauning), where he was brought before a "military court", sentenced and hanged together with a group of supporters and officials. But not only his immediate surroundings, but also the people living in his sphere of influence were "punished" by burning entire villages. Today a memorial stone in Kilwa commemorates Makunganya, which was erected on the site of his execution in the post-colonial era. Appropriation context: Hans Glauning, who was then a lieutenant in the so-called Imperial Guard, faced Makunganya as an enemy and donated the captured "gong" to the Royal Museum of Ethnology in 1896. It was very likely that he conveyed the information to the Berlin ethnologists that it was an "upatu wa vita" (Kiswahili for "Gong of War"). So it was known that the object was related to the war. The extent to which Makunganya himself or other people on site still provided information about the property is not known, nor is the exact circumstances of Glauning's appropriation and encounter with Makunganya. The alleged "gong" could have been among the objects confiscated in the caves, taken from Makungaya during his arrest, or passed into the hands of Glauning during the transfer to Kilwa by the Eighth Company. The fact that Glauning identified the object as explicit property or possession of the Makunganya could also have served to underline the trophy character of this piece and thus its value - especially with regard to the presentation of the supposed "gong" in the First German Colonial Exhibition in 1896 in Berlin Treptow. However, it is certain that the property was captured during the war against Hassan bin Omari, its officials and supporters and the population - there is still no definitive evidence that it actually belonged to him. Object interpretations The function and meaning of the Makunganya object was unknown at the time, and a transcription and translation of the inscription was most likely not given due to the fact that it was based on "senseless magic formulas", and so it was also "forgotten for decades in the museum's depots" “- when the piece was entered in the museum database, the once famous“ Sultan ”was also no longer known, so that only“ East Africa ”was given as the origin. According to the Mwalimu Hakim Saleh from Zanzibar Town, the piece is a "talasimu" (Kiswahili: talisman), which was probably used to protect ("kinga") against all possible problems and also against ghosts ("majini") and probably could also be hung up. Similar plate-shaped objects made of a copper alloy ("shaba") could be used as a gong, but this specific one with writing could not. Rather, it can also be used as medicine (dawa), for example in the case of illness - the material itself is actually medicine; then it could be used for kombe - the "drinking" of Koranic verses by writing them with saffron and dissolving them in water - because the words written on them had the same healing effects as those written in saffron. It was only during a short research trip by Tanzanian scientists in September 2016 that local experts for Arabic manuscripts, Islamic literature and religion in Kilwa Kiwinje and Kilwa Masoko partially transcribed and translated the inscription on the plate-shaped object. These are sura 54 (al-Qamar, the moon), verses 45 and 46, which read as follows in German translation: (45) “(Yes) the great mass will be beaten and they will turn their backs (and flee). (46) The hour (of judgment) is the time that is set for them. And the hour (of judgment) is even more ominous and bitter (or: is extremely ominous and bitter). ”The historian Oswald Masebo relates these verses to Makunganya's struggle against the Germans. According to him, this is a key message from the Prophet Mohammed, which he used to inspire his followers in the early stages of the spread of the Islamic religion when faced with non-believers who refused to accept Islam. This verse was intended to give Muhammad's followers confidence that Muslims would be victorious in spreading their faith. Makunganya was a devout Muslim and may have used the teachings of Mohammed and the Koran in his struggle against the German colonial army to protect his sphere of interests and power. His opposition to the Germans, Masebo suspects, could be deeply rooted in the religion of Islam. Sources: Baumann, Oskar (1895): "To the board of the Association for Geography in Leipzig", December 17th, 1895, in: Announcements of the Association for Geography in Leipzig 1895, pp. 12–13. José AS Castcro (2007): Utenzi, War Poems, and the German conquest of East Africa. Trenton, New Jersey: African World Press. Gwassa, Gilbert CK (2005): The Outbreak and Development of the Majji-Maji-War 1905-1907. Cologne: Rüdiger Köppe publishing house. Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 66-149. Masebo, Oswald (2018): Objects of Resistance against German Colonialism in Southeast Tanzania. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 222-265. Rudi Paret (1966): The Koran. Stuttgart [ua]: Kohlhammer. Deutsches Kolonialblatt 1894: Fights at Kilwa, pp. 572–574. Deutsches Kolonialblatt 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On the course of the expedition against Hassan bin Omari. Deutsches Kolonialblatt 1896: About the situation in the south of the reserve. Federal Archives 1001/4812 Federal Archives 1001/287 Federal Archives 1001/747 SMB-PK, EM, I / MV 715, E 254/1896 Vita na Hassan bin Omari ("The struggle with Hassan bin Omar") by Mwalimu Mbaraka bin Shomari (communications from Seminars for Oriental Languages [MSOS] African Studies 1916, pp. 135–148) and Shairi la Makunganya ("The Makunganya Song") by Mwalimu Mzee bin Ali bin Kidogo bin Il-Qadiri, written after the victory over Hassan bin Omari (MSOS. African Studies 1898, pp. 86-114) Interview with Hakim Saleh conducted by Hanna Nieber in August 2015 in Vikokotoni / Zanzibar Town.</t>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Historic main catalog: "" upatu wa vita. "Warplate by" Sultan "Hassan bin Omari. Gong-like musical instrument made of brass with apparently senseless magic formulas in Arabic script. 33.5 cm in diameter. (Hassan b. O. called Makunganja, chief of a branch of Slave traders at Marudji, was hanged in Kilwa on November 26, 1995.) "
+Previous owner
+Hassan bin Omari (Makunganya) (until 1905)
+Biographical fragments of Hassan bin Omari (Makunganya):
+Hassan bin Omari, also called Makunganya, was one of the most influential traders in the southeast of today's Tanzania. Its origin is said to go back to the Makanjila-Yao near Lake Nyassa, but he lived in Kilwa Kisiwani from an early age, was very well integrated into the Swahili Muslim coastal community and controlled the slave trade and caravan routes from Makanjila to to the coast. As early as 1888 he was said to have participated in the resistance against representatives of the German-East African society. Hassan bin Omari fought so successfully against the Germans' claim to power in parts of the southern coastal region that the latter had no control over the territory and the population outside the heavily fortified district of Kilwa, whose fort Makunganya was said to have attacked with several thousand soldiers in 1894. In 1895, four companies of the so-called Imperial Guard under the command of Lieutenant Colonel Lothar von Trotha advanced against Makunganya and his followers with the declared aim of "destroying" him. His residence was destroyed and his possessions, including correspondence, captured and Makunganya finally captured. In November 1895, he was brought to Kilwa by German troops (including the "collector" of Lieutnant Hans Glauning), where he was brought before a "military court", sentenced and hanged together with a group of supporters and officials. But not only his immediate surroundings, but also the people living in his sphere of influence were "punished" by burning entire villages. Today a memorial stone in Kilwa commemorates Makunganya, which was erected on the site of his execution in the post-colonial era.
+Appropriation context:
+Hans Glauning, who was then lieutenant in the so-called Imperial Guard, faced Makunganya as an enemy and donated the captured "Gong" to the Royal Museum of Ethnology in 1896. It was very likely that he conveyed the information to the Berlin ethnologists that it was an "upatu wa vita" (Kiswahili for "Gong of War"). So it was known that the object was related to the war. The extent to which Makunganya himself or other people on site still provided information about the property is not known, as are the more specific circumstances of appropriation and Glauning's encounter with Makunganya. The alleged "gong" could have been among the objects confiscated in the caves, taken from Makungaya during his arrest, or passed into the hands of Glauning during the transfer to Kilwa by the Eighth Company. The fact that Glauning identified the object as explicit property or possession of the Makunganya could also have served to underline the trophy character of this piece and thus its value - especially with regard to the presentation of the supposed "gong" in the First German Colonial Exhibition in 1896 in Berlin Treptow. However, it is certain that the property was captured during the war against Hassan bin Omari, its officials and supporters and the population - there is still no definitive evidence that it actually belonged to him.
+Object interpretations
+The function and meaning of the Makunganya object was unknown at the time, and it was highly unlikely that a transcription and translation of the inscription would be initiated because it was based on “senseless magic formulas”, and so it had been “forgotten” in the museum's depots for decades. - when the piece was entered in the museum database, the once famous “Sultan” was also no longer known, so that only “East Africa” was given as the origin. According to the Mwalimu Hakim Saleh from Zanzibar Town, the piece is a "talasimu" (Kiswahili: talisman), which was probably used to protect ("kinga") against all possible problems and also against ghosts ("majini") and probably could also be hung up. Similar plate-shaped objects made of a copper alloy ("shaba") could be used as a gong, but this specific one with writing could not. Rather, it can also be used as medicine (dawa), for example in the case of illness - the material itself is actually medicine; then it could be used for kombe - the "drinking" of Koranic verses by writing them with saffron and dissolving them in water - because the words written on them had the same healing effects as those written in saffron. It was only during a short research trip by Tanzanian scientists in September 2016 that local experts for Arabic manuscripts, Islamic literature and religion in Kilwa Kiwinje and Kilwa Masoko partially transcribed and translated the inscription on the plate-shaped object. These are sura 54 (al-Qamar, the moon), verses 45 and 46, which read as follows in German translation: (45) “(Yes) the great mass will be beaten and they will turn their backs (and flee). (46) The hour (of judgment) is the time that is set for them. And the hour (of judgment) is even more ominous and bitter (or: is extremely ominous and bitter). ”The historian Oswald Masebo relates these verses to Makunganya's struggle against the Germans. According to him, this is a key message from the Prophet Mohammed, which he used to inspire his followers in the early stages of the spread of the Islamic religion when faced with non-believers who refused to accept Islam. This verse was intended to give Muhammad's followers confidence that Muslims would be victorious in spreading their faith. Makunganya was a devout Muslim and may have used the teachings of Mohammed and the Koran in his struggle against the German colonial army to protect his sphere of interests and power. His opposition to the Germans, Masebo suspects, could be deeply rooted in the religion of Islam.
+Sources:
+Baumann, Oskar (1895): "To the board of the Association for Geography in Leipzig", December 17, 1895, in: Announcements of the Association for Geography in Leipzig 1895, pp. 12–13.
+José A. S. Castcro (2007): Utenzi, War Poems, and the German conquest of East Africa. Trenton, New Jersey: African World Press.
+Gwassa, Gilbert C.K. (2005): The Outbreak and Development of the Majji-Maji-War 1905-1907. Cologne: Rüdiger Köppe publishing house.
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 66-149.
+Masebo, Oswald (2018): Objects of Resistance against German Colonialism in Southeast Tanzania. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 222-265.
+Rudi Paret (1966): The Koran. Stuttgart [u. a.]: Kohlhammer.
+Deutsches Kolonialblatt 1894: Fights at Kilwa, pp. 572–574.
+Deutsches Kolonialblatt 1895: On the raids of the chief Machemba.
+Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: On the course of the expedition against Hassan bin Omari.
+Deutsches Kolonialblatt 1896: About the situation in the south of the reserve.
+Federal Archives 1001/4812
+Federal Archives 1001/287
+Federal Archives 1001/747
+SMB-PK, EM, I / MV 715, E 254/1896
+Vita na Hassan bin Omari ("The Struggle with Hassan bin Omar") by Mwalimu Mbaraka bin Shomari (Messages from the Seminar for Oriental Languages [MSOS]. African Studies 1916, pp. 135–148) and Shairi la Makunganya ("The Makunganya- Song “) by Mwalimu Mzee bin Ali bin Kidogo bin Il-Qadiri, written after the victory over Hassan bin Omari (MSOS. African Studies 1898, pp. 86-114)
+Interview with Hakim Saleh conducted by Hanna Nieber in August 2015 in Vikokotoni / Zanzibar Town.</t>
         </is>
       </c>
       <c r="D170" t="n">
@@ -37455,9 +37759,12 @@
 Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B171" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'ifa iroke' Horn-shaped knocker made of ivory; decorated with notch carving and line patterns. L .: 27 cm. North Yoruba"</t>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Historic main catalog: "'ifa iroke'
+Horn-shaped ivory knocker; decorated with notch carving and line patterns.
+L .: 27 cm.
+North Yoruba "</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -37473,9 +37780,12 @@
 Mittel-Pare)."</t>
         </is>
       </c>
-      <c r="B172" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'itele.' Ear wire made of copper wire; the end turns are wrapped with brass wire. Work by Wapare - Fundis. 4.5 cm lg. Ibaia (Madji ya ju) middle pare). "</t>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'itele.' Ear wire made of copper wire, the end turns are wrapped with brass wire, work by Wapare - Fundis.
+4.5 cm lg.
+Ibaia (Madji ya ju)
+Middle Pare). "</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -37491,9 +37801,12 @@
 Mittel-Pare).]"</t>
         </is>
       </c>
-      <c r="B173" s="3" t="inlineStr">
-        <is>
-          <t>Historic main catalog: "'kidisa'. Brass neck ring of women. Decorated. 17.5 cm in diameter. Ebendaher. [= Ibaia (Madji ya ju) middle pare).]"</t>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'kidisa'. Brass neck ring of women. Decorated.
+17.5 cm diam.
+Therefore. [= Ibaia (Madji ya ju)
+Middle Pare).] "</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -37508,9 +37821,11 @@
 Tanga, Süd-Pare."</t>
         </is>
       </c>
-      <c r="B174" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'kitschumbi'. Wooden chair, with 4 feet. 21 cm high, 29 cm diameter of seat. Tanga, south pare."</t>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'kitschumbi'. Wooden chair, with 4 feet.
+21 cm h., 29 cm dia. d. Seat.
+Tanga, south pare. "</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -37525,9 +37840,11 @@
 Ebendaher [= Wawemba (Muliro])]"</t>
         </is>
       </c>
-      <c r="B175" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'mutute'. Hookah. Bottle gourd with clay head. 43 cm lg. Ebendaher [= Wawemba (Muliro])]"</t>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'mutute'. Hookah. Bottle gourd with clay head.
+43 cm lg.
+Therefore [= Wawemba (Muliro])] "</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -37543,9 +37860,12 @@
 (Mutindi am Malinga-Berg)."</t>
         </is>
       </c>
-      <c r="B176" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "'nondo'. Hammer of a fundi. 28 cm lg. Unyamwanga (Mutindi on Malinga mountain)."</t>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "'nondo'. Hammer of a fund.
+28 cm lg.
+Unyamwanga
+(Mutindi on Malinga mountain). "</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -37558,7 +37878,7 @@
           <t>Historischer Hauptkatalog: ""itenga" Ohrpflock aus Holz, mit 5 Messingnägeln verziert. Von Weibern getragen. 3,8 cm Dm. 1,2 cm dick. Kirurumo (Uvanda)."</t>
         </is>
       </c>
-      <c r="B177" s="3" t="inlineStr">
+      <c r="B177" t="inlineStr">
         <is>
           <t>Historical main catalog: "" itenga "ear peg made of wood, decorated with 5 brass nails. Worn by women. 3.8 cm diameter 1.2 cm thick. Kirurumo (Uvanda)."</t>
         </is>
@@ -37573,7 +37893,7 @@
           <t>Historischer Hauptkatalog: ""matenga" 4 Ohrpflöcke aus Holz, von Weibern gearbeitet und getragen. [Maße] Ramsamba am Momba-Fl. (Uvanda)"</t>
         </is>
       </c>
-      <c r="B178" s="3" t="inlineStr">
+      <c r="B178" t="inlineStr">
         <is>
           <t>Historical main catalog: "" matenga "4 ear pegs made of wood, worked and worn by women. [Dimensions] Ramsamba on Momba-Fl. (Uvanda)"</t>
         </is>
@@ -37588,7 +37908,7 @@
           <t>Historischer Hauptkatalog: ""tegre". Schnupftabaksbüchse aus Bambus-, mit Eisen-u. Messingdraht umwickelt. Boden und Deckel aus Kürbis. Der Bambus stammt aus Konde-Land. Arbeit der Jumben von Gasisi. 5 cm h. Gasisi am Momba ( Mkurue)."</t>
         </is>
       </c>
-      <c r="B179" s="3" t="inlineStr">
+      <c r="B179" t="inlineStr">
         <is>
           <t>Historical main catalog: "" tegre ". Snuff box made of bamboo, wrapped with iron and brass wire. Bottom and lid made of pumpkin. The bamboo comes from Konde-Land. Work of the Jumben von Gasisi. 5 cm h. Gasisi am Momba (Mkurue ). "</t>
         </is>
@@ -37606,9 +37926,12 @@
 Iraku."</t>
         </is>
       </c>
-      <c r="B180" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "2 of the same [= III C 8582: wooden ear peg] made of shell but shell [...] (with fiber [?] Wrapping) a) 3.7 cm dm. B) 3.8 cm dm. Iraq. "</t>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "2 of the same [= III C 8582: ear peg made of wood] made of shell but shell [...] (with fiber [?] Wrapping)
+a) 3.7 cm dm.
+b) 3.8 cm dm.
+Iraqu. "</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -37624,9 +37947,12 @@
 (Schabrumaleute.)"</t>
         </is>
       </c>
-      <c r="B181" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "2 combs. 12 cm long Magwangwara des Mkomakiro (Schabruma people.)"</t>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "2 combs.
+12 cm lg.
+Magwangwara of Mkomakiro
+(Schabruma people.) "</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -37639,7 +37965,7 @@
           <t>Historischer Hauptkatalog: "2 Ohrpflöcke aus Holz, einer mit Eisenblech - Verzierung. Von den Wabungu - Weibern getragen. 6,6 cm Dm. Ebendaher [Bungu am Rukwa-See]"</t>
         </is>
       </c>
-      <c r="B182" s="3" t="inlineStr">
+      <c r="B182" t="inlineStr">
         <is>
           <t>Historical main catalog: "2 ear pegs made of wood, one with iron sheet ornament. Wabungu women wear it. 6.6 cm diameter. Ebendaher [Bungu on Lake Rukwa]"</t>
         </is>
@@ -37678,9 +38004,33 @@
 Vita na Hassan bin Omari („Der Kampf mit Hassan bin Omar“) von Mwalimu Mbaraka bin Shomari (Mitteilungen des Seminars für Orientalische Sprachen [MSOS]. Afrikanische Studien 1916, S. 135–148) und Shairi la Makunganya („Das Makunganya-Lied“) von Mwalimu Mzee bin Ali bin Kidogo bin Il-Qadiri, verfasst nach dem Sieg über Hassan bin Omari (MSOS. Afrikanische Studien 1898, S. 86–114)</t>
         </is>
       </c>
-      <c r="B183" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "8 bullets made of iron. Mavudji. (Hassan bin Omari)" Pre-owned Hassan bin Omari (Makunganya) (until 1905) Biographical fragments of Hassan bin Omari (Makunganya) Hassan bin Omari, also called Makunganya, was one of the most influential traders in the southeast of today's Tanzania. Its origin is said to go back to the Makanjila-Yao near Lake Nyassa, but he lived in Kilwa Kisiwani from an early age, was very well integrated into the Swahili Muslim coastal community and controlled the slave trade and caravan routes from Makanjila to to the coast. As early as 1888 he was said to have participated in the resistance against representatives of the German-East African society. Hassan bin Omari fought so successfully against the Germans' claim to power in parts of the southern coastal region that the latter had no control over the territory and the population outside the heavily fortified district of Kilwa, whose fort Makunganya was said to have attacked with several thousand soldiers in 1894. In 1895, four companies of the so-called Imperial Guard under the command of Lieutenant Colonel Lothar von Trotha advanced against Makunganya and his followers with the declared aim of "destroying" him. His residence was destroyed and his possessions, including correspondence, captured and Makunganya finally captured. In November 1895, he was brought to Kilwa by German troops (including the "collector" of Lieutnant Hans Glauning), where he was brought before a "military court", sentenced and hanged together with a group of supporters and officials. But not only his immediate surroundings, but the people living in his sphere of influence were "punished" by burning entire villages. Today a memorial stone in Kilwa commemorates Makunganya, which was erected on the site of his execution in the post-colonial era. Appropriation context Hans Glauning, who was a lieutenant in the so-called Imperial Protection Force for German East Africa at the time of the war against Hassan bin Omari and who also "collected" eagerly for the Berlin Museum of Ethnology in the following years, faced Makunganya as an enemy and gave the projectiles in 1896 the Royal Museum of Ethnology. The exact circumstances of Glauning's appropriation and encounter with Makunganya are not known. The projectiles could have been among the objects confiscated in the caves, Makungaya had been removed during his arrest, or had fallen into the hands of Glauning during the transfer to Kilwa by the Eighth Company. The fact that Glauning identified the projectiles as the explicit property of the Makunganya could also have served to underline the trophy character of these pieces and thus their value. However, it is certain that the projectiles were captured during the war against Hassan bin Omari, his officials and supporters and the population - there is still no definitive evidence that it actually belonged to him. Sources Baumann, Oskar (1895): "To the board of the Association for Geography in Leipzig", December 17, 1895, in: Announcements of the Association for Geography in Leipzig 1895, pp. 12–13. José AS Castcro (2007): Utenzi, War Poems, and the German conquest of East Africa. Trenton, New Jersey: African World Press. Gwassa, Gilbert CK (2005): The Outbreak and Development of the Majji-Maji-War 1905-1907. Cologne: Rüdiger Köppe publishing house. Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 66-149. Masebo, Oswald (2018): Objects of Resistance against German Colonialism in Southeast Tanzania. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 222-265. Rudi Paret (1966): The Koran. Stuttgart [ua]: Kohlhammer. Deutsches Kolonialblatt 1894: Fights at Kilwa, pp. 572–574. Deutsches Kolonialblatt 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On the course of the expedition against Hassan bin Omari. Deutsches Kolonialblatt 1896: About the situation in the south of the reserve. Federal Archives 1001/4812 Federal Archives 1001/287 Federal Archives 1001/747 SMB-PK, EM, I / MV 715, E 254/1896 Vita na Hassan bin Omari ("The struggle with Hassan bin Omar") by Mwalimu Mbaraka bin Shomari (communications from Seminars for Oriental Languages [MSOS] African Studies 1916, pp. 135–148) and Shairi la Makunganya ("The Makunganya Song") by Mwalimu Mzee bin Ali bin Kidogo bin Il-Qadiri, written after the victory over Hassan bin Omari (MSOS. African Studies 1898, pp. 86-114)</t>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Historic main catalog: "8 [later noted] bullets made of iron. Mavudji. (Hassan bin Omari)"
+Pre-owned
+Hassan bin Omari (Makunganya) (until 1905)
+Biographical Fragments of Hassan bin Omari (Makunganya)
+Hassan bin Omari, also called Makunganya, was one of the most influential traders in the southeast of today's Tanzania. Its origin is said to go back to the Makanjila-Yao near Lake Nyassa, but he lived in Kilwa Kisiwani from an early age, was very well integrated into the Swahili Muslim coastal community and controlled the slave trade and caravan routes from Makanjila to to the coast. As early as 1888 he was said to have participated in the resistance against representatives of the German-East African society. Hassan bin Omari fought so successfully against the Germans' claim to power in parts of the southern coastal region that the latter had no control over the territory and the population outside the heavily fortified district of Kilwa, whose fort Makunganya was said to have attacked with several thousand soldiers in 1894. In 1895, four companies of the so-called Imperial Guard under the command of Lieutenant Colonel Lothar von Trotha advanced against Makunganya and his followers with the declared aim of "destroying" him. His residence was destroyed and his possessions, including correspondence, captured and Makunganya finally captured. In November 1895, he was brought to Kilwa by German troops (including the "collector" of Lieutnant Hans Glauning), where he was brought before a "military court", sentenced and hanged together with a group of supporters and officials. But not only his immediate surroundings, but the people living in his sphere of influence were "punished" by burning entire villages. Today a memorial stone in Kilwa commemorates Makunganya, which was erected on the site of his execution in the post-colonial era.
+Appropriation context
+Hans Glauning, who was a lieutenant in the so-called Imperial Protection Force for German East Africa at the time of the war against Hassan bin Omari and also "collected" eagerly for the Berlin Museum of Ethnology in the following years, faced Makunganya as an enemy and gave the bullets in the year 1896 the Royal Museum of Ethnology. The exact circumstances of Glauning's appropriation and encounter with Makunganya are not known. The projectiles might have been among the objects confiscated in the caves, taken from Makungaya during his arrest, or passed into the hands of Glauning during his transfer to Kilwa by the Eighth Company. The fact that Glauning identified the projectiles as the explicit property of the Makunganya could also have served to underline the trophy character of these pieces and thus their value. However, it is certain that the projectiles were captured during the war against Hassan bin Omari, his officials and supporters and the population - there is still no definitive evidence that it actually belonged to him.
+sources
+Baumann, Oskar (1895): "To the board of the Association for Geography in Leipzig", December 17, 1895, in: Announcements of the Association for Geography in Leipzig 1895, pp. 12–13.
+José A. S. Castcro (2007): Utenzi, War Poems, and the German conquest of East Africa. Trenton, New Jersey: African World Press.
+Gwassa, Gilbert C.K. (2005): The Outbreak and Development of the Majji-Maji-War 1905-1907. Cologne: Rüdiger Köppe publishing house.
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 66-149.
+Masebo, Oswald (2018): Objects of Resistance against German Colonialism in Southeast Tanzania. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin, Reimer, pp. 222-265.
+Rudi Paret (1966): The Koran. Stuttgart [u. a.]: Kohlhammer.
+Deutsches Kolonialblatt 1894: Fights at Kilwa, pp. 572–574.
+Deutsches Kolonialblatt 1895: On the raids of the chief Machemba.
+Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: On the course of the expedition against Hassan bin Omari.
+Deutsches Kolonialblatt 1896: About the situation in the south of the reserve.
+Federal Archives 1001/4812
+Federal Archives 1001/287
+Federal Archives 1001/747
+SMB-PK, EM, I / MV 715, E 254/1896
+Vita na Hassan bin Omari ("The Struggle with Hassan bin Omar") by Mwalimu Mbaraka bin Shomari (Messages from the Seminar for Oriental Languages [MSOS]. African Studies 1916, pp. 135–148) and Shairi la Makunganya ("The Makunganya- Song “) by Mwalimu Mzee bin Ali bin Kidogo bin Il-Qadiri, written after the victory over Hassan bin Omari (MSOS. African Studies 1898, pp. 86-114)</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -37696,9 +38046,12 @@
 Sswahili Küste"</t>
         </is>
       </c>
-      <c r="B184" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Anchor stone made of coral, from a Ghalawa boat (double boom) for a description of such a boat, see articles on ethnology, p.61 dia. 17 cm height 11.5 cm Sswahili coast"</t>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Anchor stone made of coral, from a Ghalawa boat (double boom). For a description of such a boat, see articles on ethnology, p.61
+Dm. 17 cm
+Height 11.5 cm
+Sswahili coast "</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -37713,9 +38066,11 @@
 Wagogo."</t>
         </is>
       </c>
-      <c r="B185" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Copper arm ring. Work of Fundi Kipanga from Misuri (Nyamba); worn by Sultan Sabugo by Nyamba: 6.7 cm diameter. Wagogo."</t>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Main historical catalog: "Copper arm ring. Work of Fundi Kipanga from Misuri (Nyamba); worn by Sultan Sabugo v. Nyamba
+6.7 cm diameter
+Wagogo. "</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -37728,7 +38083,7 @@
           <t>Historischer Hauptkatalog: "Armring, Elfenbein. [Maße] Sukuma Gogo?"</t>
         </is>
       </c>
-      <c r="B186" s="3" t="inlineStr">
+      <c r="B186" t="inlineStr">
         <is>
           <t>Historical main catalog: "Armring, ivory. [Dimensions] Sukuma Gogo?"</t>
         </is>
@@ -37743,7 +38098,7 @@
           <t>Historischer Hauptkatalog: "Armschmuck, Eisenspirale. Die oberste Windung ist mit Messingdraht umwunden. H.22 D.10,5 cm, Masai"</t>
         </is>
       </c>
-      <c r="B187" s="3" t="inlineStr">
+      <c r="B187" t="inlineStr">
         <is>
           <t>Historical main catalog: "Bracelets, iron spiral. The top turn is wound with brass wire. H.22 D.10.5 cm, Masai"</t>
         </is>
@@ -37758,7 +38113,7 @@
           <t>Historischer Hauptkatalog: "Armspange aus Horn. Enden mit Kupferdraht umwickelt, zeigen nach oben. Wagogo (aus Nsuguni)"</t>
         </is>
       </c>
-      <c r="B188" s="3" t="inlineStr">
+      <c r="B188" t="inlineStr">
         <is>
           <t>Historical main catalog: "Horn bangle. Wrapped ends with copper wire, point upwards. Wagogo (from Nsuguni)"</t>
         </is>
@@ -37796,9 +38151,32 @@
 SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
-      <c r="B189" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Bow made of red-brown wood, drilled at both ends for fastening the tendon; this made of leather. At one end of the bow a short brass spiral. Height of the bow 1.20m. Matschemba." Previous owner Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of what is now Tanzania Biographical fragments Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and has been from the Makonde plateau since the 1870s dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania. His residence was in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908. Appropriation context When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. Von Trotha reports: “Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched on the 6th from Sudi, where the companies were gathered partly by steamers, partly by foot, to Luagalla, the residence of Matschembas , from. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys a great reputation among his people and through several small features he showed that he has a more developed sense of decency than the native chiefs. ”(Deutsches Kolonialblatt 1896, p. 101) Trotha decided to stay in Luagalla only for a short time and so she marched 8. Company with Glauning with powder, ivory and guns back to the coast. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102). In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known. Sources Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag. Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest. Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On a visit to Machemba , Pp. 408-411. Deutsches Kolonialblatt 1897: On the situation in the hinterland of Lindi, p. 167. Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510. Bundesarchiv R 1001/287 Bundesarchiv R 1001/747 SMB -PK, EM, E 254/1896 SMB-PK, EM, E 1150/1896 SMB-PK, EM, E 1021/1896</t>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Bow made of red-brown wood, drilled at both ends for fastening the tendon; this made of leather. At one end of the bow a short brass spiral. Height of the bow 1.20m. Matschemba."
+Previous owner
+Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of today's Tanzania
+Biographical fragments
+Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and had dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania from the Makonde plateau since the 1870s. His residence was among others in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908.
+Appropriation context
+When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. From Trotha reports:
+"Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched from Sudi on the 6th, where the companies were gathered, partly by steamboat, partly by foot, to Luagalla, the residence of Matschemba. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys great prestige among his people and, through several small traits, shows that he has a more developed sense of decency than the native chiefs otherwise. ”(Deutsches Kolonialblatt 1896, p. 101)
+Trotha decided to stay in Luagalla only for a short time and so the 8th company marched back to the coast with powder, ivory and guns under Glauning. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102).
+In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known.
+sources
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag.
+Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest.
+Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the Raids of the Chief Machemba.
+Deutsches Kolonialblatt 1896: About his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: About a visit to Machemba, pp. 408-411.
+Deutsches Kolonialblatt 1897: About the conditions in the hinterland by Lindi, p. 167.
+Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510.
+Federal archive R 1001/287
+Federal archive R 1001/747
+SMB-PK, EM, E 254/1896
+SMB-PK, EM, E 1150/1896
+SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -37811,7 +38189,7 @@
           <t>Historischer Hauptkatalog: "Cylindrische Büchse, Holz. Deckel und Boden mit Kupferdrahtspiralen und Perlen bekleidet Vergl. IIIE10871-74 Masai"</t>
         </is>
       </c>
-      <c r="B190" s="3" t="inlineStr">
+      <c r="B190" t="inlineStr">
         <is>
           <t>Historical main catalog: "Cylindrical rifle, wood. Lid and base clad with copper wire spirals and pearls cf. IIIE10871-74 Masai"</t>
         </is>
@@ -37829,9 +38207,12 @@
 (erworben in Muliro, Tawa)."</t>
         </is>
       </c>
-      <c r="B191" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "The same. [= III C 7994 a, b: Knife with sheath] Sheath and handle carved from wood. A cartridge case is attached to the handle and to the lower end of the sheath. Knife 28 cm long (blade 18, 5 cm), sheath 23 cm. Made in Marungu (acquired in Muliro, Tawa). "</t>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "The same. [= III C 7994 a, b: Knife with sheath] Sheath and handle carved from wood. A cartridge case is attached to the handle and to the lower end of the sheath.
+Knife 28 cm lg. (Blade 18.5 cm), scabbard 23 cm.
+Made in Marungu
+(acquired in Muliro, Tawa). "</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -37844,7 +38225,7 @@
           <t>Historischer Hauptkatalog: "Desgl. [Kopfschmuck, von Männern beim Tanzen getragen. Lederriemen mit Messing- und Kupferplättchen besetzt] Wanyaturu."</t>
         </is>
       </c>
-      <c r="B192" s="3" t="inlineStr">
+      <c r="B192" t="inlineStr">
         <is>
           <t>Historical main catalog: "Desgl. [Headdress, worn by men while dancing. Leather straps with brass and copper plates] Wanyaturu."</t>
         </is>
@@ -37859,9 +38240,9 @@
           <t>Historischer Hauptkatalog: "Desgl. [Kuhglocke aus Eisen "ngorgor". Mit Ledergehänge. Glocke v.s. Wahehe erbeutet. Wahumba]."</t>
         </is>
       </c>
-      <c r="B193" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Desgl. [Cow bell made of iron" ngorgor ". With leather hangings. Bell vs. captured woe. Wahumba]."</t>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Desgl. [Iron cow bell" ngorgor ". With leather hangings. Bell v.s. Wahehe captured. Wahumba]."</t>
         </is>
       </c>
       <c r="D193" t="n">
@@ -37877,9 +38258,12 @@
 Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B194" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Ditto [= III C 27217: 'ifa iroke'] knocker made of wood, in the form of an ivory horn with notched carving ornaments. L .: 37.5 cm. North Yoruba"</t>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Ditto [= III C 27217: 'ifa iroke']
+Knocker made of wood, in the form of an ivory horn with carved ornaments.
+L .: 37.5 cm.
+North Yoruba "</t>
         </is>
       </c>
       <c r="D194" t="n">
@@ -37892,7 +38276,7 @@
           <t>Historischer Hauptkatalog: "dito [= III C 29319: 'kusson' Ahnenkrug aus Ton]</t>
         </is>
       </c>
-      <c r="B195" s="3" t="inlineStr">
+      <c r="B195" t="inlineStr">
         <is>
           <t>Historical main catalog: "Ditto [= III C 29319: 'kusson' ancestral jug made of clay]</t>
         </is>
@@ -37911,9 +38295,13 @@
 Tansania [nachträgl. hinzugefügt]"</t>
         </is>
       </c>
-      <c r="B196" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Large carved chair with 3 feet. 36 cm high, diameter of the round seat 40 cm. Ukimbu. Kimbu [added later] Tanzania [added later]"</t>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Large carved chair with 3 feet.
+36 cm h., Diam. the round seat 40 cm.
+Ukimbu.
+Kimbu [ex post added]
+Tanzania [ex. added] "</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -37944,9 +38332,27 @@
 SMB-PK, EM, I/MV 956</t>
         </is>
       </c>
-      <c r="B197" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Necklace made of 4 cone covers. (Kobe). Like pieces 4117-19 by Manamahome, the brother of Mhenge Sakkamanga Mahenge - Mafiti." Previous owner Mwanamhomi, 'sub-chief' of the Bena (1897 to 1906/1907), Kilombero Valley, today southwestern Tanzania Biographical fragments Mwanamhomi was one of twenty sons of the 'mtema' Mtengera, who was 'chief' of the Bena in 1884 Kilombero Valley was where they lived since fighting with the hehe in the 1870s. After Mtengera's death, Kiwanga became his successor in 1884 and remained 'mtema' until his death in the Maji Maji war in 1905. His younger brother Sagamaganga did not accept the establishment of Kiwanga and allied himself with the Ngoni 'chief' Chabruma. The warfare ended when the Germans entered the region at the beginning of the 1890s. Although Sagamaganga was officially subordinate to Kiwanga, it effectively governed the southern regions of the Bena region (the Germans called it "Ubena"). Mwanamhomi was probably more connected to Sagamaganga than to Kiwanga. So he took over from Sagamaganga after his suicide in 1897. The elders of the Bena said that Kiwanga had appointed Mwanamhomi, but this should possibly hide Sagamaganga's actual independence. Mwanamhomi collaborated with the Germans during the Maji Maji War, which in turn points to the still great influence of Kiwanga, who had been a close ally of the German colonizers since 1890 and the Germans in their wars against Mkwawa and the Hehe in the 1890s Years had supported. Mwanamhomi presumably ruled until 1906 and 1907. Conspiracy context Hans Glauning, who had been stationed in Kilwa as the company leader (8th company) of the so-called Imperial Guard for German East Africa since 1895, undertook an "expedition" to Barikiwa, a German military post, in May 1895 to secure the rubber trade in the southeast of today's Tanzania. In addition to two other German military personnel, it included twelve African soldiers (so-called 'askari'), 55 porters, the women who accompanied them and so-called 'boys'. His duties included replacing the head of the post and sick 'askari' as well as route recordings, but above all it was about ordering Mhomakiro, the brother of the influential 'chief' of the Ngoni named Chabruma, to peace negotiations in Kilwa. From Barikiwa, Glauning undertook small trips to the surrounding area, on which he also acquired so-called ethnographic objects. He was in contact with Felix von Luschan, Assistant Director at the Royal Museum of Ethnology in Berlin, and also informed him about this militarized expedition as a welcome opportunity to "collect". Glauning also downplayed campaigns dubbed "punitive expeditions" as a welcome opportunity. According to sources, there were no violent clashes on this venture. About the acquisition context of the "neck cord" (together with three other objects III E 4117, III E 4118, III E 4119) can only be read in Glauning's list of objects in the acquisition files: "From the brother of Mhenge Sakkamanga [Sagamaganga] Manamahome [Mwanamhomi] who returned from the coast by an ivory transport. ”(SMB-PK, EM, I / MV 071, E 1239/1895) Sources Culwick, AT u. Culwick, GM (1935): Ubena of the Rivers. London: George Allen &amp; Unwin Ltd. Gulliver, PH (1974), "Political Evolution in the Songea Ngoni Chiefdoms, 1850-1905," in: Bulletin of the School of Oriental and African Studies 37 (1), pp. 93-94. Iliffe, John (1979): A modern History of Tanganyika. Cambridge: Cambridge University Press. Prince, Magdalena von (1908): A woman in the interior of German East Africa. Berlin: Ernst Friedrich Mittler and son. Monson, Jamie (2000): "Memory, Migration, and the Authority of History in Southern Tanzania, 1860-1960," in: Journal of African History 41, pp. 347-372. Federal Archives R 1001/287 SMB-PK, EM, I / MV 071, E 1239/1895 SMB-PK, EM, I / MV 956</t>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Necklace made of 4 cone covers. (Kobe). Like pieces 4117-19 by Manamahome, the brother of Mhenge Sakkamanga
+Mahenge - Mafiti. "
+Previous owner
+Mwanamhomi, 'sub-chief' of the Bena (1897 to 1906/1907), Kilombero Valley, today southwestern Tanzania
+Biographical fragments
+Mwanamhomi was one of twenty sons of the 'mtema' Mtengera, who until 1884 was the 'chief' of the Bena in the Kilombero Valley, where they had lived since fighting with the hehe in the 1870s. After Mtengera's death, Kiwanga became his successor in 1884 and remained 'mtema' until his death in the Maji Maji War in 1905. His younger brother Sagamaganga did not accept the establishment of Kiwanga and allied himself with the Ngoni 'chief' Chabruma. The warfare ended when the Germans entered the region at the beginning of the 1890s. Although Sagamaganga was officially subordinate to Kiwanga, it effectively governed the southern regions of the Bena region (the Germans called it "Ubena"). Mwanamhomi was probably more connected to Sagamaganga than to Kiwanga. So he took over from Sagamaganga after his suicide in 1897. The elders of the Bena said that Kiwanga had appointed Mwanamhomi, but this should possibly hide Sagamaganga's actual independence. Mwanamhomi collaborated with the Germans during the Maji Maji War, which in turn points to the still great influence of Kiwanga, who had been a close ally of the German colonizers since 1890 and the Germans in their wars against Mkwawa and the Hehe in the 1890s Years had supported. Mwanamhomi presumably ruled until 1906 and 1907.
+Dislike context
+Hans Glauning, who had been the company leader (8th company) of the so-called Imperial Guard for German East Africa in Kilwa since 1895, undertook an "expedition" to Barikiwa, a German military post to secure the rubber trade in southeastern Tanzania in May 1895. In addition to two other German military personnel, it included twelve African soldiers (so-called 'askari'), 55 porters who accompanied them and so-called 'boys'. His duties included the replacement of the head of the post and sick 'askari' as well as route recordings, but above all it was about ordering Mhomakiro, the brother of the influential 'chief' of the Ngoni named Chabruma, to peace negotiations in Kilwa. From Barikiwa, Glauning undertook small trips to the surrounding area, on which he also acquired so-called ethnographic objects. He was in contact with Felix von Luschan, Assistant Director at the Royal Museum of Ethnology in Berlin, and also informed him about this militarized expedition as a welcome opportunity to "collect". Glauning also downplayed campaigns dubbed "punitive expeditions" as a welcome opportunity. According to sources, there were no violent clashes on this venture.
+In Glauning's list of objects in the acquisition files you can only read about the context of acquisition of the "neck cord" (together with three other objects III E 4117, III E 4118, III E 4119):
+"Acquired from the brother of Mhenge Sakkamanga [Sagamaganga] Manamahome [Mwanamhomi] who returned from the coast by an ivory transport." (SMB-PK, EM, I / MV 071, E 1239/1895)
+sources
+Culwick, A.T. u. Culwick, G.M. (1935): Ubena of the Rivers. London: George Allen &amp; Unwin Ltd.
+Gulliver, P.H. (1974), "Political Evolution in the Songea Ngoni Chiefdoms, 1850-1905," in: Bulletin of the School of Oriental and African Studies 37 (1), pp. 93-94.
+Iliffe, John (1979): A modern History of Tanganyika. Cambridge: Cambridge University Press.
+Prince, Magdalena von (1908): A woman in the interior of German East Africa. Berlin: Ernst Friedrich Mittler and son.
+Monson, Jamie (2000): "Memory, Migration, and the Authority of History in Southern Tanzania, 1860-1960," in: Journal of African History 41, pp. 347-372.
+Federal archive R 1001/287
+SMB-PK, EM, I / MV 071, E 1239/1895
+SMB-PK, EM, I / MV 956</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -37961,9 +38367,11 @@
 Erwerbung: s. III E 19903"</t>
         </is>
       </c>
-      <c r="B198" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Wooden figure: 'Goddess Tara' (Tibet) H. 25.7 cm, Makonde acquisition: see III E 19903"</t>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Wooden figure: 'Goddess Tara' (Tibet)
+H. 25.7 cm, Makonde
+Acquisition: s. III E 19903 "</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -37977,9 +38385,10 @@
 Erwerbung: s. III E 19903"</t>
         </is>
       </c>
-      <c r="B199" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Wooden figure: Maria, holding the dead Jesus in her arms. H. 27.5 cm, Makonde Acquisition: see III E 19903"</t>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Wooden figure: Maria, holding the dead Jesus in her arms. H. 27.5 cm, Makonde
+Acquisition: s. III E 19903 "</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -37994,9 +38403,11 @@
 Erwerbung: s. III E 19903"</t>
         </is>
       </c>
-      <c r="B200" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Wooden figure: replica of a sprite bottle H. 24.7 cm, Makonde acquisition: see III E 19903"</t>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Wooden figure: replica of a sprite bottle
+H. 24.7 cm, Makonde
+Acquisition: s. III E 19903 "</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -38009,7 +38420,7 @@
           <t>Historischer Hauptkatalog: "Kamm aus Elfenbein. 12 cm lg. Ebendaher [Wawemba] (Muliro)."</t>
         </is>
       </c>
-      <c r="B201" s="3" t="inlineStr">
+      <c r="B201" t="inlineStr">
         <is>
           <t>Historical main catalog: "Ivory comb. 12 cm long. Ebendaher [Wawemba] (Muliro)."</t>
         </is>
@@ -38024,7 +38435,7 @@
           <t>Historischer Hauptkatalog: "Kamm aus Holz. Wawemba (Muliro u. Kakoma)"</t>
         </is>
       </c>
-      <c r="B202" s="3" t="inlineStr">
+      <c r="B202" t="inlineStr">
         <is>
           <t>Historical main catalog: "Wooden comb. Wawemba (Muliro and Kakoma)"</t>
         </is>
@@ -38040,9 +38451,10 @@
 Uhehe"</t>
         </is>
       </c>
-      <c r="B203" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Small chain made of brass beads; weaving. In the past, such chains made of copper were often wrapped around the ankles as a sign of the sultan's dignity. 24 cm long [sketch] Uhehe"</t>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Small chain made of brass beads; weaving. In the past, such chains made of copper were often wrapped around the ankles as a sign of the sultan's dignity. 24 cm long. [Sketch]
+Uhehe "</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -38080,9 +38492,34 @@
 SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
-      <c r="B204" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Small comb made of wooden sticks partially wrapped with tinfoil. 5.7 cm long. Matschemba." Previous owner Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of what is now Tanzania Biographical fragments Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and has been from the Makonde plateau since the 1870s dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania. His residence was in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908. Appropriation context When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. Von Trotha reports: “Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched on the 6th from Sudi, where the companies were gathered partly by steamers, partly by foot, to Luagalla, the residence of Matschembas , from. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys a great reputation among his people and through several small features he showed that he has a more developed sense of decency than the native chiefs. ”(Deutsches Kolonialblatt 1896, p. 101) Trotha decided to stay in Luagalla only for a short time and so she marched 8. Company with Glauning with powder, ivory and guns back to the coast. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102). In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known. Sources Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag. Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest. Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On a visit to Machemba , Pp. 408-411. Deutsches Kolonialblatt 1897: On the situation in the hinterland of Lindi, p. 167. Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510. Bundesarchiv R 1001/287 Bundesarchiv R 1001/747 SMB -PK, EM, E 254/1896 SMB-PK, EM, E 1150/1896 SMB-PK, EM, E 1021/1896</t>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Small comb made of wooden sticks partially wrapped with tinfoil.
+5.7 cm long.
+Matschemba. "
+Previous owner
+Machemba bin Mshame al Masaninga (until 1895), trader and 'chief' in the hinterland of the southern coastal region of today's Tanzania
+Biographical fragments
+Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and had dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania from the Makonde plateau since the 1870s. His residence was among others in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908.
+Appropriation context
+When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. From Trotha reports:
+"Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched from Sudi on the 6th, where the companies were gathered, partly by steamboat, partly by foot, to Luagalla, the residence of Matschemba. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys great prestige among his people and, through several small traits, shows that he has a more developed sense of decency than the native chiefs otherwise. ”(Deutsches Kolonialblatt 1896, p. 101)
+Trotha decided to stay in Luagalla only for a short time and so the 8th company marched back to the coast with powder, ivory and guns under Glauning. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102).
+In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known.
+sources
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag.
+Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest.
+Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the Raids of the Chief Machemba.
+Deutsches Kolonialblatt 1896: About his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: About a visit to Machemba, pp. 408-411.
+Deutsches Kolonialblatt 1897: About the conditions in the hinterland by Lindi, p. 167.
+Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510.
+Federal archive R 1001/287
+Federal archive R 1001/747
+SMB-PK, EM, E 254/1896
+SMB-PK, EM, E 1150/1896
+SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
       <c r="D204" t="n">
@@ -38096,9 +38533,10 @@
 Wangindo"</t>
         </is>
       </c>
-      <c r="B205" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Headrest (kidehu) made of wood. 39 cm above. Length 10.5 cm high (outside) Wangindo"</t>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Headrest (kidehu) made of wood. 39 cm above. Length 10.5 cm high (outside)
+Wangindo "</t>
         </is>
       </c>
       <c r="D205" t="n">
@@ -38111,7 +38549,7 @@
           <t>Historischer Hauptkatalog: "Kriegsbeil mit Blattförmiger Klinge. Das verdickte obere Ende des Schaftes mit Messing- u. Kupferstiften verziert. Schaft 75 cm lg. Klinge 40,5 cm. Irangi"</t>
         </is>
       </c>
-      <c r="B206" s="3" t="inlineStr">
+      <c r="B206" t="inlineStr">
         <is>
           <t>Historical main catalog: "hatchet with leaf-shaped blade. The thickened upper end of the shaft decorated with brass and copper pins. 75 cm long shaft. 40.5 cm blade. Irangi"</t>
         </is>
@@ -38126,7 +38564,7 @@
           <t>Historischer Hauptkatalog: "Kugel aus Rotholzpulover. Das Pulver wird mit Wasser zu einem Teig geknetet, zu Kugeln geformt und an der Sonne getrocknet. Hiervon wird nach Bedarf entnommen. 14 cm Dm. Ebendaher [Wawemba]"</t>
         </is>
       </c>
-      <c r="B207" s="3" t="inlineStr">
+      <c r="B207" t="inlineStr">
         <is>
           <t>Historical main catalog: "Ball of redwood powder. The powder is kneaded with water into a dough, formed into balls and dried in the sun. From this is taken as required. 14 cm diameter. Ebendaher [Wawemba]"</t>
         </is>
@@ -38142,9 +38580,10 @@
 Wakinga."</t>
         </is>
       </c>
-      <c r="B208" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Grass braided together into a closed ring, ready for basket weaving. Wakinga."</t>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Grass braided together into a closed ring, ready for basket weaving.
+Wakinga. "</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -38159,9 +38598,11 @@
 Unyamwanga (Msuma)."</t>
         </is>
       </c>
-      <c r="B209" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Ear peg of a woman. Made of wood, on one side with tinfoil coating and with a brass button in the middle. 4.4 cm in diameter, 1.7 cm thick. Unyamwanga (Msuma)."</t>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Ear peg of a woman. Made of wood, on one side with tinfoil coating and with a brass button in the middle.
+4.4 cm diameter, 1.7 cm thick.
+Unyamwanga (Msuma). "</t>
         </is>
       </c>
       <c r="D209" t="n">
@@ -38174,7 +38615,7 @@
           <t>Historischer Hauptkatalog: "Ohrring aus Messing mit Kupferdrahtspirale umwickelt; mit rotem Stein (tunguluasi). Der Stein stammt angeblich aus Umburru bei Mangati, woselbst diese Steine gefunden , verarbeitet u. gegen Ziegen verkauft werden. Irangi (Vom Sultan Muhâmba von Paî in Irangi, Ostabhang der Irangiberge, getragen.)"</t>
         </is>
       </c>
-      <c r="B210" s="3" t="inlineStr">
+      <c r="B210" t="inlineStr">
         <is>
           <t>Historical main catalog: "Brass earring wrapped with copper wire spiral; with red stone (tunguluasi). The stone is said to come from Umburru near Mangati, where these stones are found, processed and sold to goats. Irangi (By Sultan Muhâmba von Paî in Irangi, Eastern slope of the Iran mountains, worn.) "</t>
         </is>
@@ -38189,9 +38630,9 @@
           <t>Historischer Hauptkatalog: "ose sango", Zeremonialgerät des Donnergottes [Saulgo], Tanzkeule, Glied einer ose-Sänger-Kette. L. 21,3</t>
         </is>
       </c>
-      <c r="B211" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "ose sango", ceremonial device of the god of thunder [Saulgo], dance club, link in an ose-singer chain. L. 21.3</t>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "ose sango", ceremonial device of the god of thunder [Saulgo], dance club, link in an ose singer chain. L. 21.3</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -38228,9 +38669,33 @@
 SMP-PK, EM, I/MV 956</t>
         </is>
       </c>
-      <c r="B212" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Stringed instrument" gombo "= 4964 resonance box, also unrepairable, therefore destroyed. It was kept in a large sack made of cotton fabric of the shape [drawing] a. 107 cm long. The handle runs out into a stylized face. Uhehe "a) 6-string (missing), a carved handle with a stylized head and a cotton sack (b) in which the resonance calabash was kept. But since it was destroyed according to the documents, it was destroyed. Previous owner Mkwavinyika Munyigumba Mwamuyinga (Mkwawa), 'chief' of the Hehe (1879 to 1898) Biographical fragments of Mkwawa Mwavinyika Munyigumba Mwamu, also called Mkwawa, was ruler of the Hehe Empire from 1879. His father Munyigumba is considered the founder and left his son a centralized state with a high degree of military organization, in which political and social control was in the hands of the state. The expansion of the Hehe Empire was characterized not only by peaceful phases since the 1860s, but also by wars. The hehe is made up of the conquered and annexed populations. Those who opposed the tribunal system of the state were fought, those willing to cooperate were integrated into the Hehe society through kinship relationships, the territory of which made up a good fifth of the area of what would later become German East Africa. In order to protect his rule and power structures, Mkwawa probably supported the uprising of the population between 1888 and 1890, as well as the economic and administrative elites in the northern coastal region of today's Tanzania against the claim to rule of German-East African society. The Germans then tried to enforce their rule inland and to control the ties routes. In 1891 Mkwawa near Rugaro (today Luagalo, near Iringa) defeated German troops under the leadership of Emil von Zelewski. For the so-called Imperial Guard, it was one of the most loss-making defeats in its history. After this - from a German perspective - disgraceful defeat, which questioned the invincibility of the Germans and deconstructed their feelings of superiority anchored in colonial ideology, Mkwawa became a formative enemy for the German colonizers. Mkwawa and his followers should be destroyed. Mkwawa tried repeatedly to negotiate with the German administration in the following years - without success. Years of war began. In 1894 the Germans conquered the capital of the Hehe Empire, Kalenga, with their colonial troops and almost completely destroyed it. They captured, among other things, large quantities of ivory and also objects captured by the Germans during the battles of Rugaro through the hehe. Mkwawa escaped with his troops. Mkwawa's power shrank, not least because the Germans increasingly controlled the caravan routes. The economy of the Hehe Empire and its power was based on access to the caravan trade - he could distribute less and less to his subordinates. There was also increasing rivalry within the Hehe leadership (eg with his brother Mpangile) and more and more Hehe cooperated with the Germans and fought on their side. The period after 1896 was more and more like a civil war, in which Mkwawa brutally acted against those who were no longer loyal. The Germans, on the other hand, pursued a scorched earth policy against the Hehe, which Mkwawa supposedly supported. In 1896 Mkwawa's brother Mpangile was used by the Germans as the 'chief' of the Hehe, but was executed as early as 1897 because he was accused of continuing to support Mkwawa. In 1896 and 1897 the Germans led two campaigns to capture Mkwawa, who waged a guerrilla war and was able to escape the Germans and their allies again and again. In 1898 he was followed by a small German patrol with the few remaining followers and circled. He committed suicide on July 19, 1898 with his rifle near the cave at Mlambalasi, where he had probably spent the last months of his life. Appropriation context The station chief of Mpapua Hans Glauning, lieutenant of the so-called Imperial Guard for German East Africa, received on September 25, 1896 a letter from Captain Tom von Prince from Iringa with a request for troops to "finally defeat" Mkwawa. Glauning was entrusted with the persecution of Mkwawa, which lasted about fifty days but was unsuccessful - Mkwawa escaped, but a musical instrument (a shell zither) came into Glauning's possession that Mkwawa was said to have heard personally. Probably at the beginning of November 1896 Glauning reached the Mlogolo Mountains (today Iringa region in Tanzania), where they were able to locate the Mkwawa caravan through trapped heights: "I sent down patrols on either side of the path. We had already been noticed, however Weir warriors on the cue threw themselves at us as the patrols on the right and left of the caravan intervened in the fight after a short resistance, after a short resistance the escapes escaped, leaving several dead, their loads and even spears and shields on the Escaping through the thicket prevented a close pursuit of the light-footed opponent was impossible for the Askaris carrying their luggage in the difficult terrain. Among the prisoners were two young sons of the Kwawa who had fled the first shots. His loads of food, cloth , Powder, utensils, many spears and shields fell into our hands. " (Glauning, Hans (1898): Uhehe (negotiations of the Berlin-Charlottenburg department of the German Colonial Society). Berlin: Reimer Verlag, p. 49) "The Gomas (drums) and stringed instruments found prove that the Wahehe also deal with music. Kwawa even carried a stringed instrument in a cloth wrapping with him during the flight. (Glauning 1898, p. 63) "In a letter from Glauning to Felix von Luschan, the assistant director of the Museum of Ethnology in Berlin, on June 20, 1897, he emphasized first, that it is a musical instrument from Mkwawa. “I captured the big pumpkin musical instrument from Quawa myself, whom I came across during the persecution, as it is now, without strings and in an Americano case. I purposely didn't change anything. 2 children of Quawa, whom I caught on this occasion, expressly assured that it was their father's musical instrument. ”(SMP-PK, EM, I / MV 956)" Musical instrument (gombo), Quawa's personal property in the case, from Quawa himself captured. " (List of objects Glauning, SMB-PK, EM, I / MV 717, 675/1897, Bl. 225) Sources Baer, Martin and Schröter, Olaf (2001): A headhunt. Germans in East Africa. Berlin: Ch. Links. Glauning, Hans (1898): Uhehe (negotiations of the Berlin-Charlottenburg department of the German Colonial Society). Berlin: Reimer Verlag. Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin: Reimer, pp. 66-149. Nigmann, E. (1908): The Wahehe. Their history, cult, legal, war and hunting customs. Berlin: Ernst Siegfried Mittler and son. Pizzo, David (2010): "To devour the land of Mkwawa": Colonial Violence and the German-Hehe War in East Africa c. 1884-1914. Dissertation at the Department of History, University of North Carolina. Redmayne, Alison (1964). The Wahehe People of Tanzania. Oxford: Dissertation. Redmayne (1968) “Mkwawa and the Hehe Wars.” Journal of African History, IX (3), pp. 409-36. Weber, Kristin (2005): Objects as a Mirror of Colonial Relationships - The Collecting of Ethnographica at the Time of German Colonial Expansion in East Africa (1884–1914). Master thesis at the Seminar for African Studies, Humboldt University Berlin. SMB-PK, EM, I / MV 717, E 675/1897 SMP-PK, EM, I / MV 956</t>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Stringed instrument" gombo "= 4964 resonance box, also unrepairable, therefore destroyed. It was kept in a large sack made of cotton fabric with the shape [drawing] a. 107 cm long. The handle runs out into a stylized face. Uhehe "
+a) 6-string (missing), a carved handle with a stylized head and a cotton sack (b) in which the resonance calabash was kept. But since it was destroyed according to the documents, it was destroyed.
+Previous owner
+Mkwavinyika Munyigumba Mwamuyinga (Mkwawa), 'chief' of the Hehe (1879 to 1898)
+Biographical fragments of Mkwawa
+Mwavinyika Munyigumba Mwamu, also called Mkwawa, was ruler of the Hehe Empire from 1879. His father Munyigumba is considered the founder and left his son a centralized state with a high degree of military organization, in which political and social control was in the hands of the state. The expansion of the Hehe Empire was characterized not only by peaceful phases since the 1860s, but also by wars. The hehe is made up of the conquered and annexed populations. Those who opposed the tribunal system of the state were fought, those willing to cooperate were integrated into the Hehe society through kinship relationships, the territory of which made up a good fifth of the area of what would later become German East Africa. In order to protect his rule and power structures, Mkwawa probably supported the uprising of the population from 1888 to 1890 as well as the economic and administrative elites in the northern coastal region of today's Tanzania against the claim to rule of German-East African society. The Germans then tried to enforce their rule inland and to control the ties routes. In 1891 Mkwawa near Rugaro (today Luagalo, near Iringa) defeated German troops under the leadership of Emil von Zelewski. For the so-called Imperial Guard, it was one of the most loss-making defeats in its history. After this - from a German perspective - disgraceful defeat, which questioned the invincibility of the Germans and deconstructed their feelings of superiority anchored in colonial ideology, Mkwawa became a formative enemy for the German colonizers. Mkwawa and his followers should be destroyed. Mkwawa tried repeatedly to negotiate with the German administration in the following years - without success. Years of war began. In 1894 the Germans conquered the capital of the Hehe Empire, Kalenga, with their colonial troops and almost completely destroyed it. Among other things, they captured large quantities of ivory and also objects captured by the Germans during the battles of Rugaro through the hehe. Mkwawa escaped with his troops. Mkwawa's power shrank, not least because the Germans increasingly controlled the caravan routes. The economy of the Hehe Empire and its power was based on access to the caravan trade - he could distribute less and less to his subordinates. There were also increasing rivalries within the Hehe leadership (e.g. with his brother Mpangile) and more and more Hehe cooperated with the Germans and fought on their side. The period after 1896 was more and more like a civil war, in which Mkwawa brutally acted against those who were no longer loyal. The Germans, on the other hand, pursued a scorched earth policy against the Hehe, which Mkwawa supposedly supported. In 1896, Mkwawa's brother Mpangile was used by the Germans as the 'chief' of the Hehe, but was executed in 1897 because of the continued support of Mkwawa. In 1896 and 1897 the Germans led two campaigns to capture Mkwawa, who waged a guerrilla war and was able to escape the Germans and their allies again and again. In 1898 he was followed by a small German patrol with the few remaining followers and circled. He committed suicide on July 19, 1898 with his rifle near the cave at Mlambalasi, where he had probably spent the last months of his life.
+Appropriation context
+The station chief of Mpapua Hans Glauning, lieutenant of the so-called Imperial Guard for German East Africa, received on September 25, 1896 a letter from Captain Tom von Prince from Iringa with a request for troops to "finally defeat" Mkwawa. Glauning was entrusted with the persecution of Mkwawa, which took about fifty days but was unsuccessful - Mkwawa escaped, but a musical instrument (a shell zither) came into Glauning's possession that Mkwawa was said to have heard personally. Probably at the beginning of November 1896 Glauning reached the Mlogolo Mountains (today Iringa region in Tanzania), where they were able to locate the Mkwawa caravan through trapped hehe:
+"I sent patrols on either side of the way. We had already been noticed, however. The war-warriors at the cue threw themselves against us, while the patrols on the right and left of the caravan intervened in the fight. After short resistance. After a short resistance escaped the Wahhehe, leaving several dead, their loads, and even spears and shields that prevented them from escaping through the thicket.Tight-footed pursuit of the light-footed opponent was impossible for the Askaris carrying their luggage in the difficult terrain two young sons of the Kwawas, who had fled the first shots. His loads of food, cloth, powder, utensils, many spears and shields fell into our hands. " (Glauning, Hans (1898): Uhehe (negotiations of the Berlin-Charlottenburg department of the German Colonial Society). Berlin: Reimer Verlag, p. 49)
+"The Gomas (drums) and stringed instruments found prove that the Wahehe also deal with music. Kwawa even carried with him a stringed instrument in a cloth cover. (Glauning 1898, p. 63)"
+In a letter from Glauning to Felix von Luschan, the assistant director of the Museum für Völkerkunde in Berlin, dated June 20, 1897, he emphasized once again that it was Mkwawa's musical instrument.
+“I captured the big pumpkin musical instrument from Quawa myself, whom I came across during the persecution, as it is now, without strings and in an Americano case. I purposely didn't change anything. 2 Quawa's children, whom I caught on this occasion, expressly assured that it was her father's musical instrument. ”(SMP-PK, EM, I / MV 956)
+"Musical instrument (gombo), Quawa's personal property in its case, captured by Quawa himself." (Object list Glauning, SMB-PK, EM, I / MV 717, 675/1897, Bl. 225)
+sources
+Baer, Martin and Schröter, Olaf (2001): A headhunt. Germans in East Africa. Berlin: Ch. Links.
+Glauning, Hans (1898): Uhehe (negotiations of the Berlin-Charlottenburg department of the German Colonial Society). Berlin: Reimer Verlag.
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Ivanov, Paola and Kristin Weber-Sinn (2018): Generosity and Violence: Objects from Colonial Wars in the Depot of the Ethnological Museum, Berlin. In: Lili Reyels, Ivanov, Weber-Sinn (ed.): Objects from the colonial wars in the Ethnological Museum, Berlin. A Tanzanian-German dialogue. Berlin: Reimer, pp. 66-149.
+Nigmann, E. (1908): The Wahehe. Their history, cult, legal, war and hunting customs. Berlin: Ernst Siegfried Mittler and son.
+Pizzo, David (2010): "To devour the land of Mkwawa": Colonial Violence and the German-Hehe War in East Africa c. 1884-1914. Dissertation at the Department of History, University of North Carolina.
+Redmayne, Alison (1964). The Wahehe People of Tanzania. Oxford: Dissertation.
+Redmayne (1968) “Mkwawa and the Hehe Wars.” Journal of African History, IX (3), pp. 409-36.
+Weber, Kristin (2005): Objects as a Mirror of Colonial Relationships - The Collecting of Ethnographica at the Time of German Colonial Expansion in East Africa (1884–1914). Master thesis at the Seminar for African Studies, Humboldt University Berlin.
+SMB-PK, EM, I / MV 717, E 675/1897
+SMP-PK, EM, I / MV 956</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -38244,9 +38709,10 @@
 Waburungi"</t>
         </is>
       </c>
-      <c r="B213" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Jewelry of the Sultan Damass von Goima in Burungi (Wagogo work). A) Leather ring, 7.5 cm in diameter b and c) 2 thin brass arm rings, 6.5 cm in diameter d, e, f) 3 thin iron chains. Waburungi "</t>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Jewelry of the Sultan Damass von Goima in Burungi (Wagogo work). A) Leather ring, 7.5 cm in diameter b and c) 2 thin brass arm rings, 6.5 cm in diameter d, e, f) 3 thin iron chains.
+Waburungi "</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -38259,7 +38725,7 @@
           <t>Historischer Hauptkatalog: "Schnupftabaksbüchse aus Bambus, mit Schnitzereien verziert. 63 cm lang. Süd-Usaramo (südl. vom Liwala)"</t>
         </is>
       </c>
-      <c r="B214" s="3" t="inlineStr">
+      <c r="B214" t="inlineStr">
         <is>
           <t>Historical main catalog: "Snuffbox made of bamboo, decorated with carvings. 63 cm long. South Usaramo (south of Liwala)"</t>
         </is>
@@ -38297,9 +38763,32 @@
 SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
-      <c r="B215" s="3" t="inlineStr">
-        <is>
-          <t>Main historical catalog: "Walking stick, also a tobacco rifle, carved. 87 cm long. Matschemba" Previous owner Machemba bin Mshame al Masaninga, dealer and 'chief' in the hinterland of the southern coastal region of today's Tanzania Biographical fragments Machemba bin Mshame al Masaninga was an influential dealer belonged to the Yao and had dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania from the Makonde plateau since the 1870s. His residence was in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908. Appropriation context When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. Von Trotha reports: “Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched on the 6th from Sudi, where the companies were gathered partly by steamers, partly by foot, to Luagalla, the residence of Matschembas , from. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys a great reputation among his people and through several small features he showed that he has a more developed sense of decency than the native chiefs. ”(Deutsches Kolonialblatt 1896, p. 101) Trotha decided to stay in Luagalla only for a short time and so she marched 8. Company with Glauning with powder, ivory and guns back to the coast. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102). In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known. Sources Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press. Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag. Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest. Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the raids of the chief Machemba. Deutsches Kolonialblatt 1896: On his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101. Deutsches Kolonialblatt 1896: On a visit to Machemba , Pp. 408-411. Deutsches Kolonialblatt 1897: On the situation in the hinterland of Lindi, p. 167. Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510. Bundesarchiv R 1001/287 Bundesarchiv R 1001/747 SMB -PK, EM, E 254/1896 SMB-PK, EM, E 1150/1896 SMB-PK, EM, E 1021/1896</t>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Walking stick, also tobacco rifle, carved. 87 cm long. Matschemba"
+Previous owner
+Machemba bin Mshame al Masaninga, trader and 'chief' in the hinterland of the southern coastal region of today's Tanzania
+Biographical fragments
+Machemba bin Mshame al Masaninga was an influential trader who belonged to the Yao and had dominated the hinterland of the southern coastal region (from Kilwa in the north to the south to Mikindani) of today's Tanzania from the Makonde plateau since the 1870s. His residence was among others in Luagalla on the Makonde plateau. He also had great support from the Yao on the Portuguese side (today's Mozambique). He offered refuge to slaves who had fled the coast and thus gained a large following, from which he also recruited his fighters. In terms of trade policy, he competed with the Swahili traders on the coast and reduced their profits by selling coveted imported goods to the caravans coming from inland, which consequently no longer traveled to the coastal cities. This later also minimized the profit of the Germans, who tried to subdue Machemba in several war campaigns. Machemba successfully resisted the claim to German rule for a long time, pretended to cooperate, but at the same time pursued his own agenda. In 1898, however, he had to flee to the neighboring Portuguese territory, where he died in 1908.
+Appropriation context
+When Hans Glauning took up his duties in Kilwa in early 1895 as a non-commissioned officer and company leader of the so-called Imperial Guard for East Africa, military action against Machemba was planned, which Glauning also wrote to Felix von Luschan, the assistant director at the Kgl. Museum of Ethnology announced. After Glauning had previously taken part in the war against the trader Hassan bin Omari (Makunganya) and brought the prisoners, including Makunganya, to Kilwa Kiwinje with the 8th company, the order to Lt. Lothar von Trotha was issued on 2 December 1895 with three companies to stand by in Lindi "to deal with the Machemba affair". The 8th company and with it Hans Glauning came from Kilwa to Lindi via steamer. From Trotha reports:
+"Matschemba had not come to the coast, as he had promised as a sign of submission, and I consequently marched from Sudi on the 6th, where the companies were gathered, partly by steamboat, partly by foot, to Luagalla, the residence of Matschemba. The march there, except for a few comments, which I will allow myself to conclude, offered nothing remarkable militarily. Matschemba appeared halfway at Masno, returned to Luagalla with me, and most emphatically explained to me his willing intention to submit and keep the peace with the government. He could not or did not want to fulfill the penalties imposed on him in ivory and powder in full, but he immediately gave up a large part of his rifles immediately when I told him that they should be the replacement for the missing ivory and powder . Matschemba made a good impression on me. He enjoys great prestige among his people and, through several small traits, shows that he has a more developed sense of decency than the native chiefs otherwise. ”(Deutsches Kolonialblatt 1896, p. 101)
+Trotha decided to stay in Luagalla only for a short time and so the 8th company marched back to the coast with powder, ivory and guns under Glauning. The other companies also left Luagalla. Machemba's offer of peace was accepted and therefore no station was planned in the Luagalla area. Because of the prevailing famine, Machemba was not obliged to cater for German "expeditions". "The expedition was poor in military activity, the richer in marching performance, (...), so von Trotha concluded in his report (Deutsches Kolonialblatt 1896, pp. 101-102).
+In the context of the meeting, objects that were partly attributed to Machemba came into Glauning's possession. The exact circumstances of the appropriation are not yet known.
+sources
+Iliffe, John (1979): A Modern History of Tanganyika. Cambridge: Cambridge University Press.
+Luschan, Felix von (1897): Contributions to the ethnology of the German protected areas (extended special edition from the "Official report on the first German colonial exhibition in Treptow 1896"). Berlin: Dietrich Reimer Verlag.
+Müller, Fritz F. (1959): Germany, Zanzibar, East Africa. History of a German colonial conquest.
+Deutsches Kolonialblatt (Official Gazette for the Protected Areas of the German Reich 1895: On the Raids of the Chief Machemba.
+Deutsches Kolonialblatt 1896: About his happily ended expedition against Hassan bin Omari and Matschemba, pp. 99-101.
+Deutsches Kolonialblatt 1896: About a visit to Machemba, pp. 408-411.
+Deutsches Kolonialblatt 1897: About the conditions in the hinterland by Lindi, p. 167.
+Deutsches Kolonialblatt 1899: Expedition against the chief Machemba, pp. 509-510.
+Federal archive R 1001/287
+Federal archive R 1001/747
+SMB-PK, EM, E 254/1896
+SMB-PK, EM, E 1150/1896
+SMB-PK, EM, E 1021/1896</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -38312,7 +38801,7 @@
           <t>Historischer Hauptkatalog: "Streitaxt. Stiel 80 cm lg. wird zu 2en neben dem Stoßspeer) im Innern des Schildes getragen. Schabrumaleute (Mafiti)"</t>
         </is>
       </c>
-      <c r="B216" s="3" t="inlineStr">
+      <c r="B216" t="inlineStr">
         <is>
           <t>Historical main catalog: "Battle ax. Handle 80 cm lg. Is carried in groups of 2 next to the shock spear) inside the shield. Schabruma people (Mafiti)"</t>
         </is>
@@ -38328,9 +38817,10 @@
 Konde (Landschaft Nseria)"</t>
         </is>
       </c>
-      <c r="B217" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Chair made of wood, depicting a hyena (kikonde:" kindingo "). May only be used by the Sultan. 65 cm long. Konde (landscape Nseria)"</t>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Chair made of wood, depicting a hyena (kikonde:" kindingo "). May only be used by the Sultan. 65 cm lg.
+Konde (landscape Nseria) "</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -38343,7 +38833,7 @@
           <t>Historischer Hauptkatalog: "Wurfkeule aus Holz, "luguma". Werden den fliehenden Feinden nachgeworfen. 56 cm lg. Wahumba u. Massai"</t>
         </is>
       </c>
-      <c r="B218" s="3" t="inlineStr">
+      <c r="B218" t="inlineStr">
         <is>
           <t>Historical main catalog: "Throwing club made of wood," luguma ". Thrown at the fleeing enemies. 56 cm long Wahumba and Maasai"</t>
         </is>
@@ -38359,9 +38849,10 @@
 Wangindo"</t>
         </is>
       </c>
-      <c r="B219" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Two combs (kikwe [...] uro). Worn in man's and woman's hair. Braided with hair, covered with staniol. Wangindo"</t>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Two combs (kikwe [...] uro). Worn in man's and woman's hair. Braided with hair, covered with tinfoil.
+Wangindo "</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -38374,7 +38865,7 @@
           <t>Historischer Hauptkatalog: "Zwei Ohrpflöcke 1,7 cm hoch 2,5 cm dm. Wagogo"</t>
         </is>
       </c>
-      <c r="B220" s="3" t="inlineStr">
+      <c r="B220" t="inlineStr">
         <is>
           <t>Historical main catalog: "Two ear pegs 1.7 cm high 2.5 cm dm. Wagogo"</t>
         </is>
@@ -38391,9 +38882,11 @@
 Wanguru u. Wakaguru."</t>
         </is>
       </c>
-      <c r="B221" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Two ear pegs made of ebony, one decorated with brass nail. About 4 cm in diameter. Wanguru and Wakaguru."</t>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Two ear pegs made of ebony, one decorated with a brass nail.
+approx. 4 cm in diameter
+Wanguru et al. Wakaguru. "</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -38411,9 +38904,14 @@
 Uhehe"</t>
         </is>
       </c>
-      <c r="B222" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Two spindles (from) and a stick with wound cotton thread. A: 43.5 cm lg. B: 44.5 cm lg. C: 42.0 cm lg. From: niondo [?]. Uhehe"</t>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Two spindles (from) and a rod with wound cotton thread.
+a: 43.5 cm lg.
+b: 44.5 cm lg.
+c: 42.0 cm lg.
+from: niondo [?].
+Uhehe "</t>
         </is>
       </c>
       <c r="D222" t="n">
@@ -38426,7 +38924,7 @@
           <t>Historischer Hauptkatalog: "´kitenga´. 2 Ohrpflöcke aus Holz, eine Fläche mit Eisenblech belegt. Von Weibern getragen. Sollen aus Mambue eingeführt oder Nachahmung von Mambue-Arbeit sein. 3,8 cm Dm. Ebendaher [Fipa]"</t>
         </is>
       </c>
-      <c r="B223" s="3" t="inlineStr">
+      <c r="B223" t="inlineStr">
         <is>
           <t>Historical main catalog: "´kitenga´. 2 wooden earpicks, one surface covered with sheet iron. Worn by women. Should be imported from mambue or imitation of mambue work. 3.8 cm diameter. Ebendaher [Fipa]"</t>
         </is>
@@ -38441,7 +38939,7 @@
           <t>Historischer Hauptkatalog: "´magandu´. Taillenband aus kleinen Messingperlen; an beiden Enden der Schnur je 1 Doppelspirale aus Messing (wie bei III E 7422). Getragen von Sultan maisida im Ukinga-Gebirge. 180 cm lg. (von Spirale zu Spirale). Wakinga-Arbeit"</t>
         </is>
       </c>
-      <c r="B224" s="3" t="inlineStr">
+      <c r="B224" t="inlineStr">
         <is>
           <t>Historical main catalog: "´magandu". Waistband made of small brass beads; 1 double spiral made of brass at both ends of the cord (as with III E 7422). Worn by Sultan maisida in the Ukinga Mountains. 180 cm long (from spiral to spiral) Wakinga work "</t>
         </is>
@@ -38456,7 +38954,7 @@
           <t>Historischer Hauptkatalog: "´ndevule´ Ohrpflock aus Flaschenkürbis. Eine Seite mit blauen u. weißen Perlen verziert, auf der entgegengesetzten 4 runde Löcher, mit Kupfer- u. Messingblech gerandet. 4,8 cm Dm. 2,4 cm dick. Von Wasafua-Weibern getragen (wahrschnl. Wanyika-Arbeit). Vora am Songwe"</t>
         </is>
       </c>
-      <c r="B225" s="3" t="inlineStr">
+      <c r="B225" t="inlineStr">
         <is>
           <t>Historic main catalog: "´ndevule´ ear plug made of bottle gourd. One side decorated with blue and white pearls, on the opposite 4 round holes, edged with copper and brass sheet. 4.8 cm diameter. 2.4 cm thick. From Wasafua -Women worn (probably Wanyika work). Especially on the Songwe "</t>
         </is>
@@ -38471,7 +38969,7 @@
           <t>Historischer Hauptkatalog: "´ose sango´. Nord Yoruba. Tanzkeule; Glied einer ose-sango-Kette. L. 12,7 cm"</t>
         </is>
       </c>
-      <c r="B226" s="3" t="inlineStr">
+      <c r="B226" t="inlineStr">
         <is>
           <t>Historical main catalog: "´ose sango". North Yoruba. Dance club; link of an ose-sango chain. L. 12.7 cm "</t>
         </is>
@@ -38486,7 +38984,7 @@
           <t>Historischer Hauptkatalog: "´ose schango´ Nord Yoruba. Tanzkeule; einfacher, runder Stab mit einer Öse am unteren Ende und 2 großen Donnerkeilen am oberen Ende, zwischen denen sich auf jeder Seite je ein menschliches Gesicht befindet. H.: 47,5 cm. Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B227" s="3" t="inlineStr">
+      <c r="B227" t="inlineStr">
         <is>
           <t>Historical main catalog: "´ose schango´ North Yoruba. Dance club; simple, round stick with an eyelet at the lower end and 2 large thunderbolts at the upper end, between which there is a human face on each side. H .: 47.5 cm North Yoruba "</t>
         </is>
@@ -38501,9 +38999,9 @@
           <t>Historischer Hauptkatalog: "´ose schango´. Tanzkeule; auf einem stabförmigen Sockel stehende menschliche Figur mit künstlerischer Haarfrisur und 2 Donnerkeilen auf dem Kopfe; auf beiden Schultern liegt eine Schlange, die mit den Händen festgehalten wird. H.: 64,4 cm. Nord Yoruba"</t>
         </is>
       </c>
-      <c r="B228" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "´ose schango". Dance club; human figure standing on a rod-shaped base with an artistic hairstyle and 2 thunderbolts on the head; on both shoulders is a snake, which is held with the hands. H .: 64.4 cm. North Yoruba "</t>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "´ose schango". Dance club; human figure standing on a rod-shaped base with artistic hairstyle and 2 thunderbolts on the head; on both shoulders is a snake that is held with the hands. H .: 64.4 cm. North Yoruba "</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -38517,9 +39015,10 @@
 Ahnenkrug aus Ton mit Kopf, der wahrscheinlich den Verstorbenen vorstellt.</t>
         </is>
       </c>
-      <c r="B229" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: 'kusson' clay jug with a head, which probably introduces the deceased.</t>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Historic main catalog: 'kusson'
+Clay ancestral jar with a head, which probably introduces the deceased.</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -38532,7 +39031,7 @@
           <t>Historischer Hauptkatalog: (Geschnitzte Zeremonialaxt des Gottes Schango.) stilisierte menschl. (weibl.) Figur mit 2 Donnerkeilen ("ara-dung") auf dem Kopfe; rot bemalt. H. 46,3 cm. Nord Yoruba</t>
         </is>
       </c>
-      <c r="B230" s="3" t="inlineStr">
+      <c r="B230" t="inlineStr">
         <is>
           <t>Main historical catalog: (Carved ceremonial ax of the god Schango.) Stylized human. (female) figure with 2 thunderbolts ("ara-dung") on the head; painted red. H. 46.3 cm. North Yoruba</t>
         </is>
@@ -38547,7 +39046,7 @@
           <t>historischer Hauptkatalog: Nagelfetisch in Tiergestalt mit zwei Köpfen</t>
         </is>
       </c>
-      <c r="B231" s="3" t="inlineStr">
+      <c r="B231" t="inlineStr">
         <is>
           <t>historical main catalog: nail fetish in animal form with two heads</t>
         </is>
@@ -38565,9 +39064,12 @@
 Landschaft Tunda, Land Kamba."</t>
         </is>
       </c>
-      <c r="B232" s="3" t="inlineStr">
-        <is>
-          <t>Historical main catalog: "Round perforated stone, Regenda [...]. Supposedly fell from the sky. Probably used earlier to insert the tips of the bellows. 9.7: 6.2 cm in diameter. Mkendi's village, landscape tunda, country Kamba. "</t>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Historical main catalog: "Round perforated stone, Regenda [...]. Allegedly fallen from the sky. Probably used earlier to insert the tips of the bellows.
+9.7: 6.2 cm dia.
+Mkendi's village,
+Tunda landscape, Kamba country. "</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -38580,7 +39082,7 @@
           <t>Historischer Hausptkatalog: "Kopfbank 26 cm. br. 20cm hoch. Zambezi-Gebiet"</t>
         </is>
       </c>
-      <c r="B233" s="3" t="inlineStr">
+      <c r="B233" t="inlineStr">
         <is>
           <t>Historical house catalog: "Head bench 26 cm. Br. 20cm high. Zambezi area"</t>
         </is>
@@ -38595,7 +39097,7 @@
           <t>Hocker mit weiblicher Trägerfigur</t>
         </is>
       </c>
-      <c r="B234" s="3" t="inlineStr">
+      <c r="B234" t="inlineStr">
         <is>
           <t>Stool with a female figure</t>
         </is>
@@ -38610,7 +39112,7 @@
           <t>Hohler Tonring, der eine Öffnung mit hochgezogenem Rand aufweist (eine Art Aufsatz). Dieser ist mit runden und eckigen geometr. Muster - Typ. Kadiweu-Mustern - versehen. Oberseite ist bunt bemalt.</t>
         </is>
       </c>
-      <c r="B235" s="3" t="inlineStr">
+      <c r="B235" t="inlineStr">
         <is>
           <t>Hollow clay ring with an opening with a raised edge (a kind of attachment). This is with round and angular geometr. Pattern - type. Kadiweu patterns - provided. The top is colorfully painted.</t>
         </is>
@@ -38625,7 +39127,7 @@
           <t>Holz, geschnitz, zweizinkig</t>
         </is>
       </c>
-      <c r="B236" s="3" t="inlineStr">
+      <c r="B236" t="inlineStr">
         <is>
           <t>Wood, carved, two-pronged</t>
         </is>
@@ -38640,7 +39142,7 @@
           <t>Holzsandale;in Form einer Holzsohle, die Oberfläche mit Ritzverzierungen und die Ränder gezackt, mit sechs Füßchen darunter. Den Halt für den Fuß bieten Lederriemen, welche durch drei Löcher in der Holzsohle gezogen und verknotet waren aber jetzt zum Teil zerrissen sind.</t>
         </is>
       </c>
-      <c r="B237" s="3" t="inlineStr">
+      <c r="B237" t="inlineStr">
         <is>
           <t>Wooden sandal; in the form of a wooden sole, the surface with incised decorations and the edges serrated, with six feet underneath. The support for the foot is provided by leather straps, which were pulled through three holes in the wooden sole and knotted but are now partially torn.</t>
         </is>
@@ -38655,7 +39157,7 @@
           <t>Karteikarte  "Halsring MBAMBA, aus Messing, unverziert, mit Grünspan."</t>
         </is>
       </c>
-      <c r="B238" s="3" t="inlineStr">
+      <c r="B238" t="inlineStr">
         <is>
           <t>Index card "Neck ring MBAMBA, made of brass, unadorned, with verdigris."</t>
         </is>
@@ -38670,7 +39172,7 @@
           <t>Karteikarte  "Mbamba. Halsring aus Messing, Enden hakenförmig umgebogen zum Zusammenhaken. Auf denselben gereiht 11 Menschenköpfe, gleichfalls aus Messing, mit hohem durchbrochenen Kopfputz. Bei den Bamum ist das Tragen von Schmuck ein Privileg der regierenden Klasse."</t>
         </is>
       </c>
-      <c r="B239" s="3" t="inlineStr">
+      <c r="B239" t="inlineStr">
         <is>
           <t>Index card "Mbamba. Neck ring made of brass, ends bent in a hook shape for hooking. 11 human heads, also made of brass, with high openwork headdresses are lined up on them. With the Bamum, wearing jewelry is a privilege of the ruling class."</t>
         </is>
@@ -38686,9 +39188,10 @@
 Auf eine Bastkapuze aus braunem Bast ist eine Gesichtsscheibe aus Bast, Harz und Leichtholz angeheftet. Die seitlich angenähten Ohren, bemalt, sind rund.</t>
         </is>
       </c>
-      <c r="B240" s="3" t="inlineStr">
-        <is>
-          <t>Index card: bast mask A face disk made of bast, resin and light wood is attached to a bast hood made of brown bast. The ears sewn on the side, painted, are round.</t>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Index card: bast mask
+A face disk made of bast, resin and light wood is attached to a bast hood made of brown bast. The ears sewn on the side, painted, are round.</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -38701,7 +39204,7 @@
           <t>Karteikarte : bemalter Tonkrug.</t>
         </is>
       </c>
-      <c r="B241" s="3" t="inlineStr">
+      <c r="B241" t="inlineStr">
         <is>
           <t>Index card: painted clay jug.</t>
         </is>
@@ -38719,9 +39222,12 @@
 Farben: schwarz, rot, gelb</t>
         </is>
       </c>
-      <c r="B242" s="3" t="inlineStr">
-        <is>
-          <t>Index card: mask made of brownish raffia and carved face part to which the raffia is attached. The bast hood, tied in bast fibers, is tacked together at the top. With the exception of the red painted eyes and mouth, the face is coated with resin. Extremely large and round ears (painted). Colors: black, red, yellow</t>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Index card: mask made of brownish raffia and carved face part to which the raffia is attached.
+The bast hood, tied in bast fibers, is tacked together at the top. With the exception of the red painted eyes and mouth, the face is coated with resin.
+Extremely large and round ears (painted).
+Colors: black, red, yellow</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -38734,7 +39240,7 @@
           <t>Karteikarte : Schale, innen mit roten Mustern bemalt, tiefer</t>
         </is>
       </c>
-      <c r="B243" s="3" t="inlineStr">
+      <c r="B243" t="inlineStr">
         <is>
           <t>Index card: shell, painted inside with red patterns, deeper</t>
         </is>
@@ -38749,7 +39255,7 @@
           <t>Karteikarte : Schale, innen mit roten Mustern bemalt.</t>
         </is>
       </c>
-      <c r="B244" s="3" t="inlineStr">
+      <c r="B244" t="inlineStr">
         <is>
           <t>Index card: Shell, painted inside with red patterns.</t>
         </is>
@@ -38764,7 +39270,7 @@
           <t>Karteikarte : Schale, innen rotes Muster</t>
         </is>
       </c>
-      <c r="B245" s="3" t="inlineStr">
+      <c r="B245" t="inlineStr">
         <is>
           <t>Index card: shell, red pattern on the inside</t>
         </is>
@@ -38780,9 +39286,10 @@
 Schwarz - rote Bemalung auf weißem Grund.</t>
         </is>
       </c>
-      <c r="B246" s="3" t="inlineStr">
-        <is>
-          <t>Index card: clay pot black - red painting on a white background.</t>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Index card: clay pot
+Black and red painting on a white background.</t>
         </is>
       </c>
       <c r="D246" t="n">
@@ -38796,9 +39303,10 @@
 Von außen schwarz - rote Bemalung auf weißem Grund.</t>
         </is>
       </c>
-      <c r="B247" s="3" t="inlineStr">
-        <is>
-          <t>Index card: clay bowl from the outside black - red painting on a white background.</t>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Index card: clay bowl
+From the outside black - red painting on a white background.</t>
         </is>
       </c>
       <c r="D247" t="n">
@@ -38811,7 +39319,7 @@
           <t>Karteikarte : Trinkschale aus Ton, bemalt.</t>
         </is>
       </c>
-      <c r="B248" s="3" t="inlineStr">
+      <c r="B248" t="inlineStr">
         <is>
           <t>Index card: drinking bowl made of clay, painted.</t>
         </is>
@@ -38826,7 +39334,7 @@
           <t>Karteikarte : Wassertopf, mit roten Mustern, gehenkelt.</t>
         </is>
       </c>
-      <c r="B249" s="3" t="inlineStr">
+      <c r="B249" t="inlineStr">
         <is>
           <t>Index card: water pot, with red patterns, go down.</t>
         </is>
@@ -38842,9 +39350,10 @@
 Karteikarte : Maskenkopf.</t>
         </is>
       </c>
-      <c r="B250" s="3" t="inlineStr">
-        <is>
-          <t>Catalog: with this fish mask, light bast is drawn over a cane and attached to the mouth opening, which is reinforced by palm tree stripes. Several different colored concentric circles indicate the eyes. The palms on the sides above and below the open mouth consist of raffia beads. Index card: mask head.</t>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Catalog: with this fish mask, light bast is drawn over a cane and attached to the mouth opening, which is reinforced by palm tree stripes. Several different colored concentric circles indicate the eyes. The palms on the sides above and below the open mouth consist of raffia beads.
+Index card: mask head.</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -38859,9 +39368,11 @@
 Karteikarte : Kleine Gesichtsmaske.</t>
         </is>
       </c>
-      <c r="B251" s="3" t="inlineStr">
-        <is>
-          <t>Small face mask catalog: On a halved, black colored calabash as a face a bright bast hood with two successive protuberances ("horns") is attached. A large, strongly curved wooden nose, two round pegs made of light light wood as eyes and an over-modeled animal bit with inserted, cut teeth made of tin plate are glued to the calabash. The ears are formed by plant stems bent out with bast fabric. There are two holes under the wooden eyes for the eyes of the mask wearer. Index card: small face mask.</t>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Small face mask
+Catalog: On a halved, black-colored calabash as a face a bright bast hood with two successive protrusions ("horns") is attached. A large, strongly curved wooden nose, two round pegs made of light light wood as eyes and an over-modeled animal bit with inserted, cut teeth made of tin plate are glued to the calabash. The ears are formed by plant stems bent out with bast fabric. There are two holes under the wooden eyes for the eyes of the mask wearer.
+Index card: small face mask.</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -38874,7 +39385,7 @@
           <t>Kleiner tönerer Hund mit gerundeten geometrischen Mustern versehen, bunt bemalt.</t>
         </is>
       </c>
-      <c r="B252" s="3" t="inlineStr">
+      <c r="B252" t="inlineStr">
         <is>
           <t>Small clay dog with rounded geometric patterns, brightly painted.</t>
         </is>
@@ -38889,7 +39400,7 @@
           <t>Mann und Frau sitzen auf einem Untersatz (Sattel). Hüftschnüre mit Kauris und roten Perlen.</t>
         </is>
       </c>
-      <c r="B253" s="3" t="inlineStr">
+      <c r="B253" t="inlineStr">
         <is>
           <t>Man and woman sit on a pedestal (saddle). Hip strings with cowries and red pearls.</t>
         </is>
@@ -38904,7 +39415,7 @@
           <t>Mantel für Kinder, aus dem Fell des Bisonkalbes (Geo Karteikarte )</t>
         </is>
       </c>
-      <c r="B254" s="3" t="inlineStr">
+      <c r="B254" t="inlineStr">
         <is>
           <t>Coat for children, from the fur of the bison calf (Geo index card)</t>
         </is>
@@ -38919,7 +39430,7 @@
           <t>Menschlicher Kopf mit einer flachen, durchbrochenen Kopfbedeckung. Grünliche Patina "Jägerstil"</t>
         </is>
       </c>
-      <c r="B255" s="3" t="inlineStr">
+      <c r="B255" t="inlineStr">
         <is>
           <t>Human head with a flat, openwork hat. Greenish patina "hunting style"</t>
         </is>
@@ -38934,7 +39445,7 @@
           <t>Mistkäfergesicht ist laut Dr. Koloß die Auskunft vom Schnitzer.</t>
         </is>
       </c>
-      <c r="B256" s="3" t="inlineStr">
+      <c r="B256" t="inlineStr">
         <is>
           <t>Dung beetle face is, according to Dr. Colossus the information from the carver.</t>
         </is>
@@ -38951,9 +39462,11 @@
 Eintrag im historischen Hauptkatalog: "Beil mit quergestellter langer schmaler Klinge. Stiel geschnitzt, am oberen Ende ein Kopf, in dessen Mund die Klinge steckt"</t>
         </is>
       </c>
-      <c r="B257" s="3" t="inlineStr">
-        <is>
-          <t>with a long, narrow blade, a handle Human head and foot Entry in the historical main catalog: "hatchet with a long, narrow blade, a handle, carved, a head at the top, the blade in the mouth of which"</t>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>with a long, narrow blade
+Stalk human head and foot
+Entry in the historical main catalog: "Hatchet with a long, narrow blade placed crosswise. Carved handle, at the upper end a head with the blade in the mouth"</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -38966,7 +39479,7 @@
           <t>Nackenstütze (kali) aus einem Stück. Nackenstützen stützten den Kopf des liegenden Mannes und schützten seine Frisur.</t>
         </is>
       </c>
-      <c r="B258" s="3" t="inlineStr">
+      <c r="B258" t="inlineStr">
         <is>
           <t>One-piece headrest (kali). Neck supports supported the lying man's head and protected his hairstyle.</t>
         </is>
@@ -38981,7 +39494,7 @@
           <t>Neben Truthähnen waren kleine haarlose Hunde die einzigen Haustiere in Mesoamerika. Ihr Fleisch galt als schmackhaft.</t>
         </is>
       </c>
-      <c r="B259" s="3" t="inlineStr">
+      <c r="B259" t="inlineStr">
         <is>
           <t>In addition to turkeys, small hairless dogs were the only pets in Mesoamerica. Their meat was considered tasty.</t>
         </is>
@@ -38996,7 +39509,7 @@
           <t>Optisch aufgeteilt in große schwarze und weiße Karos</t>
         </is>
       </c>
-      <c r="B260" s="3" t="inlineStr">
+      <c r="B260" t="inlineStr">
         <is>
           <t>Optically divided into large black and white checks</t>
         </is>
@@ -39011,7 +39524,7 @@
           <t>Paar Mokassins für Kinder, schwarz mit Perlen bestickt, mit bestickten Sohlen. (Dead man ´s Mocassins)</t>
         </is>
       </c>
-      <c r="B261" s="3" t="inlineStr">
+      <c r="B261" t="inlineStr">
         <is>
           <t>Pair of moccasins for children, black embroidered with pearls, with embroidered soles. (Dead man's moccasins)</t>
         </is>
@@ -39026,7 +39539,7 @@
           <t>Prunkaxt des Holo-Oberhauptes Tembo Aluma</t>
         </is>
       </c>
-      <c r="B262" s="3" t="inlineStr">
+      <c r="B262" t="inlineStr">
         <is>
           <t>Magnificent ax of the Holo head Tembo Aluma</t>
         </is>
@@ -39041,7 +39554,7 @@
           <t>Runder Tonanhänger; oben mittig Perforation für Kette; Vorderseite rundes geometrisches Muster in Schwarz, olivgrün und Ocker.</t>
         </is>
       </c>
-      <c r="B263" s="3" t="inlineStr">
+      <c r="B263" t="inlineStr">
         <is>
           <t>Round clay pendant; Perforation for chain in the middle; Front round geometric pattern in black, olive green and ocher.</t>
         </is>
@@ -39056,7 +39569,7 @@
           <t>Rundes Tontellerchen, innen bunt bemalt, mit runden und eckigen geometrischen Mustern, typ. Kadiweu-Mustern, versehen.</t>
         </is>
       </c>
-      <c r="B264" s="3" t="inlineStr">
+      <c r="B264" t="inlineStr">
         <is>
           <t>Round clay plate, brightly painted on the inside, with round and angular geometric patterns, typical Kadiweu patterns.</t>
         </is>
@@ -39071,7 +39584,7 @@
           <t>Schon die ersten Siedler der fidschianischen Inseln, die "Lapita-Leute",  besaßen bei ihrer Ankunft vor ca. 3000 Jahren Töpferwaren und das Wissen zu töpfern. Dieses Gefäß stammt aus dem 19. Jahrhundert. Zu dieser Zeit stellten Frauen aus den seefahrenden Klanen die Töpferware her. Das Wassergefäß besteht aus drei miteinander verbundenen Hohlkörpern. Die Form der Hohlkörper wird in der Literatur mit der Pottwalzahngabe (tabua), dem Bootsrumpf (cama) oder einer Banane (vudi) verglichen. Bananen sind in Fidschi hochangesehene Nahrungsmittel und Gaben. Um aus den Gefäßen zu trinken, wurden sie in die Höhe gehalten und der Wasserstrahl direkt in den Mund geleitet.</t>
         </is>
       </c>
-      <c r="B265" s="3" t="inlineStr">
+      <c r="B265" t="inlineStr">
         <is>
           <t>The first settlers of the Fijian Islands, the "Lapita people", had pottery and the knowledge of pottery when they arrived about 3000 years ago. This vessel dates from the 19th century. At that time, women made the pottery from the seafaring clans. The water vessel consists of three interconnected hollow bodies. The shape of the hollow body is compared in the literature with the sperm whale tooth (tabua), the boat hull (cama) or a banana (vudi). Bananas are highly regarded food and gifts in Fiji. In order to drink from the vessels, they were held up and the water jet was directed directly into the mouth.</t>
         </is>
@@ -39086,7 +39599,7 @@
           <t>Schon die ersten Siedler der fidschianischen Inseln, die "Lapita-Leute",  besaßen bei ihrer Ankunft vor ca. 3000 Jahren Töpferwaren und das Wissen zu töpfern. Dieses Gefäß stammt aus dem 19. Jahrhundert. Zu dieser Zeit stellten Frauen aus den seefahrenden Klanen die Töpferware her. Das Wassergefäß besteht aus fünf kugeligen miteinander verbundenen Hohlkörpern. Da diese Hohlkörper Zitrusfrüchten (moli) ähneln, werden solche Gefäße saqa moli genannt. Um aus den Gefäßen zu trinken, wurden sie in die Höhe gehalten und der Wasserstrahl direkt in den Mund geleitet.</t>
         </is>
       </c>
-      <c r="B266" s="3" t="inlineStr">
+      <c r="B266" t="inlineStr">
         <is>
           <t>The first settlers of the Fijian Islands, the "Lapita people", had pottery and the knowledge of pottery when they arrived about 3000 years ago. This vessel dates from the 19th century. At that time, women made the pottery from the seafaring clans. The water vessel consists of five spherical, interconnected hollow bodies. Since these hollow bodies resemble citrus fruits (moli), such vessels are called saqa moli. In order to drink from the vessels, they were held up and the water jet was directed directly into the mouth.</t>
         </is>
@@ -39101,7 +39614,7 @@
           <t>Schon die ersten Siedler der fidschianischen Inseln, die "Lapita-Leute",  besaßen bei ihrer Ankunft vor ca. 3000 Jahren Töpferwaren und das Wissen zu töpfern. Dieses Gefäß stammt aus dem 19. Jahrhundert. Zu dieser Zeit stellten Frauen aus den seefahrenden Klanen die Töpferware her. Das Wassergefäß besteht aus zwei kugeligen miteinander verbundenen Hohlkörpern. Da diese Hohlkörper Zitrusfrüchten (moli) ähneln, werden solche Gefäße saqa moli genannt. Um aus den Gefäßen zu trinken, wurden sie in die Höhe gehalten und der Wasserstrahl direkt in den Mund geleitet.</t>
         </is>
       </c>
-      <c r="B267" s="3" t="inlineStr">
+      <c r="B267" t="inlineStr">
         <is>
           <t>The first settlers of the Fijian Islands, the "Lapita people", had pottery and the knowledge of pottery when they arrived about 3000 years ago. This vessel dates from the 19th century. At that time, women made the pottery from the seafaring clans. The water vessel consists of two spherical hollow bodies connected together. Since these hollow bodies resemble citrus fruits (moli), such vessels are called saqa moli. In order to drink from the vessels, they were held up and the water jet was directed directly into the mouth.</t>
         </is>
@@ -39116,7 +39629,7 @@
           <t>Schon die ersten Siedler der fidschianischen Inseln, die "Lapita-Leute",  besaßen bei ihrer Ankunft vor ca. 3000 Jahren Töpferwaren und das Wissen zu töpfern. Dieses Gefäß stammt aus dem 19. Jahrhundert. Zu dieser Zeit stellten Frauen aus den seefahrenden Klanen die Töpferware her. Das Wassergefäß zeigt eine auf dem Rücken liegende Schildkröte - in der Position, in der sie auch bei Opferfesten dargebracht wurde. Schildkröten waren hochgeschätzte Tiere und Opfergaben und ein beliebtes Motiv in der Töpferei. Um aus den Gefäßen zu trinken, wurden sie in die Höhe gehalten und der Wasserstrahl direkt in den Mund geleitet.</t>
         </is>
       </c>
-      <c r="B268" s="3" t="inlineStr">
+      <c r="B268" t="inlineStr">
         <is>
           <t>The first settlers of the Fijian Islands, the "Lapita people", had pottery and the knowledge of pottery when they arrived about 3000 years ago. This vessel dates from the 19th century. At that time, women made the pottery from the seafaring clans. The water container shows a turtle lying on its back - in the position in which it was also offered at sacrificial festivals. Turtles were highly valued animals and offerings and a popular motif in pottery. In order to drink from the vessels, they were held up and the water jet was directed directly into the mouth.</t>
         </is>
@@ -39131,7 +39644,7 @@
           <t>Schritt 1</t>
         </is>
       </c>
-      <c r="B269" s="3" t="inlineStr">
+      <c r="B269" t="inlineStr">
         <is>
           <t>Step 1</t>
         </is>
@@ -39146,7 +39659,7 @@
           <t>Schritt 4</t>
         </is>
       </c>
-      <c r="B270" s="3" t="inlineStr">
+      <c r="B270" t="inlineStr">
         <is>
           <t>Step 4</t>
         </is>
@@ -39162,9 +39675,10 @@
 Eintrag im historischen Hauptkatalog: "Weibliche Wächterahnenmaske"</t>
         </is>
       </c>
-      <c r="B271" s="3" t="inlineStr">
-        <is>
-          <t>Black patina. White eye area, fastening straps over the forehead. Entry in the historical main catalog: "Female guardian mask"</t>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Black patina. White eye area, fastening straps over the forehead.
+Entry in the historical main catalog: "Female guardian mask"</t>
         </is>
       </c>
       <c r="D271" t="n">
@@ -39177,7 +39691,7 @@
           <t>Schwer, hohl, mit kugelartigen Verzierungen</t>
         </is>
       </c>
-      <c r="B272" s="3" t="inlineStr">
+      <c r="B272" t="inlineStr">
         <is>
           <t>Heavy, hollow, with spherical decorations</t>
         </is>
@@ -39192,9 +39706,9 @@
           <t>Thongefäß [dto. wie V A 983] mit Einkerbungen (Eintrag im historischen Hauptkatalog alt)</t>
         </is>
       </c>
-      <c r="B273" s="3" t="inlineStr">
-        <is>
-          <t>Clay pot [dto. like VA 983] with notches (entry in the historical main catalog old)</t>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Clay pot [dto. like V A 983] with notches (entry in the historical main catalog old)</t>
         </is>
       </c>
       <c r="D273" t="n">
@@ -39211,9 +39725,13 @@
 Eintrag im historischen Hauptkatalog: Topf aus Ton Tierfigur</t>
         </is>
       </c>
-      <c r="B274" s="3" t="inlineStr">
-        <is>
-          <t>Clay pot: animal figure (B) clay bowl made of black clay (W) Note (SK): probably turtle representation Catalog: pot made of clay, depicting an animal figure. Entry in the historical main catalog: Pot made of clay animal figure</t>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Clay pot: animal figure (B)
+Clay bowl made of black clay (W)
+Note (S.K.): probably representation of turtles
+Catalog: Pot made of clay, depicting an animal figure.
+Entry in the historical main catalog: Pot made of clay animal figure</t>
         </is>
       </c>
       <c r="D274" t="n">
@@ -39226,7 +39744,7 @@
           <t>Trinkbecher in gedrungener Frauengestalt. Steht auf kurzen Beinen. Mit Narbentatauierung</t>
         </is>
       </c>
-      <c r="B275" s="3" t="inlineStr">
+      <c r="B275" t="inlineStr">
         <is>
           <t>Drinking cup in a squat woman. Stands on short legs. With scar tissue</t>
         </is>
@@ -39243,9 +39761,11 @@
 Es ist nicht klar, ob sie je geraucht wurde. Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B276" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. It is decorated with an image of an elephant's head with magnificent tusks, narrow spirals and small metal balls. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century. It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. It is decorated with an image of an elephant's head with magnificent tusks, narrow spirals and small metal balls. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century.
+It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -39260,9 +39780,11 @@
 Es ist nicht klar, ob sie je geraucht wurde. Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B277" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. It is decorated with an image of a little bird and tight spirals. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century. It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. It is decorated with an image of a little bird and tight spirals. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century.
+It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -39278,9 +39800,12 @@
 Hauptkatalog: "Tabakspfeife, Kopf und Rohr aus Messing gegossen. Kopf mit 2 Reihen von Spiralen verziert, auf der vorderen Fläche sitzt ein Vogel, auf dem Knie ein aus Spiralen gebildeter hohler Kegel."</t>
         </is>
       </c>
-      <c r="B278" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. It is decorated with an illustration of a small bird, narrow spirals, and a hollow cone. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century. It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them. Main catalog: "Tobacco pipe, head and pipe cast from brass. Head decorated with 2 rows of spirals, a bird sits on the front surface, a hollow cone made of spirals on the knee."</t>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. It is decorated with an illustration of a small bird, narrow spirals, and a hollow cone. Despite its modest size, it shows the high level of casting and metal technology in the Kingdom of Bamum in the first years of the 20th century.
+It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.
+Main catalog: "Tobacco pipe, head and pipe cast from brass. Head decorated with 2 rows of spirals, a bird sits on the front surface, a hollow cone made of spirals on the knee."</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -39296,9 +39821,12 @@
 Hauptkatalog: "Tabakspfeife. Kopf und Rohr aus Messing gegossen, beide reich mit Spiralen verziert, letzteres auch mit Schnurmuster. Das Rohr besteht aus 2 Teilen, einem kürzerem dicken und einem längeren dünnen."</t>
         </is>
       </c>
-      <c r="B279" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. It is decorated with spirals and braids. It was made by artists in the Bamum kingdom in the early years of the 20th century. It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them. Main catalog: "Tobacco pipe. Head and tube made of brass, both richly decorated with spirals, the latter also with a cord pattern. The tube consists of 2 parts, a shorter thick and a longer thin."</t>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. It is decorated with spirals and braids. It was made by artists in the Bamum kingdom in the early years of the 20th century.
+It is not clear if it has ever been smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.
+Main catalog: "Tobacco pipe. Head and tube made of brass, both richly decorated with spirals, the latter also with a cord pattern. The tube consists of 2 parts, a shorter thick and a longer thin."</t>
         </is>
       </c>
       <c r="D279" t="n">
@@ -39315,9 +39843,13 @@
 Karteikarte  "Ähnelt europäischen Pfeifen in der Form. Pfeifenkopf: Portrait eines Europäers mit gezwirbelten Bart und Schildmütze. Unten sind 2 Messingkugeln angebracht. Pfeifenrohr und -kopf durch ein Holzstück (nicht sichtbar) verbunden. Am Pfeifenrohr ist ein Ring angegeossen."</t>
         </is>
       </c>
-      <c r="B280" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. They made artists in the Kingdom of Bamum in the early years of the 20th century. The pipe bowl represents the head of a European with a cap. Many tobacco pipe bowls from the Cameroon grasslands have the shape of human heads made of clay or brass. Smoking from the head of a person, especially from the head of a depicted ruler or dignitary, was presumably a sign of power and strength. Here, however, the head shown is not from a local ruler but from a European. The artist was probably trying to symbolically indicate that the smoker could also have power over the Europeans. It is not clear whether the price was ever smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them. Main catalog: "TAMTON tobacco pipe, head and pipe made of brass, stuck on a common short wooden pipe. Head in the form of a European head with a cap. A ring instead of a hook on the pipe." Index card "Similar in shape to European pipes. Pipe head: Portrait of a European with a whisked beard and shield cap. Two brass balls are attached below. Pipe pipe and head connected by a piece of wood (not visible). A ring is cast on the pipe pipe."</t>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. They made artists in the Kingdom of Bamum in the early years of the 20th century. The pipe bowl represents the head of a European with a cap. Many tobacco pipe bowls from the Cameroon grasslands have the shape of human heads made of clay or brass. Smoking from the head of a person, especially from the head of a depicted ruler or dignitary, was presumably a sign of power and strength. Here, however, the head shown is not from a local ruler but from a European. The artist was probably trying to symbolically indicate that the smoker could also have power over the Europeans.
+It is not clear whether the price was ever smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.
+Main catalog: "TAMTON tobacco pipe, head and tube made of brass, stuck on a common short wooden tube. Head in the form of a European head with a cap. A ring instead of a hook on the tube."
+"Similar to European pipes in shape. Pipe head: Portrait of a European with a whisked beard and a shield cap. Two brass balls are attached below. Pipe pipe and head are connected by a piece of wood (not visible). A ring is cast on the pipe pipe."</t>
         </is>
       </c>
       <c r="D280" t="n">
@@ -39333,9 +39865,12 @@
 Hauptkatalog: "TAMTON Tabakspfeife. Kopf und Rohr aus Messing auf einem gemeinsamen kurzen Holzrohr steckend. Kopf in Gestalt eines Europäerkopfes mit Mütze. Am Rohr hinten ein Haken"</t>
         </is>
       </c>
-      <c r="B281" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. They made artists in the Kingdom of Bamum in the early years of the 20th century. The pipe bowl represents the head of a European with a cap. Many tobacco pipe bowls from the Cameroon grasslands have the shape of human heads made of clay or brass. Smoking from the head of a person, especially from the head of a depicted ruler or dignitary, was presumably a sign of power and strength. Here, however, the head shown is not from a local ruler but from a European. The artist was probably trying to symbolically indicate that the smoker could also have power over the Europeans. It is not clear whether the price was ever smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them. Main catalog: "TAMTON tobacco pipe. Head and tube made of brass stuck on a common short wooden tube. Head in the form of a European head with a cap. A hook on the tube behind"</t>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. They made artists in the Kingdom of Bamum in the early years of the 20th century. The pipe bowl represents the head of a European with a cap. Many tobacco pipe bowls from the Cameroon grasslands have the shape of human heads made of clay or brass. Smoking from the head of a person, especially from the head of a depicted ruler or dignitary, was presumably a sign of power and strength. Here, however, the head shown is not from a local ruler but from a European. The artist was probably trying to symbolically indicate that the smoker could also have power over the Europeans.
+It is not clear whether the price was ever smoked. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.
+Main catalog: "TAMTON tobacco pipe. Head and tube made of brass stuck on a common short wooden tube. Head in the form of a European head with a cap. A hook on the tube behind"</t>
         </is>
       </c>
       <c r="D281" t="n">
@@ -39350,9 +39885,11 @@
 Um 1908 gab der Ethnologe Bernhard Ankermann (*1869 - †1943) während einer Forschungsreise nach Kamerun Dutzende von Tabakspfeifen bei lokalen Künstlern in Auftrag.  Er kaufte andere Pfeifen in lokalen Märkten. Sie waren unbenutzt als das damalige Königliche Museum für Völkerkunde sie erwarb.</t>
         </is>
       </c>
-      <c r="B282" s="3" t="inlineStr">
-        <is>
-          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be. This tobacco pipe is made of cast brass. It was made by artists in the Bamum kingdom in the early years of the 20th century. Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Around 1900 kings, dignitaries and heads of families liked to smoke tobacco in the grasslands of Cameroon. The higher the rank of the smoker, the more magnificent the pipe should be.
+This tobacco pipe is made of cast brass. It was made by artists in the Bamum kingdom in the early years of the 20th century.
+Around 1908, the ethnologist Bernhard Ankermann (* 1869 - † 1943) commissioned dozens of tobacco pipes from local artists during a research trip to Cameroon. He bought other pipes in local markets. They were unused when the then Royal Museum of Ethnology acquired them.</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -39367,9 +39904,11 @@
 Bedeutung: Ahne fordert vom Frager ein Opfer.KB-246/29</t>
         </is>
       </c>
-      <c r="B283" s="3" t="inlineStr">
-        <is>
-          <t>Fortune telling symbol A woman is sitting in a bowed pose. The elbows are supported on the knees and the chin is in the hands. Meaning: Ahne demands a sacrifice from the questioner. KB-246/29</t>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Fortune telling symbol
+A woman is sitting in a bowed pose. The elbows are supported on the knees and the chin is in the hands
+Meaning: Ahne demands a victim from the questioner. KB-246/29</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -39382,7 +39921,7 @@
           <t>Weibliche Ahnenmaske mit dunkelbrauner Patina.</t>
         </is>
       </c>
-      <c r="B284" s="3" t="inlineStr">
+      <c r="B284" t="inlineStr">
         <is>
           <t>Female ancestral mask with dark brown patina.</t>
         </is>
@@ -39397,7 +39936,7 @@
           <t>Zierkamm mit Menschenkopf, ornamentiert</t>
         </is>
       </c>
-      <c r="B285" s="3" t="inlineStr">
+      <c r="B285" t="inlineStr">
         <is>
           <t>Decorative comb with human head, ornamented</t>
         </is>
@@ -39412,7 +39951,7 @@
           <t>Zwei mit dem Rücken zueinanderstehende Frauen stehen auf einer runden Sockelplatte und tragen gemeinsam mit ausgestreckten Armen eine ebenfalls runde Sitzplatte über ihren Köpfen.</t>
         </is>
       </c>
-      <c r="B286" s="3" t="inlineStr">
+      <c r="B286" t="inlineStr">
         <is>
           <t>Two women standing with their backs to each other stand on a round base plate and, with their arms outstretched, carry a round seat plate above their heads.</t>
         </is>

</xml_diff>

<commit_message>
vindex, translate: went thru geogrBezug again
</commit_message>
<xml_diff>
--- a/data2/EM-SM/translate.xlsx
+++ b/data2/EM-SM/translate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="5" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="erwerbungsart" sheetId="1" state="visible" r:id="rId1"/>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -152,6 +152,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5911,18 +5914,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1114"/>
+  <dimension ref="A1:E1116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A871" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A883" sqref="A883"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="24" customWidth="1" style="3" min="1" max="1"/>
-    <col width="20.7109375" customWidth="1" style="10" min="2" max="2"/>
-    <col width="14.140625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="30.7109375" customWidth="1" style="3" min="1" max="1"/>
+    <col width="27.7109375" customWidth="1" style="10" min="2" max="2"/>
+    <col width="38" customWidth="1" style="3" min="3" max="3"/>
     <col width="13.7109375" customWidth="1" style="11" min="4" max="4"/>
     <col width="31.140625" customWidth="1" style="3" min="5" max="5"/>
   </cols>
@@ -8446,7 +8449,7 @@
           <t>Demokratische Republik Kongo</t>
         </is>
       </c>
-      <c r="B234" s="12" t="inlineStr">
+      <c r="B234" s="22" t="inlineStr">
         <is>
           <t>Democratic Republic of the Congo</t>
         </is>
@@ -9716,7 +9719,7 @@
           <t>Hochland von Guatemala</t>
         </is>
       </c>
-      <c r="B348" s="12" t="inlineStr">
+      <c r="B348" s="22" t="inlineStr">
         <is>
           <t>Guatemalan Highlands</t>
         </is>
@@ -12161,7 +12164,7 @@
           <t>Marianen</t>
         </is>
       </c>
-      <c r="B573" s="12" t="inlineStr">
+      <c r="B573" s="22" t="inlineStr">
         <is>
           <t>Mariana Islands</t>
         </is>
@@ -12981,7 +12984,7 @@
           <t>Moçambique</t>
         </is>
       </c>
-      <c r="B646" s="12" t="inlineStr">
+      <c r="B646" s="22" t="inlineStr">
         <is>
           <t>Mozambique</t>
         </is>
@@ -15154,7 +15157,7 @@
           <t>Republik Kongo</t>
         </is>
       </c>
-      <c r="B827" s="12" t="inlineStr">
+      <c r="B827" s="22" t="inlineStr">
         <is>
           <t>Republic of the Congo</t>
         </is>
@@ -15673,15 +15676,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="875" ht="90" customHeight="1" s="11">
+    <row r="875" ht="91.5" customHeight="1" s="11">
       <c r="A875" s="3" t="inlineStr">
         <is>
           <t>Santa Barbara</t>
         </is>
       </c>
+      <c r="B875" s="3" t="n"/>
       <c r="C875" s="3" t="inlineStr">
         <is>
-          <t>Wir sollten uns einig werden, wie mit Diakritika umzugehen ist.</t>
+          <t xml:space="preserve"> Diakritika sind erlaubt und wir hoffen, dass Search Enginge diese auch ohne findet. Es gibt ein Santa Barbara (z.B. in Kalifornien) und ein Santa Bárbara in Boliviren. Also kann man hier nichts automatisiert ersetzen</t>
         </is>
       </c>
       <c r="D875" t="n">
@@ -15694,6 +15698,11 @@
           <t>Santa Bárbara</t>
         </is>
       </c>
+      <c r="C876" s="3" t="inlineStr">
+        <is>
+          <t>vgl. Santa Barbara</t>
+        </is>
+      </c>
       <c r="D876" t="n">
         <v>26</v>
       </c>
@@ -15951,27 +15960,43 @@
     <row r="898" ht="30" customHeight="1" s="11">
       <c r="A898" s="3" t="inlineStr">
         <is>
-          <t>Simbai-Tal</t>
-        </is>
-      </c>
+          <t>Simbabwe</t>
+        </is>
+      </c>
+      <c r="B898" s="10" t="inlineStr">
+        <is>
+          <t>Zimbabwe</t>
+        </is>
+      </c>
+      <c r="C898" s="3" t="n"/>
       <c r="D898" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E898" s="3" t="inlineStr">
+        <is>
+          <t>AA, wikipedia</t>
+        </is>
       </c>
     </row>
     <row r="899" ht="30" customHeight="1" s="11">
       <c r="A899" s="3" t="inlineStr">
         <is>
+          <t>Simbai-Tal</t>
+        </is>
+      </c>
+      <c r="B899" s="10" t="inlineStr">
+        <is>
+          <t>Simbai-Valley</t>
+        </is>
+      </c>
+      <c r="D899" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="900" ht="30" customHeight="1" s="11">
+      <c r="A900" s="3" t="inlineStr">
+        <is>
           <t>Simbang</t>
-        </is>
-      </c>
-      <c r="D899" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="900">
-      <c r="A900" s="3" t="inlineStr">
-        <is>
-          <t>Simbo</t>
         </is>
       </c>
       <c r="D900" t="n">
@@ -15981,207 +16006,207 @@
     <row r="901">
       <c r="A901" s="3" t="inlineStr">
         <is>
-          <t>Simbu-Tal</t>
-        </is>
-      </c>
-      <c r="B901" s="10" t="inlineStr">
-        <is>
-          <t>Simbu-Valley</t>
+          <t>Simbo</t>
         </is>
       </c>
       <c r="D901" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="902">
       <c r="A902" s="3" t="inlineStr">
         <is>
-          <t>Sinasina</t>
+          <t>Simbu-Tal</t>
+        </is>
+      </c>
+      <c r="B902" s="10" t="inlineStr">
+        <is>
+          <t>Simbu-Valley</t>
         </is>
       </c>
       <c r="D902" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="903">
       <c r="A903" s="3" t="inlineStr">
         <is>
-          <t>Sioux</t>
+          <t>Sinasina</t>
         </is>
       </c>
       <c r="D903" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="904">
       <c r="A904" s="3" t="inlineStr">
         <is>
-          <t>Sioux (?)</t>
+          <t>Sioux</t>
         </is>
       </c>
       <c r="D904" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="905">
       <c r="A905" s="3" t="inlineStr">
         <is>
-          <t>Siusi</t>
+          <t>Sioux (?)</t>
         </is>
       </c>
       <c r="D905" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="906">
       <c r="A906" s="3" t="inlineStr">
         <is>
+          <t>Siusi</t>
+        </is>
+      </c>
+      <c r="D906" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="3" t="inlineStr">
+        <is>
           <t>Siusi (Baniwa)</t>
         </is>
       </c>
-      <c r="D906" t="n">
+      <c r="D907" t="n">
         <v>11</v>
-      </c>
-    </row>
-    <row r="907" ht="30" customHeight="1" s="11">
-      <c r="A907" s="3" t="inlineStr">
-        <is>
-          <t>Sklavenküste (Diego Cao)</t>
-        </is>
-      </c>
-      <c r="B907" t="inlineStr">
-        <is>
-          <t>Diego Cao</t>
-        </is>
-      </c>
-      <c r="D907" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="908" ht="30" customHeight="1" s="11">
       <c r="A908" s="3" t="inlineStr">
         <is>
-          <t>Songe</t>
+          <t>Sklavenküste (Diego Cao)</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Diego Cao</t>
         </is>
       </c>
       <c r="D908" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="909" ht="30" customHeight="1" s="11">
       <c r="A909" s="3" t="inlineStr">
         <is>
-          <t>Songo</t>
+          <t>Songe</t>
         </is>
       </c>
       <c r="D909" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="910" ht="30" customHeight="1" s="11">
       <c r="A910" s="3" t="inlineStr">
         <is>
-          <t>Songwe</t>
+          <t>Songo</t>
         </is>
       </c>
       <c r="D910" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="911" ht="30" customHeight="1" s="11">
       <c r="A911" s="3" t="inlineStr">
         <is>
-          <t>Songye</t>
+          <t>Songwe</t>
         </is>
       </c>
       <c r="D911" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="912" ht="30" customHeight="1" s="11">
       <c r="A912" s="3" t="inlineStr">
         <is>
+          <t>Songye</t>
+        </is>
+      </c>
+      <c r="D912" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="913" ht="30" customHeight="1" s="11">
+      <c r="A913" s="3" t="inlineStr">
+        <is>
           <t>Songye (?)</t>
         </is>
       </c>
-      <c r="D912" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="913">
-      <c r="A913" s="3" t="inlineStr">
+      <c r="D913" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="3" t="inlineStr">
         <is>
           <t>Songye (Bassonge)</t>
         </is>
       </c>
-      <c r="D913" t="n">
+      <c r="D914" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="914" ht="30" customHeight="1" s="11">
-      <c r="A914" s="3" t="inlineStr">
+    <row r="915" ht="30" customHeight="1" s="11">
+      <c r="A915" s="3" t="inlineStr">
         <is>
           <t>Sonserol</t>
         </is>
       </c>
-      <c r="D914" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="915">
-      <c r="A915" s="3" t="inlineStr">
+      <c r="C915" s="3" t="inlineStr">
+        <is>
+          <t>vgl. Sonsorol</t>
+        </is>
+      </c>
+      <c r="D915" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="3" t="inlineStr">
         <is>
           <t>Sonsorol</t>
         </is>
       </c>
-      <c r="D915" t="n">
+      <c r="D916" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="916" ht="30" customHeight="1" s="11">
-      <c r="A916" s="3" t="inlineStr">
+    <row r="917" ht="30" customHeight="1" s="11">
+      <c r="A917" s="3" t="inlineStr">
         <is>
           <t>Sswahili Küste</t>
         </is>
       </c>
-      <c r="B916" s="10" t="inlineStr">
+      <c r="B917" s="10" t="inlineStr">
         <is>
           <t>Swahili Coast</t>
         </is>
       </c>
-      <c r="C916" s="3" t="inlineStr">
+      <c r="C917" s="3" t="inlineStr">
         <is>
           <t>upstream korrigieren</t>
         </is>
       </c>
-      <c r="D916" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="917">
-      <c r="A917" s="3" t="inlineStr">
+      <c r="D917" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="3" t="inlineStr">
         <is>
           <t>Sta. Barbara</t>
         </is>
       </c>
-      <c r="B917" s="10" t="inlineStr">
+      <c r="B918" s="10" t="inlineStr">
         <is>
           <t>Santa Barbara</t>
-        </is>
-      </c>
-      <c r="D917" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="918" ht="30" customHeight="1" s="11">
-      <c r="A918" s="3" t="inlineStr">
-        <is>
-          <t>Sta. Cruz</t>
-        </is>
-      </c>
-      <c r="B918" s="10" t="inlineStr">
-        <is>
-          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C918" s="3" t="inlineStr">
@@ -16193,20 +16218,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="919">
+    <row r="919" ht="30" customHeight="1" s="11">
       <c r="A919" s="3" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Sta. Cruz</t>
+        </is>
+      </c>
+      <c r="B919" s="10" t="inlineStr">
+        <is>
+          <t>Santa Cruz</t>
+        </is>
+      </c>
+      <c r="C919" s="3" t="inlineStr">
+        <is>
+          <t>keine Abkürzungen</t>
         </is>
       </c>
       <c r="D919" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="920">
       <c r="A920" s="3" t="inlineStr">
         <is>
-          <t>Suchitepequez</t>
+          <t>Strong</t>
         </is>
       </c>
       <c r="D920" t="n">
@@ -16216,12 +16251,7 @@
     <row r="921">
       <c r="A921" s="3" t="inlineStr">
         <is>
-          <t>Sud</t>
-        </is>
-      </c>
-      <c r="C921" s="3" t="inlineStr">
-        <is>
-          <t>?</t>
+          <t>Suchitepequez</t>
         </is>
       </c>
       <c r="D921" t="n">
@@ -16231,127 +16261,127 @@
     <row r="922">
       <c r="A922" s="3" t="inlineStr">
         <is>
+          <t>Sud</t>
+        </is>
+      </c>
+      <c r="C922" s="3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D922" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="3" t="inlineStr">
+        <is>
           <t>Sudan</t>
         </is>
       </c>
-      <c r="D922" t="n">
+      <c r="D923" t="n">
         <v>44</v>
-      </c>
-    </row>
-    <row r="923" ht="30" customHeight="1" s="11">
-      <c r="A923" s="3" t="inlineStr">
-        <is>
-          <t>Suku</t>
-        </is>
-      </c>
-      <c r="D923" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="924" ht="30" customHeight="1" s="11">
       <c r="A924" s="3" t="inlineStr">
         <is>
+          <t>Suku</t>
+        </is>
+      </c>
+      <c r="D924" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="925" ht="30" customHeight="1" s="11">
+      <c r="A925" s="3" t="inlineStr">
+        <is>
           <t>Sukuma Gogo?</t>
         </is>
       </c>
-      <c r="D924" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="925">
-      <c r="A925" s="3" t="inlineStr">
-        <is>
-          <t>Sumbe</t>
-        </is>
-      </c>
       <c r="D925" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="926">
       <c r="A926" s="3" t="inlineStr">
         <is>
-          <t>Sumpango</t>
+          <t>Sumbe</t>
         </is>
       </c>
       <c r="D926" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="927">
       <c r="A927" s="3" t="inlineStr">
         <is>
-          <t>Suyá</t>
+          <t>Sumpango</t>
         </is>
       </c>
       <c r="D927" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="928">
       <c r="A928" s="3" t="inlineStr">
         <is>
+          <t>Suyá</t>
+        </is>
+      </c>
+      <c r="D928" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="3" t="inlineStr">
+        <is>
           <t>Swahili</t>
         </is>
       </c>
-      <c r="D928" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="929" ht="30" customHeight="1" s="11">
-      <c r="A929" s="3" t="inlineStr">
+      <c r="D929" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="930" ht="30" customHeight="1" s="11">
+      <c r="A930" s="3" t="inlineStr">
         <is>
           <t>Swahili-Küste</t>
         </is>
       </c>
-      <c r="B929" s="10" t="inlineStr">
+      <c r="B930" s="10" t="inlineStr">
         <is>
           <t>Swahili Coast</t>
         </is>
       </c>
-      <c r="D929" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="930">
-      <c r="A930" s="3" t="inlineStr">
+      <c r="D930" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="3" t="inlineStr">
         <is>
           <t>Süd-Chiapas</t>
         </is>
       </c>
-      <c r="B930" s="10" t="inlineStr">
+      <c r="B931" s="10" t="inlineStr">
         <is>
           <t>southern Chiapas</t>
         </is>
       </c>
-      <c r="D930" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="931" ht="30" customHeight="1" s="11">
-      <c r="A931" s="3" t="inlineStr">
-        <is>
-          <t>Süd-Malekula</t>
-        </is>
-      </c>
-      <c r="B931" s="10" t="inlineStr">
-        <is>
-          <t>southern Malekula</t>
-        </is>
-      </c>
       <c r="D931" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="932" ht="30" customHeight="1" s="11">
       <c r="A932" s="3" t="inlineStr">
         <is>
-          <t>Süd-Neubritannien</t>
+          <t>Süd-Malekula</t>
         </is>
       </c>
       <c r="B932" s="10" t="inlineStr">
         <is>
-          <t>Southern New Britain</t>
+          <t>southern Malekula</t>
         </is>
       </c>
       <c r="D932" t="n">
@@ -16361,27 +16391,27 @@
     <row r="933" ht="30" customHeight="1" s="11">
       <c r="A933" s="3" t="inlineStr">
         <is>
-          <t>Süd-Neuirland</t>
+          <t>Süd-Neubritannien</t>
         </is>
       </c>
       <c r="B933" s="10" t="inlineStr">
         <is>
-          <t>southern New Ireland</t>
+          <t>Southern New Britain</t>
         </is>
       </c>
       <c r="D933" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="934" ht="30" customHeight="1" s="11">
       <c r="A934" s="3" t="inlineStr">
         <is>
-          <t>Süd-Pare</t>
+          <t>Süd-Neuirland</t>
         </is>
       </c>
       <c r="B934" s="10" t="inlineStr">
         <is>
-          <t>South Pare</t>
+          <t>southern New Ireland</t>
         </is>
       </c>
       <c r="D934" t="n">
@@ -16391,132 +16421,137 @@
     <row r="935" ht="30" customHeight="1" s="11">
       <c r="A935" s="3" t="inlineStr">
         <is>
-          <t>Süd-Sudan</t>
+          <t>Süd-Pare</t>
         </is>
       </c>
       <c r="B935" s="10" t="inlineStr">
         <is>
-          <t>South Sudan</t>
+          <t>South Pare</t>
         </is>
       </c>
       <c r="D935" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="936" ht="30" customHeight="1" s="11">
       <c r="A936" s="3" t="inlineStr">
         <is>
-          <t>Süd-Usaramo</t>
+          <t>Süd-Sudan</t>
         </is>
       </c>
       <c r="B936" s="10" t="inlineStr">
         <is>
-          <t>South Usaramo</t>
+          <t>South Sudan</t>
         </is>
       </c>
       <c r="D936" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="937" ht="30" customHeight="1" s="11">
       <c r="A937" s="3" t="inlineStr">
         <is>
-          <t>Südafrika</t>
+          <t>Süd-Usaramo</t>
         </is>
       </c>
       <c r="B937" s="10" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>South Usaramo</t>
         </is>
       </c>
       <c r="D937" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="938" ht="30" customHeight="1" s="11">
       <c r="A938" s="3" t="inlineStr">
         <is>
-          <t>Südliche Cheyenne</t>
+          <t>Südafrika</t>
         </is>
       </c>
       <c r="B938" s="10" t="inlineStr">
         <is>
-          <t>Southern Cheyenne</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="D938" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="939" ht="30" customHeight="1" s="11">
       <c r="A939" s="3" t="inlineStr">
         <is>
-          <t>südliches Chiapas</t>
+          <t>Südliche Cheyenne</t>
         </is>
       </c>
       <c r="B939" s="10" t="inlineStr">
         <is>
-          <t>Southern Chiapas</t>
+          <t>Southern Cheyenne</t>
         </is>
       </c>
       <c r="D939" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="940" ht="30" customHeight="1" s="11">
       <c r="A940" s="3" t="inlineStr">
         <is>
-          <t>Südost-Neuguinea</t>
+          <t>südliches Chiapas</t>
         </is>
       </c>
       <c r="B940" s="10" t="inlineStr">
         <is>
-          <t>Southeast New Guinea</t>
+          <t>Southern Chiapas</t>
         </is>
       </c>
       <c r="D940" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="941" ht="30" customHeight="1" s="11">
       <c r="A941" s="3" t="inlineStr">
         <is>
-          <t>Südwest-Sudan</t>
+          <t>Südost-Neuguinea</t>
         </is>
       </c>
       <c r="B941" s="10" t="inlineStr">
         <is>
-          <t>Southwest Sudan</t>
+          <t>Southeast New Guinea</t>
         </is>
       </c>
       <c r="D941" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="942" ht="30" customHeight="1" s="11">
       <c r="A942" s="3" t="inlineStr">
         <is>
-          <t>Südwestnigeria</t>
+          <t>Südwest-Sudan</t>
         </is>
       </c>
       <c r="B942" s="10" t="inlineStr">
         <is>
-          <t>Southwest Nigeria</t>
+          <t>Southwest Sudan</t>
         </is>
       </c>
       <c r="D942" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="943" ht="30" customHeight="1" s="11">
       <c r="A943" s="3" t="inlineStr">
         <is>
-          <t>südöstlich Edmonton</t>
+          <t>Südwestnigeria</t>
         </is>
       </c>
       <c r="B943" s="10" t="inlineStr">
         <is>
-          <t>Southeast of Edmonton</t>
+          <t>Southwest Nigeria</t>
+        </is>
+      </c>
+      <c r="C943" s="3" t="inlineStr">
+        <is>
+          <t>upstream soll Südwest-Nigeria sein</t>
         </is>
       </c>
       <c r="D943" t="n">
@@ -16526,402 +16561,419 @@
     <row r="944" ht="30" customHeight="1" s="11">
       <c r="A944" s="3" t="inlineStr">
         <is>
+          <t>Südwest-Nigeria</t>
+        </is>
+      </c>
+      <c r="B944" s="10" t="inlineStr">
+        <is>
+          <t>Southwest Nigeria</t>
+        </is>
+      </c>
+      <c r="C944" s="3" t="n"/>
+      <c r="D944" t="n">
+        <v>0</v>
+      </c>
+      <c r="E944" s="3" t="n"/>
+    </row>
+    <row r="945" ht="30" customHeight="1" s="11">
+      <c r="A945" s="3" t="inlineStr">
+        <is>
+          <t>südöstlich Edmonton</t>
+        </is>
+      </c>
+      <c r="B945" s="10" t="inlineStr">
+        <is>
+          <t>Southeast of Edmonton</t>
+        </is>
+      </c>
+      <c r="D945" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="946" ht="30" customHeight="1" s="11">
+      <c r="A946" s="3" t="inlineStr">
+        <is>
           <t>Tabitenen</t>
         </is>
       </c>
-      <c r="D944" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="945">
-      <c r="A945" s="3" t="inlineStr">
+      <c r="D946" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="3" t="inlineStr">
         <is>
           <t>Tabiteuea</t>
         </is>
       </c>
-      <c r="D945" t="n">
+      <c r="D947" t="n">
         <v>12</v>
-      </c>
-    </row>
-    <row r="946">
-      <c r="A946" s="3" t="inlineStr">
-        <is>
-          <t>Tableland</t>
-        </is>
-      </c>
-      <c r="D946" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="947" ht="30" customHeight="1" s="11">
-      <c r="A947" s="3" t="inlineStr">
-        <is>
-          <t>Tableland am Fortescue River</t>
-        </is>
-      </c>
-      <c r="C947" s="3" t="inlineStr">
-        <is>
-          <t>upstream korrigieren</t>
-        </is>
-      </c>
-      <c r="D947" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="948">
       <c r="A948" s="3" t="inlineStr">
         <is>
+          <t>Tableland</t>
+        </is>
+      </c>
+      <c r="D948" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="949" ht="30" customHeight="1" s="11">
+      <c r="A949" s="3" t="inlineStr">
+        <is>
+          <t>Tableland am Fortescue River</t>
+        </is>
+      </c>
+      <c r="B949" s="3" t="inlineStr">
+        <is>
+          <t>Tableland, Fortescue River</t>
+        </is>
+      </c>
+      <c r="C949" s="3" t="inlineStr">
+        <is>
+          <t>upstream korrigieren</t>
+        </is>
+      </c>
+      <c r="D949" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="3" t="inlineStr">
+        <is>
           <t>Taboga</t>
         </is>
       </c>
-      <c r="D948" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="949">
-      <c r="A949" s="3" t="inlineStr">
-        <is>
-          <t>Tabora (Tansania)</t>
-        </is>
-      </c>
-      <c r="B949" s="3" t="inlineStr">
-        <is>
-          <t>Tabora (Tanzania)</t>
-        </is>
-      </c>
-      <c r="D949" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="950" ht="30" customHeight="1" s="11">
-      <c r="A950" s="3" t="inlineStr">
-        <is>
-          <t>Tabuai</t>
-        </is>
-      </c>
       <c r="D950" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="951">
       <c r="A951" s="3" t="inlineStr">
         <is>
-          <t>Tabwa</t>
+          <t>Tabora (Tansania)</t>
+        </is>
+      </c>
+      <c r="B951" s="3" t="inlineStr">
+        <is>
+          <t>Tabora (Tanzania)</t>
         </is>
       </c>
       <c r="D951" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="952" ht="30" customHeight="1" s="11">
+      <c r="A952" s="3" t="inlineStr">
+        <is>
+          <t>Tabuai</t>
+        </is>
+      </c>
+      <c r="D952" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="952">
-      <c r="A952" s="10" t="inlineStr">
-        <is>
-          <t>Tahauku</t>
-        </is>
-      </c>
-      <c r="D952" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="953">
       <c r="A953" s="3" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Tabwa</t>
         </is>
       </c>
       <c r="D953" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="954" ht="45" customHeight="1" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="954">
       <c r="A954" s="10" t="inlineStr">
         <is>
-          <t>Tahuata</t>
+          <t>Tahauku</t>
         </is>
       </c>
       <c r="D954" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="955">
       <c r="A955" s="3" t="inlineStr">
         <is>
-          <t>Taku</t>
+          <t>Tahiti</t>
         </is>
       </c>
       <c r="D955" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="956" ht="30" customHeight="1" s="11">
-      <c r="A956" s="3" t="inlineStr">
-        <is>
-          <t>Talim</t>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="956" ht="45" customHeight="1" s="11">
+      <c r="A956" s="10" t="inlineStr">
+        <is>
+          <t>Tahuata</t>
         </is>
       </c>
       <c r="D956" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="957">
       <c r="A957" s="3" t="inlineStr">
         <is>
-          <t>Tami</t>
+          <t>Taku</t>
         </is>
       </c>
       <c r="D957" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="958">
-      <c r="A958" s="10" t="inlineStr">
-        <is>
-          <t>Tami-Inseln</t>
-        </is>
-      </c>
-      <c r="B958" s="10" t="inlineStr">
-        <is>
-          <t>Tami</t>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="958" ht="30" customHeight="1" s="11">
+      <c r="A958" s="3" t="inlineStr">
+        <is>
+          <t>Talim</t>
         </is>
       </c>
       <c r="D958" t="n">
-        <v>7</v>
-      </c>
-      <c r="E958" s="3" t="inlineStr">
-        <is>
-          <t>wikipedia</t>
-        </is>
+        <v>2</v>
       </c>
     </row>
     <row r="959">
       <c r="A959" s="3" t="inlineStr">
         <is>
+          <t>Tami</t>
+        </is>
+      </c>
+      <c r="D959" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="10" t="inlineStr">
+        <is>
+          <t>Tami-Inseln</t>
+        </is>
+      </c>
+      <c r="B960" s="10" t="inlineStr">
+        <is>
+          <t>Tami</t>
+        </is>
+      </c>
+      <c r="D960" t="n">
+        <v>7</v>
+      </c>
+      <c r="E960" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="3" t="inlineStr">
+        <is>
           <t>Tanaeang</t>
         </is>
       </c>
-      <c r="D959" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="960" ht="30" customHeight="1" s="11">
-      <c r="A960" s="3" t="inlineStr">
+      <c r="D961" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="962" ht="30" customHeight="1" s="11">
+      <c r="A962" s="3" t="inlineStr">
         <is>
           <t>Tanapag</t>
         </is>
       </c>
-      <c r="D960" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="961">
-      <c r="A961" s="10" t="inlineStr">
+      <c r="D962" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="10" t="inlineStr">
         <is>
           <t>Tanga</t>
         </is>
       </c>
-      <c r="D961" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="962">
-      <c r="A962" s="3" t="inlineStr">
+      <c r="D963" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="3" t="inlineStr">
         <is>
           <t>Tanganyikasee</t>
         </is>
       </c>
-      <c r="B962" s="10" t="inlineStr">
+      <c r="B964" s="10" t="inlineStr">
         <is>
           <t>Lake Tanganyika</t>
         </is>
       </c>
-      <c r="D962" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="963" ht="30" customHeight="1" s="11">
-      <c r="A963" s="10" t="inlineStr">
+      <c r="D964" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="965" ht="30" customHeight="1" s="11">
+      <c r="A965" s="10" t="inlineStr">
         <is>
           <t>Tanganyikasee/Kivusee</t>
         </is>
       </c>
-      <c r="B963" s="10" t="inlineStr">
+      <c r="B965" s="10" t="inlineStr">
         <is>
           <t>Lake Tanganyika/Lake Kivu</t>
         </is>
       </c>
-      <c r="D963" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="964" ht="30" customHeight="1" s="11">
-      <c r="A964" s="3" t="inlineStr">
-        <is>
-          <t>Tansania</t>
-        </is>
-      </c>
-      <c r="B964" s="10" t="inlineStr">
-        <is>
-          <t>Tanzania</t>
-        </is>
-      </c>
-      <c r="D964" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="965">
-      <c r="A965" s="3" t="inlineStr">
-        <is>
-          <t>Taui</t>
-        </is>
-      </c>
       <c r="D965" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="966" ht="30" customHeight="1" s="11">
       <c r="A966" s="3" t="inlineStr">
         <is>
+          <t>Tansania</t>
+        </is>
+      </c>
+      <c r="B966" s="10" t="inlineStr">
+        <is>
+          <t>Tanzania</t>
+        </is>
+      </c>
+      <c r="D966" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="3" t="inlineStr">
+        <is>
+          <t>Taui</t>
+        </is>
+      </c>
+      <c r="D967" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="968" ht="30" customHeight="1" s="11">
+      <c r="A968" s="3" t="inlineStr">
+        <is>
           <t>Taungaeka</t>
         </is>
       </c>
-      <c r="D966" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="967">
-      <c r="A967" s="10" t="inlineStr">
+      <c r="D968" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="10" t="inlineStr">
         <is>
           <t>Tawa</t>
         </is>
       </c>
-      <c r="D967" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="968" ht="30" customHeight="1" s="11">
-      <c r="A968" s="10" t="inlineStr">
+      <c r="D969" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="970" ht="30" customHeight="1" s="11">
+      <c r="A970" s="10" t="inlineStr">
         <is>
           <t>Tecomavaca</t>
         </is>
       </c>
-      <c r="D968" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="969" ht="30" customHeight="1" s="11">
-      <c r="A969" s="3" t="inlineStr">
+      <c r="D970" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="971" ht="30" customHeight="1" s="11">
+      <c r="A971" s="3" t="inlineStr">
         <is>
           <t>Temao</t>
         </is>
       </c>
-      <c r="D969" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="970">
-      <c r="A970" s="10" t="inlineStr">
+      <c r="D971" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="10" t="inlineStr">
         <is>
           <t>Tembo Aluma</t>
         </is>
       </c>
-      <c r="D970" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="971">
-      <c r="A971" s="3" t="inlineStr">
+      <c r="D972" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="3" t="inlineStr">
         <is>
           <t>Teotitlan del Camino</t>
         </is>
       </c>
-      <c r="D971" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="972">
-      <c r="A972" s="3" t="inlineStr">
+      <c r="D973" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="3" t="inlineStr">
         <is>
           <t>Tepe</t>
         </is>
       </c>
-      <c r="D972" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="973" ht="30" customHeight="1" s="11">
-      <c r="A973" s="3" t="inlineStr">
-        <is>
-          <t>Terena</t>
-        </is>
-      </c>
-      <c r="D973" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="974">
-      <c r="A974" s="10" t="inlineStr">
-        <is>
-          <t>Terena (Tereno)</t>
-        </is>
-      </c>
       <c r="D974" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="975" ht="30" customHeight="1" s="11">
       <c r="A975" s="3" t="inlineStr">
         <is>
+          <t>Terena</t>
+        </is>
+      </c>
+      <c r="D975" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="10" t="inlineStr">
+        <is>
+          <t>Terena (Tereno)</t>
+        </is>
+      </c>
+      <c r="D976" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="977" ht="30" customHeight="1" s="11">
+      <c r="A977" s="3" t="inlineStr">
+        <is>
           <t>Teton-Sioux (Oglala, Ojilala)</t>
         </is>
       </c>
-      <c r="D975" t="n">
+      <c r="D977" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="976" ht="30" customHeight="1" s="11">
-      <c r="A976" s="3" t="inlineStr">
+    <row r="978" ht="30" customHeight="1" s="11">
+      <c r="A978" s="3" t="inlineStr">
         <is>
           <t>Tetua</t>
         </is>
       </c>
-      <c r="D976" t="n">
+      <c r="D978" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="977" ht="30" customHeight="1" s="11">
-      <c r="A977" s="10" t="inlineStr">
+    <row r="979" ht="30" customHeight="1" s="11">
+      <c r="A979" s="10" t="inlineStr">
         <is>
           <t>Tikuna (Tukuna)</t>
         </is>
       </c>
-      <c r="D977" t="n">
+      <c r="D979" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="978">
-      <c r="A978" s="3" t="inlineStr">
-        <is>
-          <t>Timboon</t>
-        </is>
-      </c>
-      <c r="D978" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="979">
-      <c r="A979" s="10" t="inlineStr">
-        <is>
-          <t>Tinian</t>
-        </is>
-      </c>
-      <c r="D979" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="980">
       <c r="A980" s="3" t="inlineStr">
         <is>
-          <t>Toba</t>
+          <t>Timboon</t>
         </is>
       </c>
       <c r="D980" t="n">
@@ -16929,44 +16981,39 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="3" t="inlineStr">
-        <is>
-          <t>Tobi</t>
+      <c r="A981" s="10" t="inlineStr">
+        <is>
+          <t>Tinian</t>
         </is>
       </c>
       <c r="D981" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="982">
       <c r="A982" s="3" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Toba</t>
         </is>
       </c>
       <c r="D982" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="983">
       <c r="A983" s="3" t="inlineStr">
         <is>
-          <t>Tonga</t>
+          <t>Tobi</t>
         </is>
       </c>
       <c r="D983" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="10" t="inlineStr">
-        <is>
-          <t>Torres Straße</t>
-        </is>
-      </c>
-      <c r="B984" s="10" t="inlineStr">
-        <is>
-          <t>Torres Strait</t>
+      <c r="A984" s="3" t="inlineStr">
+        <is>
+          <t>Togo</t>
         </is>
       </c>
       <c r="D984" t="n">
@@ -16976,27 +17023,32 @@
     <row r="985">
       <c r="A985" s="3" t="inlineStr">
         <is>
+          <t>Tonga</t>
+        </is>
+      </c>
+      <c r="D985" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="10" t="inlineStr">
+        <is>
+          <t>Torres Straße</t>
+        </is>
+      </c>
+      <c r="B986" s="10" t="inlineStr">
+        <is>
+          <t>Torres Strait</t>
+        </is>
+      </c>
+      <c r="D986" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="3" t="inlineStr">
+        <is>
           <t>Torua</t>
-        </is>
-      </c>
-      <c r="D985" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="986">
-      <c r="A986" s="3" t="inlineStr">
-        <is>
-          <t>Totonicapan</t>
-        </is>
-      </c>
-      <c r="D986" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="987">
-      <c r="A987" s="10" t="inlineStr">
-        <is>
-          <t>Towranna Plains</t>
         </is>
       </c>
       <c r="D987" t="n">
@@ -17006,97 +17058,112 @@
     <row r="988">
       <c r="A988" s="3" t="inlineStr">
         <is>
-          <t>Trujillo</t>
+          <t>Totonicapan</t>
         </is>
       </c>
       <c r="D988" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="3" t="inlineStr">
-        <is>
-          <t>Trumai</t>
+      <c r="A989" s="10" t="inlineStr">
+        <is>
+          <t>Towranna Plains</t>
         </is>
       </c>
       <c r="D989" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="990">
       <c r="A990" s="3" t="inlineStr">
         <is>
-          <t>Tschamba</t>
+          <t>Trujillo</t>
         </is>
       </c>
       <c r="D990" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="991">
       <c r="A991" s="3" t="inlineStr">
         <is>
-          <t>Tschitete</t>
+          <t>Trumai</t>
         </is>
       </c>
       <c r="D991" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="992">
       <c r="A992" s="3" t="inlineStr">
         <is>
-          <t>Tschiti</t>
+          <t>Tschamba</t>
         </is>
       </c>
       <c r="D992" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="993">
       <c r="A993" s="3" t="inlineStr">
         <is>
-          <t>Tschokwe</t>
+          <t>Tschitete</t>
         </is>
       </c>
       <c r="D993" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="994">
       <c r="A994" s="3" t="inlineStr">
         <is>
-          <t>Tschokwe (Chokwe)</t>
+          <t>Tschiti</t>
         </is>
       </c>
       <c r="D994" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="995">
       <c r="A995" s="3" t="inlineStr">
         <is>
-          <t>Tshuapa</t>
+          <t>Tschokwe</t>
         </is>
       </c>
       <c r="D995" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="996">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="996" ht="30" customHeight="1" s="11">
       <c r="A996" s="3" t="inlineStr">
         <is>
-          <t>Tsiasua</t>
+          <t>Tschokwe (Chokwe)</t>
+        </is>
+      </c>
+      <c r="B996" s="10" t="inlineStr">
+        <is>
+          <t>Chokwe</t>
+        </is>
+      </c>
+      <c r="C996" s="3" t="inlineStr">
+        <is>
+          <t>Wikipedia nutzt Chokwe (en, de) als Vorzugsbezeichnung</t>
         </is>
       </c>
       <c r="D996" t="n">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="E996" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
       </c>
     </row>
     <row r="997">
       <c r="A997" s="3" t="inlineStr">
         <is>
-          <t>Tsihumbe</t>
+          <t>Tshuapa</t>
         </is>
       </c>
       <c r="D997" t="n">
@@ -17106,7 +17173,7 @@
     <row r="998">
       <c r="A998" s="3" t="inlineStr">
         <is>
-          <t>Tsikusa</t>
+          <t>Tsiasua</t>
         </is>
       </c>
       <c r="D998" t="n">
@@ -17116,7 +17183,7 @@
     <row r="999">
       <c r="A999" s="3" t="inlineStr">
         <is>
-          <t>Tsipulumgu</t>
+          <t>Tsihumbe</t>
         </is>
       </c>
       <c r="D999" t="n">
@@ -17126,7 +17193,7 @@
     <row r="1000">
       <c r="A1000" s="3" t="inlineStr">
         <is>
-          <t>Tunda</t>
+          <t>Tsikusa</t>
         </is>
       </c>
       <c r="D1000" t="n">
@@ -17136,27 +17203,27 @@
     <row r="1001">
       <c r="A1001" s="3" t="inlineStr">
         <is>
-          <t>Tunja</t>
+          <t>Tsipulumgu</t>
         </is>
       </c>
       <c r="D1001" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1002">
       <c r="A1002" s="3" t="inlineStr">
         <is>
-          <t>Ua Pou</t>
+          <t>Tunda</t>
         </is>
       </c>
       <c r="D1002" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1003">
       <c r="A1003" s="3" t="inlineStr">
         <is>
-          <t>Uapou</t>
+          <t>Tunja</t>
         </is>
       </c>
       <c r="D1003" t="n">
@@ -17166,37 +17233,37 @@
     <row r="1004">
       <c r="A1004" s="3" t="inlineStr">
         <is>
-          <t>Ubangi (Oubangui)</t>
+          <t>Ua Pou</t>
         </is>
       </c>
       <c r="D1004" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1005">
       <c r="A1005" s="3" t="inlineStr">
         <is>
-          <t>Ubudjwe</t>
+          <t>Uapou</t>
         </is>
       </c>
       <c r="D1005" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1006">
-      <c r="A1006" s="10" t="inlineStr">
-        <is>
-          <t>Uhehe</t>
+      <c r="A1006" s="3" t="inlineStr">
+        <is>
+          <t>Ubangi (Oubangui)</t>
         </is>
       </c>
       <c r="D1006" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1007">
       <c r="A1007" s="3" t="inlineStr">
         <is>
-          <t>Uiha</t>
+          <t>Ubudjwe</t>
         </is>
       </c>
       <c r="D1007" t="n">
@@ -17206,17 +17273,17 @@
     <row r="1008">
       <c r="A1008" s="10" t="inlineStr">
         <is>
-          <t>Ukimbu</t>
+          <t>Uhehe</t>
         </is>
       </c>
       <c r="D1008" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1009">
       <c r="A1009" s="3" t="inlineStr">
         <is>
-          <t>Ukinga</t>
+          <t>Uiha</t>
         </is>
       </c>
       <c r="D1009" t="n">
@@ -17224,9 +17291,9 @@
       </c>
     </row>
     <row r="1010">
-      <c r="A1010" s="3" t="inlineStr">
-        <is>
-          <t>Ukussu</t>
+      <c r="A1010" s="10" t="inlineStr">
+        <is>
+          <t>Ukimbu</t>
         </is>
       </c>
       <c r="D1010" t="n">
@@ -17236,7 +17303,7 @@
     <row r="1011">
       <c r="A1011" s="3" t="inlineStr">
         <is>
-          <t>Uleai</t>
+          <t>Ukinga</t>
         </is>
       </c>
       <c r="D1011" t="n">
@@ -17244,9 +17311,9 @@
       </c>
     </row>
     <row r="1012">
-      <c r="A1012" s="10" t="inlineStr">
-        <is>
-          <t>Umburru</t>
+      <c r="A1012" s="3" t="inlineStr">
+        <is>
+          <t>Ukussu</t>
         </is>
       </c>
       <c r="D1012" t="n">
@@ -17256,67 +17323,72 @@
     <row r="1013">
       <c r="A1013" s="3" t="inlineStr">
         <is>
+          <t>Uleai</t>
+        </is>
+      </c>
+      <c r="D1013" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="10" t="inlineStr">
+        <is>
+          <t>Umburru</t>
+        </is>
+      </c>
+      <c r="D1014" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="3" t="inlineStr">
+        <is>
           <t>Undinde</t>
         </is>
       </c>
-      <c r="D1013" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1014">
-      <c r="A1014" s="3" t="inlineStr">
-        <is>
-          <t>unterer Kongo</t>
-        </is>
-      </c>
-      <c r="D1014" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1015">
-      <c r="A1015" s="10" t="inlineStr">
-        <is>
-          <t>Unyamwanga</t>
-        </is>
-      </c>
       <c r="D1015" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1016">
       <c r="A1016" s="3" t="inlineStr">
         <is>
-          <t>Unyika</t>
+          <t>unterer Kongo</t>
+        </is>
+      </c>
+      <c r="B1016" s="10" t="inlineStr">
+        <is>
+          <t>lower Kongo</t>
         </is>
       </c>
       <c r="D1016" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1017">
       <c r="A1017" s="10" t="inlineStr">
         <is>
-          <t>Urambia</t>
+          <t>Unyamwanga</t>
         </is>
       </c>
       <c r="D1017" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1018">
       <c r="A1018" s="3" t="inlineStr">
         <is>
-          <t>Urua</t>
+          <t>Unyika</t>
         </is>
       </c>
       <c r="D1018" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1019">
-      <c r="A1019" s="3" t="inlineStr">
-        <is>
-          <t>Urua (?)</t>
+      <c r="A1019" s="10" t="inlineStr">
+        <is>
+          <t>Urambia</t>
         </is>
       </c>
       <c r="D1019" t="n">
@@ -17326,47 +17398,47 @@
     <row r="1020">
       <c r="A1020" s="3" t="inlineStr">
         <is>
+          <t>Urua</t>
+        </is>
+      </c>
+      <c r="D1020" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="3" t="inlineStr">
+        <is>
+          <t>Urua (?)</t>
+        </is>
+      </c>
+      <c r="D1021" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="3" t="inlineStr">
+        <is>
           <t>Utah</t>
         </is>
       </c>
-      <c r="D1020" t="n">
+      <c r="D1022" t="n">
         <v>20</v>
-      </c>
-    </row>
-    <row r="1021" ht="30" customHeight="1" s="11">
-      <c r="A1021" s="3" t="inlineStr">
-        <is>
-          <t>Utuan</t>
-        </is>
-      </c>
-      <c r="D1021" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1022" ht="30" customHeight="1" s="11">
-      <c r="A1022" s="10" t="inlineStr">
-        <is>
-          <t>Uvanda</t>
-        </is>
-      </c>
-      <c r="D1022" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="1023" ht="30" customHeight="1" s="11">
       <c r="A1023" s="3" t="inlineStr">
         <is>
-          <t>Uêmba</t>
+          <t>Utuan</t>
         </is>
       </c>
       <c r="D1023" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1024" ht="30" customHeight="1" s="11">
-      <c r="A1024" s="3" t="inlineStr">
-        <is>
-          <t>Vaal</t>
+      <c r="A1024" s="10" t="inlineStr">
+        <is>
+          <t>Uvanda</t>
         </is>
       </c>
       <c r="D1024" t="n">
@@ -17374,164 +17446,164 @@
       </c>
     </row>
     <row r="1025" ht="30" customHeight="1" s="11">
-      <c r="A1025" s="10" t="inlineStr">
-        <is>
-          <t>Vainillas</t>
+      <c r="A1025" s="3" t="inlineStr">
+        <is>
+          <t>Uêmba</t>
         </is>
       </c>
       <c r="D1025" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1026" ht="30" customHeight="1" s="11">
       <c r="A1026" s="3" t="inlineStr">
         <is>
-          <t>Valle del Cauca</t>
+          <t>Vaal</t>
         </is>
       </c>
       <c r="D1026" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1027" ht="30" customHeight="1" s="11">
-      <c r="A1027" s="3" t="inlineStr">
-        <is>
-          <t>Vanuatu</t>
+      <c r="A1027" s="10" t="inlineStr">
+        <is>
+          <t>Vainillas</t>
         </is>
       </c>
       <c r="D1027" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1028" ht="30" customHeight="1" s="11">
       <c r="A1028" s="3" t="inlineStr">
         <is>
-          <t>Vela</t>
+          <t>Valle del Cauca</t>
         </is>
       </c>
       <c r="D1028" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1029" ht="30" customHeight="1" s="11">
       <c r="A1029" s="3" t="inlineStr">
         <is>
-          <t>Vella Lavella</t>
+          <t>Vanuatu</t>
         </is>
       </c>
       <c r="D1029" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1030" ht="30" customHeight="1" s="11">
+      <c r="A1030" s="3" t="inlineStr">
+        <is>
+          <t>Vela</t>
+        </is>
+      </c>
+      <c r="D1030" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="1030">
-      <c r="A1030" s="3" t="inlineStr">
-        <is>
-          <t>Veracruz</t>
-        </is>
-      </c>
-      <c r="D1030" t="n">
-        <v>26</v>
       </c>
     </row>
     <row r="1031" ht="30" customHeight="1" s="11">
       <c r="A1031" s="3" t="inlineStr">
         <is>
+          <t>Vella Lavella</t>
+        </is>
+      </c>
+      <c r="D1031" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="3" t="inlineStr">
+        <is>
+          <t>Veracruz</t>
+        </is>
+      </c>
+      <c r="D1032" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1033" ht="30" customHeight="1" s="11">
+      <c r="A1033" s="3" t="inlineStr">
+        <is>
           <t>Vere</t>
         </is>
       </c>
-      <c r="C1031" s="3" t="inlineStr">
+      <c r="C1033" s="3" t="inlineStr">
         <is>
           <t>upstream korrigieren</t>
         </is>
       </c>
-      <c r="D1031" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1032" ht="30" customHeight="1" s="11">
-      <c r="A1032" s="3" t="inlineStr">
-        <is>
-          <t>Vereingte Staaten (USA)</t>
-        </is>
-      </c>
-      <c r="B1032" s="10" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="D1032" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1033">
-      <c r="A1033" s="3" t="inlineStr">
-        <is>
-          <t>Vereinigte Staaten (USA)</t>
-        </is>
-      </c>
-      <c r="B1033" s="10" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
       <c r="D1033" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1034" ht="30" customHeight="1" s="11">
       <c r="A1034" s="3" t="inlineStr">
         <is>
-          <t>verm. Guatemala</t>
-        </is>
-      </c>
-      <c r="B1034" s="10" t="inlineStr">
-        <is>
-          <t>Guatemala (?)</t>
-        </is>
-      </c>
-      <c r="C1034" s="3" t="inlineStr">
-        <is>
-          <t>upstream korrigieren</t>
+          <t>Vereingte Staaten (USA)</t>
+        </is>
+      </c>
+      <c r="B1034" s="3" t="inlineStr">
+        <is>
+          <t>Vereingte Staaten (USA)</t>
         </is>
       </c>
       <c r="D1034" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1035" ht="30" customHeight="1" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1035">
       <c r="A1035" s="3" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>Vereinigte Staaten (USA)</t>
+        </is>
+      </c>
+      <c r="B1035" s="3" t="inlineStr">
+        <is>
+          <t>Vereingte Staaten (USA)</t>
         </is>
       </c>
       <c r="D1035" t="n">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="1036" ht="30" customHeight="1" s="11">
       <c r="A1036" s="3" t="inlineStr">
         <is>
+          <t>verm. Guatemala</t>
+        </is>
+      </c>
+      <c r="B1036" s="10" t="inlineStr">
+        <is>
+          <t>Guatemala (?)</t>
+        </is>
+      </c>
+      <c r="C1036" s="3" t="inlineStr">
+        <is>
+          <t>upstream korrigieren</t>
+        </is>
+      </c>
+      <c r="D1036" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1037" ht="30" customHeight="1" s="11">
+      <c r="A1037" s="3" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="D1037" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1038" ht="30" customHeight="1" s="11">
+      <c r="A1038" s="3" t="inlineStr">
+        <is>
           <t>Vili</t>
-        </is>
-      </c>
-      <c r="D1036" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1037">
-      <c r="A1037" s="3" t="inlineStr">
-        <is>
-          <t>Vili (Bawili)</t>
-        </is>
-      </c>
-      <c r="D1037" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1038">
-      <c r="A1038" s="3" t="inlineStr">
-        <is>
-          <t>Vili (Bawili) (?)</t>
         </is>
       </c>
       <c r="D1038" t="n">
@@ -17541,127 +17613,127 @@
     <row r="1039">
       <c r="A1039" s="3" t="inlineStr">
         <is>
-          <t>Viti</t>
+          <t>Vili (Bawili)</t>
         </is>
       </c>
       <c r="D1039" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="1040">
       <c r="A1040" s="3" t="inlineStr">
         <is>
-          <t>Vora</t>
+          <t>Vili (Bawili) (?)</t>
         </is>
       </c>
       <c r="D1040" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1041">
       <c r="A1041" s="3" t="inlineStr">
         <is>
-          <t>Wabungu</t>
+          <t>Viti</t>
         </is>
       </c>
       <c r="D1041" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1042">
       <c r="A1042" s="3" t="inlineStr">
         <is>
-          <t>Waburungi</t>
+          <t>Vora</t>
         </is>
       </c>
       <c r="D1042" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1043">
       <c r="A1043" s="3" t="inlineStr">
         <is>
-          <t>Wagogo</t>
+          <t>Wabungu</t>
         </is>
       </c>
       <c r="D1043" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1044">
       <c r="A1044" s="3" t="inlineStr">
         <is>
-          <t>Waguha</t>
+          <t>Waburungi</t>
         </is>
       </c>
       <c r="D1044" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1045">
       <c r="A1045" s="3" t="inlineStr">
         <is>
-          <t>Wahehe</t>
+          <t>Wagogo</t>
         </is>
       </c>
       <c r="D1045" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1046">
       <c r="A1046" s="3" t="inlineStr">
         <is>
-          <t>Wahumba</t>
+          <t>Waguha</t>
         </is>
       </c>
       <c r="D1046" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1047">
       <c r="A1047" s="3" t="inlineStr">
         <is>
-          <t>Waikiki</t>
+          <t>Wahehe</t>
         </is>
       </c>
       <c r="D1047" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1048">
       <c r="A1048" s="3" t="inlineStr">
         <is>
-          <t>Wakaguru</t>
+          <t>Wahumba</t>
         </is>
       </c>
       <c r="D1048" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1049">
       <c r="A1049" s="3" t="inlineStr">
         <is>
-          <t>Wakinga</t>
+          <t>Waikiki</t>
         </is>
       </c>
       <c r="D1049" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1050">
       <c r="A1050" s="3" t="inlineStr">
         <is>
-          <t>Wangindo</t>
+          <t>Wakaguru</t>
         </is>
       </c>
       <c r="D1050" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1051">
       <c r="A1051" s="3" t="inlineStr">
         <is>
-          <t>Wangoni</t>
+          <t>Wakinga</t>
         </is>
       </c>
       <c r="D1051" t="n">
@@ -17671,27 +17743,27 @@
     <row r="1052">
       <c r="A1052" s="3" t="inlineStr">
         <is>
-          <t>Wanguru</t>
+          <t>Wangindo</t>
         </is>
       </c>
       <c r="D1052" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1053">
       <c r="A1053" s="3" t="inlineStr">
         <is>
-          <t>Waniramba</t>
+          <t>Wangoni</t>
         </is>
       </c>
       <c r="D1053" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1054">
       <c r="A1054" s="3" t="inlineStr">
         <is>
-          <t>Wanyamwesi</t>
+          <t>Wanguru</t>
         </is>
       </c>
       <c r="D1054" t="n">
@@ -17701,7 +17773,7 @@
     <row r="1055">
       <c r="A1055" s="3" t="inlineStr">
         <is>
-          <t>Wanyamwezi</t>
+          <t>Waniramba</t>
         </is>
       </c>
       <c r="D1055" t="n">
@@ -17711,7 +17783,7 @@
     <row r="1056">
       <c r="A1056" s="3" t="inlineStr">
         <is>
-          <t>Wanyaturu</t>
+          <t>Wanyamwesi</t>
         </is>
       </c>
       <c r="D1056" t="n">
@@ -17721,27 +17793,27 @@
     <row r="1057">
       <c r="A1057" s="3" t="inlineStr">
         <is>
-          <t>Wanyika</t>
+          <t>Wanyamwezi</t>
         </is>
       </c>
       <c r="D1057" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="1058" ht="30" customHeight="1" s="11">
+    <row r="1058">
       <c r="A1058" s="3" t="inlineStr">
         <is>
-          <t>Wanyika (?)</t>
+          <t>Wanyaturu</t>
         </is>
       </c>
       <c r="D1058" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1059">
       <c r="A1059" s="3" t="inlineStr">
         <is>
-          <t>Wapare</t>
+          <t>Wanyika</t>
         </is>
       </c>
       <c r="D1059" t="n">
@@ -17751,317 +17823,313 @@
     <row r="1060" ht="30" customHeight="1" s="11">
       <c r="A1060" s="3" t="inlineStr">
         <is>
-          <t>Waremba (Bemba)</t>
+          <t>Wanyika (?)</t>
         </is>
       </c>
       <c r="D1060" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1061">
       <c r="A1061" s="3" t="inlineStr">
         <is>
-          <t>Warua</t>
+          <t>Wapare</t>
         </is>
       </c>
       <c r="D1061" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1062" ht="30" customHeight="1" s="11">
       <c r="A1062" s="3" t="inlineStr">
         <is>
-          <t>Wasafua</t>
+          <t>Waremba (Bemba)</t>
         </is>
       </c>
       <c r="D1062" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1063">
       <c r="A1063" s="3" t="inlineStr">
         <is>
-          <t>Wassukuma</t>
+          <t>Warua</t>
         </is>
       </c>
       <c r="D1063" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1064" ht="30" customHeight="1" s="11">
       <c r="A1064" s="3" t="inlineStr">
         <is>
-          <t>Waura</t>
+          <t>Wasafua</t>
         </is>
       </c>
       <c r="D1064" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1065">
       <c r="A1065" s="3" t="inlineStr">
         <is>
+          <t>Wassukuma</t>
+        </is>
+      </c>
+      <c r="D1065" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1066" ht="30" customHeight="1" s="11">
+      <c r="A1066" s="3" t="inlineStr">
+        <is>
+          <t>Waura</t>
+        </is>
+      </c>
+      <c r="D1066" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" s="3" t="inlineStr">
+        <is>
           <t>Wawemba</t>
         </is>
       </c>
-      <c r="D1065" t="n">
+      <c r="D1067" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="1066">
-      <c r="A1066" s="3" t="inlineStr">
-        <is>
-          <t>Wayao</t>
-        </is>
-      </c>
-      <c r="D1066" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1067" ht="30" customHeight="1" s="11">
-      <c r="A1067" s="3" t="inlineStr">
-        <is>
-          <t>Weißer Nil</t>
-        </is>
-      </c>
-      <c r="B1067" s="12" t="inlineStr">
-        <is>
-          <t>White Nile</t>
-        </is>
-      </c>
-      <c r="D1067" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="1068">
       <c r="A1068" s="3" t="inlineStr">
         <is>
-          <t>Weißer-Nil</t>
-        </is>
-      </c>
-      <c r="B1068" s="12" t="inlineStr">
-        <is>
-          <t>White Nile</t>
+          <t>Wayao</t>
         </is>
       </c>
       <c r="D1068" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1069" ht="30" customHeight="1" s="11">
       <c r="A1069" s="3" t="inlineStr">
         <is>
-          <t>Werkstätten des unteren Nigers</t>
-        </is>
-      </c>
-      <c r="C1069" s="3" t="inlineStr">
-        <is>
-          <t>?</t>
+          <t>Weißer Nil</t>
+        </is>
+      </c>
+      <c r="B1069" s="22" t="inlineStr">
+        <is>
+          <t>White Nile</t>
         </is>
       </c>
       <c r="D1069" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1070">
       <c r="A1070" s="3" t="inlineStr">
         <is>
-          <t>West-Neuguinea</t>
-        </is>
-      </c>
-      <c r="B1070" s="10" t="inlineStr">
-        <is>
-          <t>Western New Guinea</t>
+          <t>Weißer-Nil</t>
+        </is>
+      </c>
+      <c r="B1070" s="22" t="inlineStr">
+        <is>
+          <t>White Nile</t>
         </is>
       </c>
       <c r="D1070" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1071" ht="30" customHeight="1" s="11">
       <c r="A1071" s="3" t="inlineStr">
         <is>
+          <t>Werkstätten des unteren Nigers</t>
+        </is>
+      </c>
+      <c r="B1071" s="10" t="inlineStr">
+        <is>
+          <t>lower Niger River</t>
+        </is>
+      </c>
+      <c r="C1071" s="3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D1071" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" s="3" t="inlineStr">
+        <is>
+          <t>West-Neuguinea</t>
+        </is>
+      </c>
+      <c r="B1072" s="10" t="inlineStr">
+        <is>
+          <t>Western New Guinea</t>
+        </is>
+      </c>
+      <c r="D1072" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1073" ht="30" customHeight="1" s="11">
+      <c r="A1073" s="3" t="inlineStr">
+        <is>
           <t>West-Victoria</t>
         </is>
       </c>
-      <c r="B1071" s="10" t="inlineStr">
+      <c r="B1073" s="10" t="inlineStr">
         <is>
           <t>Western Victoria</t>
         </is>
       </c>
-      <c r="D1071" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1072" ht="30" customHeight="1" s="11">
-      <c r="A1072" s="3" t="inlineStr">
+      <c r="D1073" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1074" ht="30" customHeight="1" s="11">
+      <c r="A1074" s="3" t="inlineStr">
         <is>
           <t>Westafrika</t>
         </is>
       </c>
-      <c r="B1072" s="10" t="inlineStr">
+      <c r="B1074" s="10" t="inlineStr">
         <is>
           <t>West Africa</t>
         </is>
       </c>
-      <c r="D1072" t="n">
+      <c r="D1074" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="1073">
-      <c r="A1073" s="3" t="inlineStr">
-        <is>
-          <t>Westaustralien</t>
-        </is>
-      </c>
-      <c r="B1073" s="3" t="inlineStr">
-        <is>
-          <t>Western Australia</t>
-        </is>
-      </c>
-      <c r="D1073" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1074">
-      <c r="A1074" s="10" t="inlineStr">
-        <is>
-          <t>Westbrasilien</t>
-        </is>
-      </c>
-      <c r="B1074" s="10" t="inlineStr">
-        <is>
-          <t>Western Brazil</t>
-        </is>
-      </c>
-      <c r="D1074" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="1075">
       <c r="A1075" s="3" t="inlineStr">
         <is>
-          <t>Westliche Inseln</t>
-        </is>
-      </c>
-      <c r="B1075" s="10" t="inlineStr">
-        <is>
-          <t>Western Islands</t>
+          <t>Westaustralien</t>
+        </is>
+      </c>
+      <c r="B1075" s="3" t="inlineStr">
+        <is>
+          <t>Western Australia</t>
         </is>
       </c>
       <c r="D1075" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="1076">
-      <c r="A1076" s="3" t="inlineStr">
-        <is>
-          <t>Westliche-Inseln</t>
+      <c r="A1076" s="10" t="inlineStr">
+        <is>
+          <t>Westbrasilien</t>
         </is>
       </c>
       <c r="B1076" s="10" t="inlineStr">
         <is>
-          <t>south Inseln</t>
+          <t>Western Brazil</t>
         </is>
       </c>
       <c r="D1076" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1077">
       <c r="A1077" s="3" t="inlineStr">
         <is>
-          <t>Westlicher Bezirk</t>
+          <t>Westliche Inseln</t>
         </is>
       </c>
       <c r="B1077" s="10" t="inlineStr">
         <is>
-          <t>south Bezirk</t>
+          <t>Western Islands</t>
         </is>
       </c>
       <c r="D1077" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="1078">
-      <c r="A1078" s="10" t="inlineStr">
-        <is>
-          <t>Westmexiko</t>
+      <c r="A1078" s="3" t="inlineStr">
+        <is>
+          <t>Westliche-Inseln</t>
         </is>
       </c>
       <c r="B1078" s="10" t="inlineStr">
         <is>
-          <t>Western Mexico</t>
+          <t>Western Islands</t>
         </is>
       </c>
       <c r="D1078" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1079">
       <c r="A1079" s="3" t="inlineStr">
         <is>
+          <t>Westlicher Bezirk</t>
+        </is>
+      </c>
+      <c r="B1079" s="10" t="inlineStr">
+        <is>
+          <t>Western District</t>
+        </is>
+      </c>
+      <c r="D1079" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1080" s="11">
+      <c r="A1080" s="10" t="inlineStr">
+        <is>
+          <t>Westmexiko</t>
+        </is>
+      </c>
+      <c r="B1080" s="10" t="inlineStr">
+        <is>
+          <t>Western Mexico</t>
+        </is>
+      </c>
+      <c r="C1080" s="3" t="inlineStr">
+        <is>
+          <t>soll West-Mexiko sein</t>
+        </is>
+      </c>
+      <c r="D1080" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1080" s="3" t="n"/>
+    </row>
+    <row r="1081">
+      <c r="A1081" s="3" t="inlineStr">
+        <is>
+          <t>West-Mexiko</t>
+        </is>
+      </c>
+      <c r="B1081" s="10" t="inlineStr">
+        <is>
+          <t>Western Mexico</t>
+        </is>
+      </c>
+      <c r="D1081" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" s="3" t="inlineStr">
+        <is>
           <t>Woleai</t>
         </is>
       </c>
-      <c r="B1079" s="10" t="inlineStr">
-        <is>
-          <t>south Woleai</t>
-        </is>
-      </c>
-      <c r="D1079" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1080">
-      <c r="A1080" s="3" t="inlineStr">
+      <c r="D1082" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" s="3" t="inlineStr">
         <is>
           <t>Womatne</t>
-        </is>
-      </c>
-      <c r="B1080" s="10" t="inlineStr">
-        <is>
-          <t>south Womatne</t>
-        </is>
-      </c>
-      <c r="D1080" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1081">
-      <c r="A1081" s="10" t="inlineStr">
-        <is>
-          <t>Wosera</t>
-        </is>
-      </c>
-      <c r="D1081" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1082">
-      <c r="A1082" s="10" t="inlineStr">
-        <is>
-          <t>Woyo</t>
-        </is>
-      </c>
-      <c r="B1082" s="10" t="inlineStr">
-        <is>
-          <t>south Woyo</t>
-        </is>
-      </c>
-      <c r="D1082" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1083">
-      <c r="A1083" s="10" t="inlineStr">
-        <is>
-          <t>Wum</t>
-        </is>
-      </c>
-      <c r="B1083" s="10" t="inlineStr">
-        <is>
-          <t>south Wum</t>
         </is>
       </c>
       <c r="D1083" t="n">
@@ -18071,37 +18139,27 @@
     <row r="1084">
       <c r="A1084" s="10" t="inlineStr">
         <is>
-          <t>Wuvulu</t>
+          <t>Wosera</t>
         </is>
       </c>
       <c r="D1084" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1085">
-      <c r="A1085" s="3" t="inlineStr">
-        <is>
-          <t>Xingú</t>
-        </is>
-      </c>
-      <c r="B1085" s="10" t="inlineStr">
-        <is>
-          <t>south Xingú</t>
+      <c r="A1085" s="10" t="inlineStr">
+        <is>
+          <t>Woyo</t>
         </is>
       </c>
       <c r="D1085" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1086">
       <c r="A1086" s="10" t="inlineStr">
         <is>
-          <t>Xoxo</t>
-        </is>
-      </c>
-      <c r="B1086" s="10" t="inlineStr">
-        <is>
-          <t>south Xoxo</t>
+          <t>Wum</t>
         </is>
       </c>
       <c r="D1086" t="n">
@@ -18111,337 +18169,307 @@
     <row r="1087">
       <c r="A1087" s="10" t="inlineStr">
         <is>
-          <t>Yaka</t>
-        </is>
-      </c>
-      <c r="B1087" s="10" t="inlineStr">
-        <is>
-          <t>south Yaka</t>
+          <t>Wuvulu</t>
         </is>
       </c>
       <c r="D1087" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1088">
-      <c r="A1088" s="10" t="inlineStr">
-        <is>
-          <t>Yap</t>
-        </is>
-      </c>
-      <c r="B1088" s="10" t="inlineStr">
-        <is>
-          <t>south Yap</t>
+      <c r="A1088" s="3" t="inlineStr">
+        <is>
+          <t>Xingú</t>
         </is>
       </c>
       <c r="D1088" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1089">
       <c r="A1089" s="10" t="inlineStr">
         <is>
-          <t>Yap-Inseln</t>
-        </is>
-      </c>
-      <c r="B1089" s="10" t="inlineStr">
-        <is>
-          <t>Yap</t>
+          <t>Xoxo</t>
         </is>
       </c>
       <c r="D1089" t="n">
-        <v>13</v>
-      </c>
-      <c r="E1089" s="3" t="inlineStr">
-        <is>
-          <t>wikipedia</t>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="1090">
-      <c r="A1090" s="3" t="inlineStr">
-        <is>
-          <t>Yarra-Stamm</t>
-        </is>
-      </c>
-      <c r="B1090" s="10" t="inlineStr">
-        <is>
-          <t>Yarra</t>
+      <c r="A1090" s="10" t="inlineStr">
+        <is>
+          <t>Yaka</t>
         </is>
       </c>
       <c r="D1090" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1091">
       <c r="A1091" s="10" t="inlineStr">
         <is>
+          <t>Yap</t>
+        </is>
+      </c>
+      <c r="D1091" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" s="10" t="inlineStr">
+        <is>
+          <t>Yap-Inseln</t>
+        </is>
+      </c>
+      <c r="B1092" s="10" t="inlineStr">
+        <is>
+          <t>Yap</t>
+        </is>
+      </c>
+      <c r="D1092" t="n">
+        <v>13</v>
+      </c>
+      <c r="E1092" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="3" t="inlineStr">
+        <is>
+          <t>Yarra-Stamm</t>
+        </is>
+      </c>
+      <c r="B1093" s="10" t="inlineStr">
+        <is>
+          <t>Yarra</t>
+        </is>
+      </c>
+      <c r="D1093" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" s="10" t="inlineStr">
+        <is>
           <t>Yaulapiti</t>
         </is>
       </c>
-      <c r="D1091" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1092">
-      <c r="A1092" s="3" t="inlineStr">
+      <c r="D1094" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" s="3" t="inlineStr">
         <is>
           <t>Yelu</t>
         </is>
       </c>
-      <c r="D1092" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1093">
-      <c r="A1093" s="10" t="inlineStr">
+      <c r="D1095" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" s="10" t="inlineStr">
         <is>
           <t>Yindjibarndi (?)</t>
         </is>
       </c>
-      <c r="D1093" t="n">
+      <c r="D1096" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="1094" ht="30" customHeight="1" s="11">
-      <c r="A1094" s="10" t="inlineStr">
+    <row r="1097" ht="30" customHeight="1" s="11">
+      <c r="A1097" s="10" t="inlineStr">
         <is>
           <t>Yombe</t>
         </is>
       </c>
-      <c r="D1094" t="n">
+      <c r="D1097" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="1095" ht="30" customHeight="1" s="11">
-      <c r="A1095" s="3" t="inlineStr">
+    <row r="1098" ht="30" customHeight="1" s="11">
+      <c r="A1098" s="3" t="inlineStr">
         <is>
           <t>Yombe (?)</t>
         </is>
       </c>
-      <c r="D1095" t="n">
+      <c r="D1098" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="1096" ht="30" customHeight="1" s="11">
-      <c r="A1096" s="10" t="inlineStr">
+    <row r="1099" ht="30" customHeight="1" s="11">
+      <c r="A1099" s="10" t="inlineStr">
         <is>
           <t>Yoruba</t>
         </is>
       </c>
-      <c r="D1096" t="n">
+      <c r="D1099" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="1097" ht="45" customHeight="1" s="11">
-      <c r="A1097" s="3" t="inlineStr">
+    <row r="1100" ht="45" customHeight="1" s="11">
+      <c r="A1100" s="3" t="inlineStr">
         <is>
           <t>Yukatan</t>
         </is>
       </c>
-      <c r="D1097" t="n">
+      <c r="D1100" t="n">
         <v>8</v>
-      </c>
-    </row>
-    <row r="1098" ht="30" customHeight="1" s="11">
-      <c r="A1098" s="10" t="inlineStr">
-        <is>
-          <t>Zacualpa</t>
-        </is>
-      </c>
-      <c r="D1098" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1099" ht="45" customHeight="1" s="11">
-      <c r="A1099" s="10" t="inlineStr">
-        <is>
-          <t>Zaire</t>
-        </is>
-      </c>
-      <c r="D1099" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1100" ht="30" customHeight="1" s="11">
-      <c r="A1100" s="3" t="inlineStr">
-        <is>
-          <t>Zaire (?)</t>
-        </is>
-      </c>
-      <c r="D1100" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="1101" ht="30" customHeight="1" s="11">
       <c r="A1101" s="10" t="inlineStr">
         <is>
-          <t>Zambezi</t>
+          <t>Zacualpa</t>
         </is>
       </c>
       <c r="D1101" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1102" ht="30" customHeight="1" s="11">
-      <c r="A1102" s="3" t="inlineStr">
-        <is>
-          <t>Zambezi-Gebiet</t>
-        </is>
-      </c>
-      <c r="B1102" s="10" t="inlineStr">
-        <is>
-          <t>Zambezi</t>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1102" ht="45" customHeight="1" s="11">
+      <c r="A1102" s="10" t="inlineStr">
+        <is>
+          <t>Zaire</t>
         </is>
       </c>
       <c r="D1102" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1103" ht="30" customHeight="1" s="11">
       <c r="A1103" s="3" t="inlineStr">
         <is>
-          <t>Zapoteken</t>
-        </is>
-      </c>
-      <c r="B1103" s="12" t="inlineStr">
-        <is>
-          <t>Zapotecs</t>
+          <t>Zaire (?)</t>
         </is>
       </c>
       <c r="D1103" t="n">
-        <v>5</v>
-      </c>
-      <c r="E1103" s="3" t="inlineStr">
-        <is>
-          <t>wikipedia</t>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="1104" ht="30" customHeight="1" s="11">
       <c r="A1104" s="10" t="inlineStr">
         <is>
-          <t>Zentral-Australien</t>
-        </is>
-      </c>
-      <c r="B1104" s="10" t="inlineStr">
-        <is>
-          <t>Central Australia</t>
+          <t>Zambezi</t>
         </is>
       </c>
       <c r="D1104" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="1105" ht="45" customHeight="1" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1105" ht="30" customHeight="1" s="11">
       <c r="A1105" s="3" t="inlineStr">
         <is>
-          <t>Zentral-Brasilien</t>
+          <t>Zambezi-Gebiet</t>
         </is>
       </c>
       <c r="B1105" s="10" t="inlineStr">
         <is>
-          <t>Central Brazil</t>
+          <t>Zambezi</t>
         </is>
       </c>
       <c r="D1105" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1106" ht="30" customHeight="1" s="11">
       <c r="A1106" s="3" t="inlineStr">
         <is>
-          <t>Zentral-Karolinen</t>
-        </is>
-      </c>
-      <c r="B1106" s="10" t="inlineStr">
-        <is>
-          <t>Central Caroline Islands</t>
+          <t>Zapoteken</t>
+        </is>
+      </c>
+      <c r="B1106" s="22" t="inlineStr">
+        <is>
+          <t>Zapotecs</t>
         </is>
       </c>
       <c r="D1106" t="n">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E1106" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
       </c>
     </row>
     <row r="1107" ht="30" customHeight="1" s="11">
-      <c r="A1107" s="3" t="inlineStr">
-        <is>
-          <t>Zentralafrikanische Republik</t>
+      <c r="A1107" s="10" t="inlineStr">
+        <is>
+          <t>Zentral-Australien</t>
         </is>
       </c>
       <c r="B1107" s="10" t="inlineStr">
         <is>
-          <t>Central African Republic</t>
+          <t>Central Australia</t>
         </is>
       </c>
       <c r="D1107" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1107" s="3" t="inlineStr">
-        <is>
-          <t>wikipedia</t>
-        </is>
-      </c>
-    </row>
-    <row r="1108" ht="30" customHeight="1" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1108" ht="45" customHeight="1" s="11">
       <c r="A1108" s="3" t="inlineStr">
         <is>
-          <t>Zentrales Hochland</t>
+          <t>Zentral-Brasilien</t>
         </is>
       </c>
       <c r="B1108" s="10" t="inlineStr">
         <is>
-          <t>south Hochland</t>
+          <t>Central Brazil</t>
         </is>
       </c>
       <c r="D1108" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1109" ht="30" customHeight="1" s="11">
       <c r="A1109" s="3" t="inlineStr">
         <is>
-          <t>zwischen Ica und Pisco</t>
+          <t>Zentral-Karolinen</t>
         </is>
       </c>
       <c r="B1109" s="10" t="inlineStr">
         <is>
-          <t>south Pisco</t>
+          <t>Central Caroline Islands</t>
         </is>
       </c>
       <c r="D1109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1110" ht="30" customHeight="1" s="11">
       <c r="A1110" s="3" t="inlineStr">
         <is>
-          <t>Zwischen Tanganyikasee und Kivusee</t>
-        </is>
-      </c>
-      <c r="B1110" s="12" t="inlineStr">
-        <is>
-          <t>Lake Tanganyika/Lake Kivu</t>
+          <t>Zentralafrikanische Republik</t>
+        </is>
+      </c>
+      <c r="B1110" s="10" t="inlineStr">
+        <is>
+          <t>Central African Republic</t>
         </is>
       </c>
       <c r="D1110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1110" s="3" t="inlineStr">
         <is>
-          <t>wikipedia</t>
+          <t>wikipedia, AA</t>
         </is>
       </c>
     </row>
     <row r="1111" ht="30" customHeight="1" s="11">
-      <c r="A1111" s="10" t="inlineStr">
-        <is>
-          <t>Äquatorialafrika</t>
+      <c r="A1111" s="3" t="inlineStr">
+        <is>
+          <t>Zentrales Hochland</t>
         </is>
       </c>
       <c r="B1111" s="10" t="inlineStr">
         <is>
-          <t>south Äquatorialafrika</t>
+          <t>central highland</t>
         </is>
       </c>
       <c r="D1111" t="n">
@@ -18451,55 +18479,106 @@
     <row r="1112" ht="30" customHeight="1" s="11">
       <c r="A1112" s="3" t="inlineStr">
         <is>
+          <t>zwischen Ica und Pisco</t>
+        </is>
+      </c>
+      <c r="B1112" s="10" t="inlineStr">
+        <is>
+          <t>Ica/Pisco</t>
+        </is>
+      </c>
+      <c r="C1112" s="3" t="inlineStr">
+        <is>
+          <t>upstream korrigieren</t>
+        </is>
+      </c>
+      <c r="D1112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1113" ht="30" customHeight="1" s="11">
+      <c r="A1113" s="3" t="inlineStr">
+        <is>
+          <t>Zwischen Tanganyikasee und Kivusee</t>
+        </is>
+      </c>
+      <c r="B1113" s="22" t="inlineStr">
+        <is>
+          <t>Lake Tanganyika/Lake Kivu</t>
+        </is>
+      </c>
+      <c r="D1113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1113" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114" ht="30" customHeight="1" s="11">
+      <c r="A1114" s="10" t="inlineStr">
+        <is>
+          <t>Äquatorialafrika</t>
+        </is>
+      </c>
+      <c r="B1114" s="22" t="inlineStr">
+        <is>
+          <t>Equatorial Africa</t>
+        </is>
+      </c>
+      <c r="C1114" s="3" t="inlineStr">
+        <is>
+          <t>mehrdeutige Bezeichnung, wenn möglich in M+ präzisieren</t>
+        </is>
+      </c>
+      <c r="D1114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1114" s="3" t="inlineStr">
+        <is>
+          <t>wikipedia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115" ht="30" customHeight="1" s="11">
+      <c r="A1115" s="3" t="inlineStr">
+        <is>
           <t>Äthiopien</t>
         </is>
       </c>
-      <c r="B1112" s="10" t="inlineStr">
+      <c r="B1115" s="10" t="inlineStr">
         <is>
           <t>Ethiopia</t>
         </is>
       </c>
-      <c r="D1112" t="n">
+      <c r="D1115" t="n">
         <v>23</v>
       </c>
-      <c r="E1112" s="3" t="inlineStr">
+      <c r="E1115" s="3" t="inlineStr">
         <is>
           <t>wikipedia</t>
         </is>
       </c>
     </row>
-    <row r="1113" ht="30" customHeight="1" s="11">
-      <c r="A1113" t="inlineStr">
+    <row r="1116" ht="30" customHeight="1" s="11">
+      <c r="A1116" t="inlineStr">
         <is>
           <t>Äthiopien (?)</t>
         </is>
       </c>
-      <c r="D1113" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1114" ht="45" customHeight="1" s="11">
-      <c r="A1114" s="3" t="inlineStr">
-        <is>
-          <t>Äthiopien ?</t>
-        </is>
-      </c>
-      <c r="B1114" s="10" t="inlineStr">
+      <c r="B1116" s="10" t="inlineStr">
         <is>
           <t>Ethiopia (?)</t>
         </is>
       </c>
-      <c r="C1114" s="3" t="inlineStr">
-        <is>
-          <t>in vindex korrigieren</t>
-        </is>
-      </c>
-      <c r="D1114" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1115" ht="45" customHeight="1" s="11"/>
-    <row r="1119" ht="30" customHeight="1" s="11"/>
+      <c r="D1116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1117" ht="45" customHeight="1" s="11"/>
+    <row r="1118" ht="45" customHeight="1" s="11"/>
+    <row r="1122" ht="30" customHeight="1" s="11"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
@@ -39439,7 +39518,7 @@
   </sheetPr>
   <dimension ref="A1:E1039"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B624" sqref="B624"/>
     </sheetView>

</xml_diff>